<commit_message>
Actualización automática - 2025-08-19 10:45
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -10,19 +10,19 @@
   </externalReferences>
   <definedNames>
     <definedName name="MP">'[1]MATERIA PRIMA'!$B$3:$B$135</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Descuentos para BOT '!$A$1:$H$317</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Descuentos para BOT '!$A$1:$H$316</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="5bjg5KHnNA6sJB+RP6Fc9g04O9Wr7/QgITlO+SyIQBM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="b13cknmLu2EuxC8+gqCOA/oPgBXN51MRefoyom0mCFo="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="426">
   <si>
     <t>Legajo</t>
   </si>
@@ -833,9 +833,6 @@
   </si>
   <si>
     <t>Canepa Santiago</t>
-  </si>
-  <si>
-    <t>Zega Maximiliano</t>
   </si>
   <si>
     <t>Maidana Ariana</t>
@@ -1311,7 +1308,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00;\(\$#,##0.00\);\$#,##0.00"/>
   </numFmts>
   <fonts count="6">
@@ -1418,9 +1415,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1801,7 +1796,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="4">
-        <f t="shared" ref="A2:A316" si="1">VLOOKUP(B2,Empleados!$B$1:$F$120,2,0)</f>
+        <f t="shared" ref="A2:A315" si="1">VLOOKUP(B2,'Empleados c nro legajo'!$B$1:$F$120,2,0)</f>
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -10171,7 +10166,7 @@
     <row r="188" ht="14.25" customHeight="1">
       <c r="A188" s="4">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B188" s="4" t="s">
         <v>270</v>
@@ -10180,19 +10175,19 @@
         <v>45838.0</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E188" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G188" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="H188" s="6">
-        <v>94069.13</v>
+        <v>136857.98</v>
       </c>
       <c r="I188" s="4"/>
       <c r="J188" s="4"/>
@@ -10216,28 +10211,28 @@
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" s="4">
         <f t="shared" si="1"/>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B189" s="4" t="s">
         <v>271</v>
       </c>
       <c r="C189" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E189" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F189" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G189" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H189" s="6">
-        <v>136857.98</v>
+        <v>125097.8</v>
       </c>
       <c r="I189" s="4"/>
       <c r="J189" s="4"/>
@@ -10261,7 +10256,7 @@
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="4">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B190" s="4" t="s">
         <v>272</v>
@@ -10282,7 +10277,7 @@
         <v>22</v>
       </c>
       <c r="H190" s="6">
-        <v>125097.8</v>
+        <v>187635.6</v>
       </c>
       <c r="I190" s="4"/>
       <c r="J190" s="4"/>
@@ -10309,25 +10304,25 @@
         <v>204</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C191" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E191" s="7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="F191" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G191" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="H191" s="6">
-        <v>187635.6</v>
+        <v>42184.94</v>
       </c>
       <c r="I191" s="4"/>
       <c r="J191" s="4"/>
@@ -10351,28 +10346,28 @@
     <row r="192" ht="14.25" customHeight="1">
       <c r="A192" s="4">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B192" s="4" t="s">
         <v>273</v>
       </c>
       <c r="C192" s="5">
-        <v>45838.0</v>
+        <v>45821.0</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E192" s="7" t="s">
-        <v>52</v>
+        <v>23</v>
+      </c>
+      <c r="E192" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G192" s="4" t="s">
-        <v>53</v>
+        <v>275</v>
       </c>
       <c r="H192" s="6">
-        <v>42184.94</v>
+        <v>67693.37</v>
       </c>
       <c r="I192" s="4"/>
       <c r="J192" s="4"/>
@@ -10399,25 +10394,25 @@
         <v>205</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C193" s="5">
-        <v>45821.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E193" s="4" t="s">
-        <v>275</v>
+        <v>51</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G193" s="4" t="s">
-        <v>276</v>
+        <v>53</v>
       </c>
       <c r="H193" s="6">
-        <v>67693.37</v>
+        <v>86600.97</v>
       </c>
       <c r="I193" s="4"/>
       <c r="J193" s="4"/>
@@ -10441,28 +10436,28 @@
     <row r="194" ht="14.25" customHeight="1">
       <c r="A194" s="4">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C194" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E194" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F194" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G194" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H194" s="6">
-        <v>86600.97</v>
+        <v>252496.51</v>
       </c>
       <c r="I194" s="4"/>
       <c r="J194" s="4"/>
@@ -10489,25 +10484,25 @@
         <v>211</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C195" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E195" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G195" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H195" s="6">
-        <v>252496.51</v>
+        <v>86243.91</v>
       </c>
       <c r="I195" s="4"/>
       <c r="J195" s="4"/>
@@ -10534,25 +10529,25 @@
         <v>211</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C196" s="5">
         <v>45838.0</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G196" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="H196" s="6">
-        <v>86243.91</v>
+        <v>88912.23</v>
       </c>
       <c r="I196" s="4"/>
       <c r="J196" s="4"/>
@@ -10576,28 +10571,28 @@
     <row r="197" ht="14.25" customHeight="1">
       <c r="A197" s="4">
         <f t="shared" si="1"/>
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B197" s="4" t="s">
         <v>277</v>
       </c>
       <c r="C197" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E197" s="7" t="s">
-        <v>52</v>
+        <v>278</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G197" s="4" t="s">
-        <v>53</v>
+        <v>280</v>
       </c>
       <c r="H197" s="6">
-        <v>88912.23</v>
+        <v>173495.64</v>
       </c>
       <c r="I197" s="4"/>
       <c r="J197" s="4"/>
@@ -10621,28 +10616,28 @@
     <row r="198" ht="14.25" customHeight="1">
       <c r="A198" s="4">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C198" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>280</v>
+        <v>72</v>
+      </c>
+      <c r="E198" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="F198" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G198" s="4" t="s">
-        <v>281</v>
+        <v>74</v>
       </c>
       <c r="H198" s="6">
-        <v>173495.64</v>
+        <v>45837.04</v>
       </c>
       <c r="I198" s="4"/>
       <c r="J198" s="4"/>
@@ -10666,28 +10661,28 @@
     <row r="199" ht="14.25" customHeight="1">
       <c r="A199" s="4">
         <f t="shared" si="1"/>
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>282</v>
       </c>
       <c r="C199" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E199" s="7" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="F199" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G199" s="4" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="H199" s="6">
-        <v>45837.04</v>
+        <v>364475.39</v>
       </c>
       <c r="I199" s="4"/>
       <c r="J199" s="4"/>
@@ -10714,25 +10709,25 @@
         <v>217</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C200" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E200" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F200" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G200" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H200" s="6">
-        <v>364475.39</v>
+        <v>54563.41</v>
       </c>
       <c r="I200" s="4"/>
       <c r="J200" s="4"/>
@@ -10759,25 +10754,25 @@
         <v>217</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C201" s="5">
         <v>45838.0</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E201" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F201" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G201" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="H201" s="6">
-        <v>54563.41</v>
+        <v>110096.58</v>
       </c>
       <c r="I201" s="4"/>
       <c r="J201" s="4"/>
@@ -10801,28 +10796,28 @@
     <row r="202" ht="14.25" customHeight="1">
       <c r="A202" s="4">
         <f t="shared" si="1"/>
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C202" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E202" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F202" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G202" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H202" s="6">
-        <v>110096.58</v>
+        <v>53146.88</v>
       </c>
       <c r="I202" s="4"/>
       <c r="J202" s="4"/>
@@ -10849,25 +10844,25 @@
         <v>219</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C203" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E203" s="7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="F203" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G203" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="H203" s="6">
-        <v>53146.88</v>
+        <v>76017.32</v>
       </c>
       <c r="I203" s="4"/>
       <c r="J203" s="4"/>
@@ -10891,28 +10886,28 @@
     <row r="204" ht="14.25" customHeight="1">
       <c r="A204" s="4">
         <f t="shared" si="1"/>
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>284</v>
       </c>
       <c r="C204" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E204" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F204" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G204" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H204" s="6">
-        <v>76017.32</v>
+        <v>109382.58</v>
       </c>
       <c r="I204" s="4"/>
       <c r="J204" s="4"/>
@@ -10939,25 +10934,25 @@
         <v>226</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C205" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E205" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F205" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G205" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H205" s="6">
-        <v>109382.58</v>
+        <v>55181.94</v>
       </c>
       <c r="I205" s="4"/>
       <c r="J205" s="4"/>
@@ -10981,7 +10976,7 @@
     <row r="206" ht="14.25" customHeight="1">
       <c r="A206" s="4">
         <f t="shared" si="1"/>
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>285</v>
@@ -10990,19 +10985,19 @@
         <v>45838.0</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="E206" s="7" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="F206" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G206" s="4" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="H206" s="6">
-        <v>55181.94</v>
+        <v>116107.44</v>
       </c>
       <c r="I206" s="4"/>
       <c r="J206" s="4"/>
@@ -11026,28 +11021,28 @@
     <row r="207" ht="14.25" customHeight="1">
       <c r="A207" s="4">
         <f t="shared" si="1"/>
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>286</v>
       </c>
       <c r="C207" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="E207" s="7" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="F207" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G207" s="4" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="H207" s="6">
-        <v>116107.44</v>
+        <v>36577.57</v>
       </c>
       <c r="I207" s="4"/>
       <c r="J207" s="4"/>
@@ -11074,25 +11069,25 @@
         <v>236</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C208" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>19</v>
+        <v>246</v>
       </c>
       <c r="E208" s="7" t="s">
-        <v>20</v>
+        <v>247</v>
       </c>
       <c r="F208" s="4" t="s">
-        <v>21</v>
+        <v>248</v>
       </c>
       <c r="G208" s="4" t="s">
-        <v>22</v>
+        <v>249</v>
       </c>
       <c r="H208" s="6">
-        <v>36577.57</v>
+        <v>202443.49</v>
       </c>
       <c r="I208" s="4"/>
       <c r="J208" s="4"/>
@@ -11116,28 +11111,28 @@
     <row r="209" ht="14.25" customHeight="1">
       <c r="A209" s="4">
         <f t="shared" si="1"/>
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B209" s="4" t="s">
         <v>287</v>
       </c>
       <c r="C209" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="E209" s="7" t="s">
-        <v>247</v>
+        <v>20</v>
       </c>
       <c r="F209" s="4" t="s">
-        <v>248</v>
+        <v>21</v>
       </c>
       <c r="G209" s="4" t="s">
-        <v>249</v>
+        <v>22</v>
       </c>
       <c r="H209" s="6">
-        <v>202443.49</v>
+        <v>217986.37</v>
       </c>
       <c r="I209" s="4"/>
       <c r="J209" s="4"/>
@@ -11164,25 +11159,25 @@
         <v>237</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C210" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E210" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F210" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G210" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H210" s="6">
-        <v>217986.37</v>
+        <v>96283.01</v>
       </c>
       <c r="I210" s="4"/>
       <c r="J210" s="4"/>
@@ -11206,28 +11201,28 @@
     <row r="211" ht="14.25" customHeight="1">
       <c r="A211" s="4">
         <f t="shared" si="1"/>
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B211" s="4" t="s">
         <v>288</v>
       </c>
       <c r="C211" s="5">
-        <v>45838.0</v>
+        <v>45821.0</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E211" s="7" t="s">
-        <v>73</v>
+        <v>23</v>
+      </c>
+      <c r="E211" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="F211" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G211" s="4" t="s">
-        <v>74</v>
+        <v>290</v>
       </c>
       <c r="H211" s="6">
-        <v>96283.01</v>
+        <v>55561.35</v>
       </c>
       <c r="I211" s="4"/>
       <c r="J211" s="4"/>
@@ -11254,25 +11249,25 @@
         <v>238</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C212" s="5">
-        <v>45821.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E212" s="4" t="s">
-        <v>290</v>
+        <v>51</v>
+      </c>
+      <c r="E212" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F212" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G212" s="4" t="s">
-        <v>291</v>
+        <v>53</v>
       </c>
       <c r="H212" s="6">
-        <v>55561.35</v>
+        <v>74636.63</v>
       </c>
       <c r="I212" s="4"/>
       <c r="J212" s="4"/>
@@ -11299,25 +11294,25 @@
         <v>238</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C213" s="5">
-        <v>45838.0</v>
+        <v>45853.0</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E213" s="7" t="s">
-        <v>52</v>
+        <v>291</v>
       </c>
       <c r="F213" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G213" s="4" t="s">
-        <v>53</v>
+        <v>292</v>
       </c>
       <c r="H213" s="6">
-        <v>74636.63</v>
+        <v>4937.66</v>
       </c>
       <c r="I213" s="4"/>
       <c r="J213" s="4"/>
@@ -11344,7 +11339,7 @@
         <v>238</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C214" s="5">
         <v>45853.0</v>
@@ -11353,7 +11348,7 @@
         <v>23</v>
       </c>
       <c r="E214" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F214" s="4" t="s">
         <v>25</v>
@@ -11362,7 +11357,7 @@
         <v>293</v>
       </c>
       <c r="H214" s="6">
-        <v>4937.66</v>
+        <v>19863.53</v>
       </c>
       <c r="I214" s="4"/>
       <c r="J214" s="4"/>
@@ -11386,28 +11381,28 @@
     <row r="215" ht="14.25" customHeight="1">
       <c r="A215" s="4">
         <f t="shared" si="1"/>
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C215" s="5">
-        <v>45853.0</v>
+        <v>45821.0</v>
       </c>
       <c r="D215" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E215" s="7" t="s">
-        <v>292</v>
+      <c r="E215" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="F215" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G215" s="4" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H215" s="6">
-        <v>19863.53</v>
+        <v>51984.92</v>
       </c>
       <c r="I215" s="4"/>
       <c r="J215" s="4"/>
@@ -11434,25 +11429,25 @@
         <v>240</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C216" s="5">
         <v>45821.0</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F216" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="G216" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H216" s="6">
-        <v>51984.92</v>
+        <v>-45818.18</v>
       </c>
       <c r="I216" s="4"/>
       <c r="J216" s="4"/>
@@ -11479,25 +11474,25 @@
         <v>240</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C217" s="5">
-        <v>45821.0</v>
+        <v>45822.0</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>60</v>
+        <v>299</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F217" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G217" s="4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H217" s="6">
-        <v>-45818.18</v>
+        <v>-5524.91</v>
       </c>
       <c r="I217" s="4"/>
       <c r="J217" s="4"/>
@@ -11524,25 +11519,25 @@
         <v>240</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C218" s="5">
-        <v>45822.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="E218" s="4" t="s">
-        <v>301</v>
+        <v>51</v>
+      </c>
+      <c r="E218" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F218" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G218" s="4" t="s">
-        <v>302</v>
+        <v>53</v>
       </c>
       <c r="H218" s="6">
-        <v>-5524.91</v>
+        <v>10450.0</v>
       </c>
       <c r="I218" s="4"/>
       <c r="J218" s="4"/>
@@ -11566,28 +11561,28 @@
     <row r="219" ht="14.25" customHeight="1">
       <c r="A219" s="4">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C219" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E219" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F219" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G219" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H219" s="6">
-        <v>10450.0</v>
+        <v>119812.21</v>
       </c>
       <c r="I219" s="4"/>
       <c r="J219" s="4"/>
@@ -11614,25 +11609,25 @@
         <v>241</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C220" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E220" s="7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="F220" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G220" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="H220" s="6">
-        <v>119812.21</v>
+        <v>55225.36</v>
       </c>
       <c r="I220" s="4"/>
       <c r="J220" s="4"/>
@@ -11656,28 +11651,28 @@
     <row r="221" ht="14.25" customHeight="1">
       <c r="A221" s="4">
         <f t="shared" si="1"/>
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B221" s="4" t="s">
         <v>303</v>
       </c>
       <c r="C221" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E221" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F221" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G221" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H221" s="6">
-        <v>55225.36</v>
+        <v>174293.97</v>
       </c>
       <c r="I221" s="4"/>
       <c r="J221" s="4"/>
@@ -11704,25 +11699,25 @@
         <v>242</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C222" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E222" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F222" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G222" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H222" s="6">
-        <v>174293.97</v>
+        <v>99030.54</v>
       </c>
       <c r="I222" s="4"/>
       <c r="J222" s="4"/>
@@ -11749,25 +11744,25 @@
         <v>242</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C223" s="5">
         <v>45838.0</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E223" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F223" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G223" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="H223" s="6">
-        <v>99030.54</v>
+        <v>167797.46</v>
       </c>
       <c r="I223" s="4"/>
       <c r="J223" s="4"/>
@@ -11791,28 +11786,28 @@
     <row r="224" ht="14.25" customHeight="1">
       <c r="A224" s="4">
         <f t="shared" si="1"/>
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>304</v>
       </c>
       <c r="C224" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E224" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F224" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G224" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H224" s="6">
-        <v>167797.46</v>
+        <v>164506.52</v>
       </c>
       <c r="I224" s="4"/>
       <c r="J224" s="4"/>
@@ -11839,25 +11834,25 @@
         <v>246</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C225" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E225" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F225" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G225" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H225" s="6">
-        <v>164506.52</v>
+        <v>102411.31</v>
       </c>
       <c r="I225" s="4"/>
       <c r="J225" s="4"/>
@@ -11881,28 +11876,28 @@
     <row r="226" ht="14.25" customHeight="1">
       <c r="A226" s="4">
         <f t="shared" si="1"/>
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B226" s="4" t="s">
         <v>305</v>
       </c>
       <c r="C226" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D226" s="4" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E226" s="7" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="F226" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G226" s="4" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="H226" s="6">
-        <v>102411.31</v>
+        <v>150425.43</v>
       </c>
       <c r="I226" s="4"/>
       <c r="J226" s="4"/>
@@ -11929,25 +11924,25 @@
         <v>250</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C227" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E227" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F227" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G227" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H227" s="6">
-        <v>150425.43</v>
+        <v>97451.86</v>
       </c>
       <c r="I227" s="4"/>
       <c r="J227" s="4"/>
@@ -11974,25 +11969,25 @@
         <v>250</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C228" s="5">
         <v>45838.0</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E228" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F228" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G228" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="H228" s="6">
-        <v>97451.86</v>
+        <v>106262.99</v>
       </c>
       <c r="I228" s="4"/>
       <c r="J228" s="4"/>
@@ -12016,28 +12011,28 @@
     <row r="229" ht="14.25" customHeight="1">
       <c r="A229" s="4">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="B229" s="4" t="s">
         <v>306</v>
       </c>
       <c r="C229" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E229" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F229" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G229" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H229" s="6">
-        <v>106262.99</v>
+        <v>14844.6</v>
       </c>
       <c r="I229" s="4"/>
       <c r="J229" s="4"/>
@@ -12061,28 +12056,28 @@
     <row r="230" ht="14.25" customHeight="1">
       <c r="A230" s="4">
         <f t="shared" si="1"/>
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B230" s="4" t="s">
         <v>307</v>
       </c>
       <c r="C230" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E230" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F230" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G230" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H230" s="6">
-        <v>14844.6</v>
+        <v>44962.66</v>
       </c>
       <c r="I230" s="4"/>
       <c r="J230" s="4"/>
@@ -12106,28 +12101,28 @@
     <row r="231" ht="14.25" customHeight="1">
       <c r="A231" s="4">
         <f t="shared" si="1"/>
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="B231" s="4" t="s">
         <v>308</v>
       </c>
       <c r="C231" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E231" s="7" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="F231" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G231" s="4" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="H231" s="6">
-        <v>44962.66</v>
+        <v>135324.67</v>
       </c>
       <c r="I231" s="4"/>
       <c r="J231" s="4"/>
@@ -12154,25 +12149,25 @@
         <v>271</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C232" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E232" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F232" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G232" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H232" s="6">
-        <v>135324.67</v>
+        <v>187600.05</v>
       </c>
       <c r="I232" s="4"/>
       <c r="J232" s="4"/>
@@ -12196,28 +12191,28 @@
     <row r="233" ht="14.25" customHeight="1">
       <c r="A233" s="4">
         <f t="shared" si="1"/>
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B233" s="4" t="s">
         <v>309</v>
       </c>
       <c r="C233" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E233" s="7" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="F233" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G233" s="4" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="H233" s="6">
-        <v>187600.05</v>
+        <v>72851.55</v>
       </c>
       <c r="I233" s="4"/>
       <c r="J233" s="4"/>
@@ -12244,25 +12239,25 @@
         <v>275</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C234" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E234" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F234" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G234" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H234" s="6">
-        <v>72851.55</v>
+        <v>191921.79</v>
       </c>
       <c r="I234" s="4"/>
       <c r="J234" s="4"/>
@@ -12289,25 +12284,25 @@
         <v>275</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C235" s="5">
         <v>45838.0</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E235" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F235" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G235" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="H235" s="6">
-        <v>191921.79</v>
+        <v>65661.18</v>
       </c>
       <c r="I235" s="4"/>
       <c r="J235" s="4"/>
@@ -12331,28 +12326,28 @@
     <row r="236" ht="14.25" customHeight="1">
       <c r="A236" s="4">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B236" s="4" t="s">
         <v>310</v>
       </c>
       <c r="C236" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E236" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F236" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G236" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H236" s="6">
-        <v>65661.18</v>
+        <v>127226.25</v>
       </c>
       <c r="I236" s="4"/>
       <c r="J236" s="4"/>
@@ -12376,28 +12371,28 @@
     <row r="237" ht="14.25" customHeight="1">
       <c r="A237" s="4">
         <f t="shared" si="1"/>
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B237" s="4" t="s">
         <v>311</v>
       </c>
       <c r="C237" s="5">
-        <v>45835.0</v>
+        <v>45833.0</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E237" s="7" t="s">
-        <v>20</v>
+        <v>312</v>
+      </c>
+      <c r="E237" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="F237" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G237" s="4" t="s">
-        <v>22</v>
+        <v>314</v>
       </c>
       <c r="H237" s="6">
-        <v>127226.25</v>
+        <v>-24054.55</v>
       </c>
       <c r="I237" s="4"/>
       <c r="J237" s="4"/>
@@ -12424,25 +12419,25 @@
         <v>288</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C238" s="5">
-        <v>45833.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D238" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="E238" s="4" t="s">
-        <v>314</v>
+        <v>19</v>
+      </c>
+      <c r="E238" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F238" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G238" s="4" t="s">
-        <v>315</v>
+        <v>22</v>
       </c>
       <c r="H238" s="6">
-        <v>-24054.55</v>
+        <v>4627.92</v>
       </c>
       <c r="I238" s="4"/>
       <c r="J238" s="4"/>
@@ -12469,25 +12464,25 @@
         <v>288</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C239" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E239" s="7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="F239" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="H239" s="6">
-        <v>4627.92</v>
+        <v>128346.29</v>
       </c>
       <c r="I239" s="4"/>
       <c r="J239" s="4"/>
@@ -12514,25 +12509,25 @@
         <v>288</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C240" s="5">
-        <v>45838.0</v>
+        <v>45845.0</v>
       </c>
       <c r="D240" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E240" s="7" t="s">
-        <v>52</v>
+        <v>60</v>
+      </c>
+      <c r="E240" s="4" t="s">
+        <v>315</v>
       </c>
       <c r="F240" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G240" s="4" t="s">
-        <v>53</v>
+        <v>316</v>
       </c>
       <c r="H240" s="6">
-        <v>128346.29</v>
+        <v>-14057.68</v>
       </c>
       <c r="I240" s="4"/>
       <c r="J240" s="4"/>
@@ -12556,28 +12551,28 @@
     <row r="241" ht="14.25" customHeight="1">
       <c r="A241" s="4">
         <f t="shared" si="1"/>
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C241" s="5">
-        <v>45845.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E241" s="4" t="s">
-        <v>316</v>
+        <v>19</v>
+      </c>
+      <c r="E241" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F241" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G241" s="4" t="s">
-        <v>317</v>
+        <v>22</v>
       </c>
       <c r="H241" s="6">
-        <v>-14057.68</v>
+        <v>147844.8</v>
       </c>
       <c r="I241" s="4"/>
       <c r="J241" s="4"/>
@@ -12604,25 +12599,25 @@
         <v>290</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C242" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E242" s="7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="F242" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G242" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="H242" s="6">
-        <v>147844.8</v>
+        <v>131995.33</v>
       </c>
       <c r="I242" s="4"/>
       <c r="J242" s="4"/>
@@ -12646,7 +12641,7 @@
     <row r="243" ht="14.25" customHeight="1">
       <c r="A243" s="4">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B243" s="4" t="s">
         <v>318</v>
@@ -12655,19 +12650,19 @@
         <v>45838.0</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E243" s="7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="F243" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G243" s="4" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="H243" s="6">
-        <v>131995.33</v>
+        <v>59371.25</v>
       </c>
       <c r="I243" s="4"/>
       <c r="J243" s="4"/>
@@ -12691,7 +12686,7 @@
     <row r="244" ht="14.25" customHeight="1">
       <c r="A244" s="4">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="B244" s="4" t="s">
         <v>319</v>
@@ -12712,7 +12707,7 @@
         <v>74</v>
       </c>
       <c r="H244" s="6">
-        <v>59371.25</v>
+        <v>50806.93</v>
       </c>
       <c r="I244" s="4"/>
       <c r="J244" s="4"/>
@@ -12736,7 +12731,7 @@
     <row r="245" ht="14.25" customHeight="1">
       <c r="A245" s="4">
         <f t="shared" si="1"/>
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="B245" s="4" t="s">
         <v>320</v>
@@ -12745,19 +12740,19 @@
         <v>45838.0</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>72</v>
+        <v>246</v>
       </c>
       <c r="E245" s="7" t="s">
-        <v>73</v>
+        <v>247</v>
       </c>
       <c r="F245" s="4" t="s">
-        <v>25</v>
+        <v>248</v>
       </c>
       <c r="G245" s="4" t="s">
-        <v>74</v>
+        <v>249</v>
       </c>
       <c r="H245" s="6">
-        <v>50806.93</v>
+        <v>21297.11</v>
       </c>
       <c r="I245" s="4"/>
       <c r="J245" s="4"/>
@@ -12781,7 +12776,7 @@
     <row r="246" ht="14.25" customHeight="1">
       <c r="A246" s="4">
         <f t="shared" si="1"/>
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B246" s="4" t="s">
         <v>321</v>
@@ -12790,19 +12785,19 @@
         <v>45838.0</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>246</v>
+        <v>51</v>
       </c>
       <c r="E246" s="7" t="s">
-        <v>247</v>
+        <v>52</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>248</v>
+        <v>21</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
       <c r="H246" s="6">
-        <v>21297.11</v>
+        <v>43056.89</v>
       </c>
       <c r="I246" s="4"/>
       <c r="J246" s="4"/>
@@ -12826,28 +12821,28 @@
     <row r="247" ht="14.25" customHeight="1">
       <c r="A247" s="4">
         <f t="shared" si="1"/>
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B247" s="4" t="s">
         <v>322</v>
       </c>
       <c r="C247" s="5">
-        <v>45838.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E247" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F247" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G247" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="H247" s="6">
-        <v>43056.89</v>
+        <v>23399.51</v>
       </c>
       <c r="I247" s="4"/>
       <c r="J247" s="4"/>
@@ -12871,7 +12866,7 @@
     <row r="248" ht="14.25" customHeight="1">
       <c r="A248" s="4">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>1002</v>
       </c>
       <c r="B248" s="4" t="s">
         <v>323</v>
@@ -12892,7 +12887,7 @@
         <v>22</v>
       </c>
       <c r="H248" s="6">
-        <v>23399.51</v>
+        <v>326368.06</v>
       </c>
       <c r="I248" s="4"/>
       <c r="J248" s="4"/>
@@ -12919,25 +12914,25 @@
         <v>1002</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C249" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E249" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F249" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G249" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H249" s="6">
-        <v>326368.06</v>
+        <v>106550.21</v>
       </c>
       <c r="I249" s="4"/>
       <c r="J249" s="4"/>
@@ -12964,25 +12959,25 @@
         <v>1002</v>
       </c>
       <c r="B250" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C250" s="5">
+        <v>45839.0</v>
+      </c>
+      <c r="D250" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E250" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C250" s="5">
-        <v>45838.0</v>
-      </c>
-      <c r="D250" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E250" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="F250" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="G250" s="4" t="s">
-        <v>74</v>
+        <v>325</v>
       </c>
       <c r="H250" s="6">
-        <v>106550.21</v>
+        <v>35232.1</v>
       </c>
       <c r="I250" s="4"/>
       <c r="J250" s="4"/>
@@ -13004,30 +12999,30 @@
       <c r="Z250" s="4"/>
     </row>
     <row r="251" ht="14.25" customHeight="1">
-      <c r="A251" s="4">
+      <c r="A251" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>1002</v>
+        <v/>
       </c>
       <c r="B251" s="4" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C251" s="5">
-        <v>45839.0</v>
+        <v>45834.0</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E251" s="4" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F251" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G251" s="4" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="H251" s="6">
-        <v>35232.1</v>
+        <v>127702.0</v>
       </c>
       <c r="I251" s="4"/>
       <c r="J251" s="4"/>
@@ -13049,30 +13044,30 @@
       <c r="Z251" s="4"/>
     </row>
     <row r="252" ht="14.25" customHeight="1">
-      <c r="A252" s="4" t="str">
+      <c r="A252" s="4">
         <f t="shared" si="1"/>
-        <v/>
+        <v>400</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C252" s="5">
-        <v>45834.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E252" s="4" t="s">
-        <v>328</v>
+        <v>19</v>
+      </c>
+      <c r="E252" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F252" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G252" s="4" t="s">
-        <v>329</v>
+        <v>22</v>
       </c>
       <c r="H252" s="6">
-        <v>127702.0</v>
+        <v>413223.14</v>
       </c>
       <c r="I252" s="4"/>
       <c r="J252" s="4"/>
@@ -13099,25 +13094,25 @@
         <v>400</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C253" s="5">
-        <v>45835.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E253" s="7" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F253" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G253" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H253" s="6">
-        <v>413223.14</v>
+        <v>381610.37</v>
       </c>
       <c r="I253" s="4"/>
       <c r="J253" s="4"/>
@@ -13139,30 +13134,30 @@
       <c r="Z253" s="4"/>
     </row>
     <row r="254" ht="14.25" customHeight="1">
-      <c r="A254" s="4">
+      <c r="A254" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v/>
       </c>
       <c r="B254" s="4" t="s">
         <v>330</v>
       </c>
       <c r="C254" s="5">
-        <v>45838.0</v>
+        <v>45809.0</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E254" s="7" t="s">
-        <v>73</v>
+        <v>331</v>
+      </c>
+      <c r="E254" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="F254" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="G254" s="4" t="s">
-        <v>74</v>
+        <v>333</v>
       </c>
       <c r="H254" s="6">
-        <v>381610.37</v>
+        <v>1.062512396E7</v>
       </c>
       <c r="I254" s="4"/>
       <c r="J254" s="4"/>
@@ -13189,25 +13184,25 @@
         <v/>
       </c>
       <c r="B255" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C255" s="5">
-        <v>45809.0</v>
+        <v>45811.0</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E255" s="4" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F255" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G255" s="4" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="H255" s="6">
-        <v>1.062512396E7</v>
+        <v>454544.63</v>
       </c>
       <c r="I255" s="4"/>
       <c r="J255" s="4"/>
@@ -13234,25 +13229,25 @@
         <v/>
       </c>
       <c r="B256" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C256" s="5">
-        <v>45811.0</v>
+        <v>45852.0</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>335</v>
+        <v>29</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F256" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G256" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H256" s="6">
-        <v>454544.63</v>
+        <v>74380.17</v>
       </c>
       <c r="I256" s="4"/>
       <c r="J256" s="4"/>
@@ -13279,26 +13274,24 @@
         <v/>
       </c>
       <c r="B257" s="4" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C257" s="5">
-        <v>45852.0</v>
+        <v>45809.0</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E257" s="4" t="s">
-        <v>338</v>
+        <v>212</v>
+      </c>
+      <c r="E257" s="7" t="s">
+        <v>340</v>
       </c>
       <c r="F257" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G257" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="H257" s="6">
-        <v>74380.17</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="H257" s="6"/>
       <c r="I257" s="4"/>
       <c r="J257" s="4"/>
       <c r="K257" s="4"/>
@@ -13324,7 +13317,7 @@
         <v/>
       </c>
       <c r="B258" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C258" s="5">
         <v>45809.0</v>
@@ -13333,7 +13326,7 @@
         <v>212</v>
       </c>
       <c r="E258" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F258" s="4" t="s">
         <v>11</v>
@@ -13341,7 +13334,9 @@
       <c r="G258" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="H258" s="6"/>
+      <c r="H258" s="6">
+        <v>-8985.74</v>
+      </c>
       <c r="I258" s="4"/>
       <c r="J258" s="4"/>
       <c r="K258" s="4"/>
@@ -13367,7 +13362,7 @@
         <v/>
       </c>
       <c r="B259" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C259" s="5">
         <v>45809.0</v>
@@ -13375,17 +13370,17 @@
       <c r="D259" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="E259" s="7" t="s">
-        <v>341</v>
+      <c r="E259" s="4" t="s">
+        <v>343</v>
       </c>
       <c r="F259" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G259" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H259" s="6">
-        <v>-8985.74</v>
+        <v>-5418.28</v>
       </c>
       <c r="I259" s="4"/>
       <c r="J259" s="4"/>
@@ -13412,7 +13407,7 @@
         <v/>
       </c>
       <c r="B260" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C260" s="5">
         <v>45809.0</v>
@@ -13427,10 +13422,10 @@
         <v>11</v>
       </c>
       <c r="G260" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H260" s="6">
-        <v>-5418.28</v>
+        <v>-7541.15</v>
       </c>
       <c r="I260" s="4"/>
       <c r="J260" s="4"/>
@@ -13452,18 +13447,18 @@
       <c r="Z260" s="4"/>
     </row>
     <row r="261" ht="14.25" customHeight="1">
-      <c r="A261" s="4" t="str">
+      <c r="A261" s="4">
         <f t="shared" si="1"/>
-        <v/>
+        <v>76</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>340</v>
+        <v>206</v>
       </c>
       <c r="C261" s="5">
-        <v>45809.0</v>
+        <v>45814.0</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E261" s="4" t="s">
         <v>345</v>
@@ -13472,10 +13467,10 @@
         <v>11</v>
       </c>
       <c r="G261" s="4" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="H261" s="6">
-        <v>-7541.15</v>
+        <v>-173553.54</v>
       </c>
       <c r="I261" s="4"/>
       <c r="J261" s="4"/>
@@ -13497,30 +13492,30 @@
       <c r="Z261" s="4"/>
     </row>
     <row r="262" ht="14.25" customHeight="1">
-      <c r="A262" s="4">
+      <c r="A262" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v/>
       </c>
       <c r="B262" s="4" t="s">
-        <v>206</v>
+        <v>339</v>
       </c>
       <c r="C262" s="5">
         <v>45814.0</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="E262" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F262" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G262" s="4" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="H262" s="6">
-        <v>-173553.54</v>
+        <v>-9703.06</v>
       </c>
       <c r="I262" s="4"/>
       <c r="J262" s="4"/>
@@ -13547,25 +13542,25 @@
         <v/>
       </c>
       <c r="B263" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C263" s="5">
-        <v>45814.0</v>
+        <v>45816.0</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E263" s="4" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F263" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G263" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="H263" s="6">
-        <v>-9703.06</v>
+        <v>-9455.21</v>
       </c>
       <c r="I263" s="4"/>
       <c r="J263" s="4"/>
@@ -13591,26 +13586,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B264" s="4" t="s">
-        <v>340</v>
+      <c r="B264" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="C264" s="5">
-        <v>45816.0</v>
+        <v>45819.0</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E264" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F264" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G264" s="4" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="H264" s="6">
-        <v>-9455.21</v>
+        <v>349752.2</v>
       </c>
       <c r="I264" s="4"/>
       <c r="J264" s="4"/>
@@ -13636,26 +13631,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B265" s="11" t="s">
-        <v>340</v>
+      <c r="B265" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="C265" s="5">
-        <v>45819.0</v>
+        <v>45822.0</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="E265" s="4" t="s">
-        <v>355</v>
+        <v>136</v>
+      </c>
+      <c r="E265" s="7" t="s">
+        <v>356</v>
       </c>
       <c r="F265" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G265" s="4" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="H265" s="6">
-        <v>349752.2</v>
+        <v>-5427.22</v>
       </c>
       <c r="I265" s="4"/>
       <c r="J265" s="4"/>
@@ -13682,7 +13677,7 @@
         <v/>
       </c>
       <c r="B266" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C266" s="5">
         <v>45822.0</v>
@@ -13691,16 +13686,17 @@
         <v>136</v>
       </c>
       <c r="E266" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F266" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G266" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="H266" s="6">
-        <v>-5427.22</v>
+      <c r="G266" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H266" s="10">
+        <f>9375.19</f>
+        <v>9375.19</v>
       </c>
       <c r="I266" s="4"/>
       <c r="J266" s="4"/>
@@ -13727,26 +13723,25 @@
         <v/>
       </c>
       <c r="B267" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C267" s="5">
-        <v>45822.0</v>
+        <v>45825.0</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E267" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E267" s="4" t="s">
         <v>357</v>
       </c>
       <c r="F267" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G267" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="H267" s="10">
-        <f>9375.19</f>
-        <v>9375.19</v>
+      <c r="G267" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="H267" s="6">
+        <v>-8938.02</v>
       </c>
       <c r="I267" s="4"/>
       <c r="J267" s="4"/>
@@ -13772,26 +13767,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B268" s="4" t="s">
-        <v>340</v>
+      <c r="B268" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="C268" s="5">
-        <v>45825.0</v>
-      </c>
-      <c r="D268" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E268" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="F268" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G268" s="4" t="s">
+        <v>45826.0</v>
+      </c>
+      <c r="D268" s="11" t="s">
         <v>359</v>
       </c>
+      <c r="E268" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="F268" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="G268" s="11" t="s">
+        <v>362</v>
+      </c>
       <c r="H268" s="6">
-        <v>-8938.02</v>
+        <v>260000.0</v>
       </c>
       <c r="I268" s="4"/>
       <c r="J268" s="4"/>
@@ -13817,26 +13812,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B269" s="11" t="s">
-        <v>340</v>
+      <c r="B269" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="C269" s="5">
-        <v>45826.0</v>
-      </c>
-      <c r="D269" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="E269" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="F269" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="G269" s="11" t="s">
+        <v>45827.0</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E269" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="F269" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G269" s="4" t="s">
+        <v>364</v>
+      </c>
       <c r="H269" s="6">
-        <v>260000.0</v>
+        <v>-6697.96</v>
       </c>
       <c r="I269" s="4"/>
       <c r="J269" s="4"/>
@@ -13863,25 +13858,25 @@
         <v/>
       </c>
       <c r="B270" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C270" s="5">
-        <v>45827.0</v>
+        <v>45832.0</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>60</v>
+        <v>212</v>
       </c>
       <c r="E270" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F270" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G270" s="4" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="H270" s="6">
-        <v>-6697.96</v>
+        <v>-4307.88</v>
       </c>
       <c r="I270" s="4"/>
       <c r="J270" s="4"/>
@@ -13907,26 +13902,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B271" s="4" t="s">
-        <v>340</v>
+      <c r="B271" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="C271" s="5">
-        <v>45832.0</v>
+        <v>45834.0</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>212</v>
+        <v>366</v>
       </c>
       <c r="E271" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F271" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G271" s="4" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="H271" s="6">
-        <v>-4307.88</v>
+        <v>187832.97</v>
       </c>
       <c r="I271" s="4"/>
       <c r="J271" s="4"/>
@@ -13952,26 +13947,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B272" s="11" t="s">
-        <v>340</v>
+      <c r="B272" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="C272" s="5">
         <v>45834.0</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E272" s="4" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F272" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G272" s="4" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="H272" s="6">
-        <v>187832.97</v>
+        <v>-17377.96</v>
       </c>
       <c r="I272" s="4"/>
       <c r="J272" s="4"/>
@@ -13998,13 +13993,13 @@
         <v/>
       </c>
       <c r="B273" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C273" s="5">
-        <v>45834.0</v>
+        <v>45835.0</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>370</v>
+        <v>60</v>
       </c>
       <c r="E273" s="4" t="s">
         <v>371</v>
@@ -14013,10 +14008,10 @@
         <v>11</v>
       </c>
       <c r="G273" s="4" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="H273" s="6">
-        <v>-17377.96</v>
+        <v>2250000.0</v>
       </c>
       <c r="I273" s="4"/>
       <c r="J273" s="4"/>
@@ -14043,25 +14038,25 @@
         <v/>
       </c>
       <c r="B274" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C274" s="5">
         <v>45835.0</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="E274" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F274" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G274" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H274" s="6">
-        <v>2250000.0</v>
+        <v>-11158.72</v>
       </c>
       <c r="I274" s="4"/>
       <c r="J274" s="4"/>
@@ -14088,25 +14083,25 @@
         <v/>
       </c>
       <c r="B275" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C275" s="5">
-        <v>45835.0</v>
+        <v>45841.0</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>136</v>
+        <v>212</v>
       </c>
       <c r="E275" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F275" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G275" s="4" t="s">
-        <v>375</v>
+        <v>342</v>
       </c>
       <c r="H275" s="6">
-        <v>-11158.72</v>
+        <v>-7176.73</v>
       </c>
       <c r="I275" s="4"/>
       <c r="J275" s="4"/>
@@ -14133,25 +14128,25 @@
         <v/>
       </c>
       <c r="B276" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C276" s="5">
-        <v>45841.0</v>
+        <v>45860.0</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>212</v>
+        <v>376</v>
       </c>
       <c r="E276" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F276" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G276" s="4" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
       <c r="H276" s="6">
-        <v>-7176.73</v>
+        <v>760000.0</v>
       </c>
       <c r="I276" s="4"/>
       <c r="J276" s="4"/>
@@ -14173,30 +14168,30 @@
       <c r="Z276" s="4"/>
     </row>
     <row r="277" ht="14.25" customHeight="1">
-      <c r="A277" s="4" t="str">
+      <c r="A277" s="4">
         <f t="shared" si="1"/>
-        <v/>
+        <v>144</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>340</v>
+        <v>379</v>
       </c>
       <c r="C277" s="5">
-        <v>45860.0</v>
+        <v>45838.0</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="E277" s="4" t="s">
-        <v>378</v>
+        <v>72</v>
+      </c>
+      <c r="E277" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="F277" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="G277" s="4" t="s">
-        <v>379</v>
+        <v>74</v>
       </c>
       <c r="H277" s="6">
-        <v>760000.0</v>
+        <v>83872.61</v>
       </c>
       <c r="I277" s="4"/>
       <c r="J277" s="4"/>
@@ -14220,10 +14215,10 @@
     <row r="278" ht="14.25" customHeight="1">
       <c r="A278" s="4">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>380</v>
+        <v>110</v>
       </c>
       <c r="C278" s="5">
         <v>45838.0</v>
@@ -14237,11 +14232,11 @@
       <c r="F278" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G278" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H278" s="6">
-        <v>83872.61</v>
+      <c r="G278" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="H278" s="10">
+        <v>-184300.43</v>
       </c>
       <c r="I278" s="4"/>
       <c r="J278" s="4"/>
@@ -14263,30 +14258,30 @@
       <c r="Z278" s="4"/>
     </row>
     <row r="279" ht="14.25" customHeight="1">
-      <c r="A279" s="4">
+      <c r="A279" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v/>
       </c>
       <c r="B279" s="4" t="s">
-        <v>110</v>
+        <v>339</v>
       </c>
       <c r="C279" s="5">
-        <v>45838.0</v>
+        <v>45822.0</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="E279" s="7" t="s">
-        <v>73</v>
+        <v>356</v>
       </c>
       <c r="F279" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="G279" s="9" t="s">
         <v>381</v>
       </c>
       <c r="H279" s="10">
-        <v>-184300.43</v>
+        <v>-9375.19</v>
       </c>
       <c r="I279" s="4"/>
       <c r="J279" s="4"/>
@@ -14313,7 +14308,7 @@
         <v/>
       </c>
       <c r="B280" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C280" s="5">
         <v>45822.0</v>
@@ -14322,7 +14317,7 @@
         <v>136</v>
       </c>
       <c r="E280" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F280" s="4" t="s">
         <v>11</v>
@@ -14330,8 +14325,9 @@
       <c r="G280" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="H280" s="10">
-        <v>-9375.19</v>
+      <c r="H280" s="12">
+        <f>9375.19-9375.19-1968.79</f>
+        <v>-1968.79</v>
       </c>
       <c r="I280" s="4"/>
       <c r="J280" s="4"/>
@@ -14353,31 +14349,30 @@
       <c r="Z280" s="4"/>
     </row>
     <row r="281" ht="14.25" customHeight="1">
-      <c r="A281" s="4" t="str">
+      <c r="A281" s="4">
         <f t="shared" si="1"/>
-        <v/>
+        <v>35</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>340</v>
+        <v>119</v>
       </c>
       <c r="C281" s="5">
-        <v>45822.0</v>
+        <v>45843.0</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E281" s="7" t="s">
-        <v>357</v>
+        <v>128</v>
       </c>
       <c r="F281" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G281" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="H281" s="12">
-        <f>9375.19-9375.19-1968.79</f>
-        <v>-1968.79</v>
+      <c r="H281" s="10">
+        <v>-9305.04</v>
       </c>
       <c r="I281" s="4"/>
       <c r="J281" s="4"/>
@@ -14421,8 +14416,9 @@
       <c r="G282" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="H282" s="10">
-        <v>-9305.04</v>
+      <c r="H282" s="12">
+        <f>9305.04-9305.04-977.03</f>
+        <v>-977.03</v>
       </c>
       <c r="I282" s="4"/>
       <c r="J282" s="4"/>
@@ -14446,29 +14442,28 @@
     <row r="283" ht="14.25" customHeight="1">
       <c r="A283" s="4">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
       <c r="C283" s="5">
-        <v>45843.0</v>
+        <v>45845.0</v>
       </c>
       <c r="D283" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E283" s="7" t="s">
-        <v>128</v>
+        <v>385</v>
+      </c>
+      <c r="E283" s="4" t="s">
+        <v>386</v>
       </c>
       <c r="F283" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G283" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="H283" s="12">
-        <f>9305.04-9305.04-977.03</f>
-        <v>-977.03</v>
+        <v>387</v>
+      </c>
+      <c r="G283" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="H283" s="6">
+        <v>17019.92</v>
       </c>
       <c r="I283" s="4"/>
       <c r="J283" s="4"/>
@@ -14501,19 +14496,19 @@
         <v>45845.0</v>
       </c>
       <c r="D284" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E284" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="E284" s="4" t="s">
+      <c r="F284" s="4" t="s">
         <v>387</v>
-      </c>
-      <c r="F284" s="4" t="s">
-        <v>388</v>
       </c>
       <c r="G284" s="4" t="s">
         <v>389</v>
       </c>
       <c r="H284" s="6">
-        <v>17019.92</v>
+        <v>123695.71</v>
       </c>
       <c r="I284" s="4"/>
       <c r="J284" s="4"/>
@@ -14546,19 +14541,19 @@
         <v>45845.0</v>
       </c>
       <c r="D285" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E285" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="E285" s="4" t="s">
+      <c r="F285" s="4" t="s">
         <v>387</v>
-      </c>
-      <c r="F285" s="4" t="s">
-        <v>388</v>
       </c>
       <c r="G285" s="4" t="s">
         <v>390</v>
       </c>
       <c r="H285" s="6">
-        <v>123695.71</v>
+        <v>3007.39</v>
       </c>
       <c r="I285" s="4"/>
       <c r="J285" s="4"/>
@@ -14591,19 +14586,19 @@
         <v>45845.0</v>
       </c>
       <c r="D286" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E286" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F286" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="F286" s="4" t="s">
-        <v>388</v>
-      </c>
       <c r="G286" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H286" s="6">
-        <v>3007.39</v>
+        <v>350000.0</v>
       </c>
       <c r="I286" s="4"/>
       <c r="J286" s="4"/>
@@ -14633,22 +14628,22 @@
         <v>8</v>
       </c>
       <c r="C287" s="5">
-        <v>45845.0</v>
+        <v>45848.0</v>
       </c>
       <c r="D287" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E287" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F287" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G287" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H287" s="6">
-        <v>350000.0</v>
+        <v>527037.09</v>
       </c>
       <c r="I287" s="4"/>
       <c r="J287" s="4"/>
@@ -14681,19 +14676,19 @@
         <v>45848.0</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E288" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F288" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G288" s="4" t="s">
         <v>395</v>
       </c>
       <c r="H288" s="6">
-        <v>527037.09</v>
+        <v>587067.87</v>
       </c>
       <c r="I288" s="4"/>
       <c r="J288" s="4"/>
@@ -14723,22 +14718,22 @@
         <v>8</v>
       </c>
       <c r="C289" s="5">
-        <v>45848.0</v>
+        <v>45852.0</v>
       </c>
       <c r="D289" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E289" s="4" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F289" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G289" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H289" s="6">
-        <v>587067.87</v>
+        <v>258889.7</v>
       </c>
       <c r="I289" s="4"/>
       <c r="J289" s="4"/>
@@ -14768,22 +14763,22 @@
         <v>8</v>
       </c>
       <c r="C290" s="5">
-        <v>45852.0</v>
+        <v>45853.0</v>
       </c>
       <c r="D290" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E290" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F290" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G290" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H290" s="6">
-        <v>258889.7</v>
+        <v>50000.0</v>
       </c>
       <c r="I290" s="4"/>
       <c r="J290" s="4"/>
@@ -14816,19 +14811,19 @@
         <v>45853.0</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E291" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F291" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G291" s="4" t="s">
         <v>400</v>
       </c>
       <c r="H291" s="6">
-        <v>50000.0</v>
+        <v>550000.0</v>
       </c>
       <c r="I291" s="4"/>
       <c r="J291" s="4"/>
@@ -14858,22 +14853,22 @@
         <v>8</v>
       </c>
       <c r="C292" s="5">
-        <v>45853.0</v>
+        <v>45862.0</v>
       </c>
       <c r="D292" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E292" s="4" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="F292" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G292" s="4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H292" s="6">
-        <v>550000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="I292" s="4"/>
       <c r="J292" s="4"/>
@@ -14897,28 +14892,28 @@
     <row r="293" ht="14.25" customHeight="1">
       <c r="A293" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C293" s="5">
-        <v>45862.0</v>
+        <v>45840.0</v>
       </c>
       <c r="D293" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E293" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F293" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G293" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H293" s="6">
-        <v>120000.0</v>
+        <v>393000.19</v>
       </c>
       <c r="I293" s="4"/>
       <c r="J293" s="4"/>
@@ -14948,22 +14943,22 @@
         <v>32</v>
       </c>
       <c r="C294" s="5">
-        <v>45840.0</v>
+        <v>45852.0</v>
       </c>
       <c r="D294" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E294" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F294" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G294" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H294" s="6">
-        <v>393000.19</v>
+        <v>182473.4</v>
       </c>
       <c r="I294" s="4"/>
       <c r="J294" s="4"/>
@@ -14993,22 +14988,22 @@
         <v>32</v>
       </c>
       <c r="C295" s="5">
-        <v>45852.0</v>
+        <v>45853.0</v>
       </c>
       <c r="D295" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E295" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F295" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G295" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H295" s="6">
-        <v>182473.4</v>
+        <v>300547.01</v>
       </c>
       <c r="I295" s="4"/>
       <c r="J295" s="4"/>
@@ -15041,19 +15036,19 @@
         <v>45853.0</v>
       </c>
       <c r="D296" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E296" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F296" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G296" s="4" t="s">
         <v>409</v>
       </c>
       <c r="H296" s="6">
-        <v>300547.01</v>
+        <v>301676.78</v>
       </c>
       <c r="I296" s="4"/>
       <c r="J296" s="4"/>
@@ -15083,22 +15078,22 @@
         <v>32</v>
       </c>
       <c r="C297" s="5">
-        <v>45853.0</v>
+        <v>45859.0</v>
       </c>
       <c r="D297" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E297" s="4" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="F297" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G297" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H297" s="6">
-        <v>301676.78</v>
+        <v>200190.14</v>
       </c>
       <c r="I297" s="4"/>
       <c r="J297" s="4"/>
@@ -15128,22 +15123,22 @@
         <v>32</v>
       </c>
       <c r="C298" s="5">
-        <v>45859.0</v>
+        <v>45863.0</v>
       </c>
       <c r="D298" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E298" s="4" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F298" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G298" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H298" s="6">
-        <v>200190.14</v>
+        <v>54684.0</v>
       </c>
       <c r="I298" s="4"/>
       <c r="J298" s="4"/>
@@ -15173,22 +15168,22 @@
         <v>32</v>
       </c>
       <c r="C299" s="5">
-        <v>45863.0</v>
+        <v>45866.0</v>
       </c>
       <c r="D299" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E299" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F299" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G299" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H299" s="6">
-        <v>54684.0</v>
+        <v>144379.5</v>
       </c>
       <c r="I299" s="4"/>
       <c r="J299" s="4"/>
@@ -15212,28 +15207,28 @@
     <row r="300" ht="14.25" customHeight="1">
       <c r="A300" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>32</v>
+        <v>223</v>
       </c>
       <c r="C300" s="5">
-        <v>45866.0</v>
+        <v>45856.0</v>
       </c>
       <c r="D300" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E300" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F300" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G300" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H300" s="6">
-        <v>144379.5</v>
+        <v>50000.0</v>
       </c>
       <c r="I300" s="4"/>
       <c r="J300" s="4"/>
@@ -15263,19 +15258,19 @@
         <v>223</v>
       </c>
       <c r="C301" s="5">
-        <v>45856.0</v>
+        <v>45863.0</v>
       </c>
       <c r="D301" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E301" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F301" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G301" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H301" s="6">
         <v>50000.0</v>
@@ -15302,28 +15297,28 @@
     <row r="302" ht="14.25" customHeight="1">
       <c r="A302" s="4">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C302" s="5">
-        <v>45863.0</v>
+        <v>45845.0</v>
       </c>
       <c r="D302" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E302" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F302" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G302" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H302" s="6">
-        <v>50000.0</v>
+        <v>552000.0</v>
       </c>
       <c r="I302" s="4"/>
       <c r="J302" s="4"/>
@@ -15353,22 +15348,22 @@
         <v>237</v>
       </c>
       <c r="C303" s="5">
-        <v>45845.0</v>
+        <v>45856.0</v>
       </c>
       <c r="D303" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E303" s="4" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F303" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G303" s="4" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H303" s="6">
-        <v>552000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="I303" s="4"/>
       <c r="J303" s="4"/>
@@ -15392,25 +15387,25 @@
     <row r="304" ht="14.25" customHeight="1">
       <c r="A304" s="4">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C304" s="5">
-        <v>45856.0</v>
+        <v>45863.0</v>
       </c>
       <c r="D304" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E304" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F304" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G304" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H304" s="6">
         <v>50000.0</v>
@@ -15437,28 +15432,28 @@
     <row r="305" ht="14.25" customHeight="1">
       <c r="A305" s="4">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C305" s="5">
-        <v>45863.0</v>
+        <v>45860.0</v>
       </c>
       <c r="D305" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E305" s="4" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="F305" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G305" s="4" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="H305" s="6">
-        <v>50000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="I305" s="4"/>
       <c r="J305" s="4"/>
@@ -15482,28 +15477,28 @@
     <row r="306" ht="14.25" customHeight="1">
       <c r="A306" s="4">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C306" s="5">
-        <v>45860.0</v>
+        <v>45863.0</v>
       </c>
       <c r="D306" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E306" s="4" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F306" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G306" s="4" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="H306" s="6">
-        <v>300000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="I306" s="4"/>
       <c r="J306" s="4"/>
@@ -15527,25 +15522,25 @@
     <row r="307" ht="14.25" customHeight="1">
       <c r="A307" s="4">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="C307" s="5">
         <v>45863.0</v>
       </c>
       <c r="D307" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E307" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="F307" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="G307" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="F307" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="G307" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="H307" s="6">
         <v>50000.0</v>
@@ -15572,25 +15567,25 @@
     <row r="308" ht="14.25" customHeight="1">
       <c r="A308" s="4">
         <f t="shared" si="1"/>
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C308" s="5">
-        <v>45863.0</v>
+        <v>45856.0</v>
       </c>
       <c r="D308" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E308" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F308" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G308" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H308" s="6">
         <v>50000.0</v>
@@ -15623,19 +15618,19 @@
         <v>269</v>
       </c>
       <c r="C309" s="5">
-        <v>45856.0</v>
+        <v>45863.0</v>
       </c>
       <c r="D309" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E309" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F309" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G309" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H309" s="6">
         <v>50000.0</v>
@@ -15662,25 +15657,25 @@
     <row r="310" ht="14.25" customHeight="1">
       <c r="A310" s="4">
         <f t="shared" si="1"/>
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="C310" s="5">
-        <v>45863.0</v>
+        <v>45856.0</v>
       </c>
       <c r="D310" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E310" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F310" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H310" s="6">
         <v>50000.0</v>
@@ -15707,28 +15702,28 @@
     <row r="311" ht="14.25" customHeight="1">
       <c r="A311" s="4">
         <f t="shared" si="1"/>
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="C311" s="5">
         <v>45856.0</v>
       </c>
       <c r="D311" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E311" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F311" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="G311" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="F311" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="G311" s="4" t="s">
-        <v>418</v>
-      </c>
       <c r="H311" s="6">
-        <v>50000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="I311" s="4"/>
       <c r="J311" s="4"/>
@@ -15752,28 +15747,28 @@
     <row r="312" ht="14.25" customHeight="1">
       <c r="A312" s="4">
         <f t="shared" si="1"/>
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C312" s="5">
-        <v>45856.0</v>
+        <v>45842.0</v>
       </c>
       <c r="D312" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E312" s="4" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="F312" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G312" s="4" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="H312" s="6">
-        <v>30000.0</v>
+        <v>286611.57</v>
       </c>
       <c r="I312" s="4"/>
       <c r="J312" s="4"/>
@@ -15797,28 +15792,28 @@
     <row r="313" ht="14.25" customHeight="1">
       <c r="A313" s="4">
         <f t="shared" si="1"/>
-        <v>251</v>
-      </c>
-      <c r="B313" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="C313" s="5">
-        <v>45842.0</v>
-      </c>
-      <c r="D313" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="E313" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="F313" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="G313" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="H313" s="6">
-        <v>286611.57</v>
+        <v>2</v>
+      </c>
+      <c r="B313" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C313" s="13">
+        <v>45810.0</v>
+      </c>
+      <c r="D313" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E313" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F313" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G313" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H313" s="14">
+        <v>-186405.0</v>
       </c>
       <c r="I313" s="4"/>
       <c r="J313" s="4"/>
@@ -15842,118 +15837,104 @@
     <row r="314" ht="14.25" customHeight="1">
       <c r="A314" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="B314" s="11" t="s">
-        <v>32</v>
+        <v>237</v>
       </c>
       <c r="C314" s="13">
-        <v>45810.0</v>
+        <v>45845.0</v>
       </c>
       <c r="D314" s="11" t="s">
-        <v>33</v>
+        <v>385</v>
       </c>
       <c r="E314" s="11" t="s">
-        <v>34</v>
+        <v>420</v>
       </c>
       <c r="F314" s="11" t="s">
-        <v>21</v>
+        <v>387</v>
       </c>
       <c r="G314" s="11" t="s">
-        <v>35</v>
+        <v>421</v>
       </c>
       <c r="H314" s="14">
-        <v>-186405.0</v>
-      </c>
-      <c r="I314" s="4"/>
-      <c r="J314" s="4"/>
-      <c r="K314" s="4"/>
-      <c r="L314" s="4"/>
-      <c r="M314" s="4"/>
-      <c r="N314" s="4"/>
-      <c r="O314" s="4"/>
-      <c r="P314" s="4"/>
-      <c r="Q314" s="4"/>
-      <c r="R314" s="4"/>
-      <c r="S314" s="4"/>
-      <c r="T314" s="4"/>
-      <c r="U314" s="4"/>
-      <c r="V314" s="4"/>
-      <c r="W314" s="4"/>
-      <c r="X314" s="4"/>
-      <c r="Y314" s="4"/>
-      <c r="Z314" s="4"/>
+        <v>-552000.0</v>
+      </c>
+      <c r="I314" s="11"/>
+      <c r="J314" s="11"/>
+      <c r="K314" s="11"/>
+      <c r="L314" s="11"/>
+      <c r="M314" s="11"/>
+      <c r="N314" s="11"/>
+      <c r="O314" s="11"/>
+      <c r="P314" s="11"/>
+      <c r="Q314" s="11"/>
+      <c r="R314" s="11"/>
+      <c r="S314" s="11"/>
+      <c r="T314" s="11"/>
+      <c r="U314" s="11"/>
+      <c r="V314" s="11"/>
+      <c r="W314" s="11"/>
+      <c r="X314" s="11"/>
+      <c r="Y314" s="11"/>
+      <c r="Z314" s="11"/>
     </row>
     <row r="315" ht="14.25" customHeight="1">
       <c r="A315" s="4">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>251</v>
       </c>
       <c r="B315" s="11" t="s">
-        <v>237</v>
+        <v>319</v>
       </c>
       <c r="C315" s="13">
-        <v>45845.0</v>
+        <v>45842.0</v>
       </c>
       <c r="D315" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E315" s="11" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F315" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G315" s="11" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="H315" s="14">
-        <v>-552000.0</v>
-      </c>
-      <c r="I315" s="11"/>
-      <c r="J315" s="11"/>
-      <c r="K315" s="11"/>
-      <c r="L315" s="11"/>
-      <c r="M315" s="11"/>
-      <c r="N315" s="11"/>
-      <c r="O315" s="11"/>
-      <c r="P315" s="11"/>
-      <c r="Q315" s="11"/>
-      <c r="R315" s="11"/>
-      <c r="S315" s="11"/>
-      <c r="T315" s="11"/>
-      <c r="U315" s="11"/>
-      <c r="V315" s="11"/>
-      <c r="W315" s="11"/>
-      <c r="X315" s="11"/>
-      <c r="Y315" s="11"/>
-      <c r="Z315" s="11"/>
+        <v>-286611.57</v>
+      </c>
+      <c r="I315" s="4"/>
+      <c r="J315" s="4"/>
+      <c r="K315" s="4"/>
+      <c r="L315" s="4"/>
+      <c r="M315" s="4"/>
+      <c r="N315" s="4"/>
+      <c r="O315" s="4"/>
+      <c r="P315" s="4"/>
+      <c r="Q315" s="4"/>
+      <c r="R315" s="4"/>
+      <c r="S315" s="4"/>
+      <c r="T315" s="4"/>
+      <c r="U315" s="4"/>
+      <c r="V315" s="4"/>
+      <c r="W315" s="4"/>
+      <c r="X315" s="4"/>
+      <c r="Y315" s="4"/>
+      <c r="Z315" s="4"/>
     </row>
     <row r="316" ht="14.25" customHeight="1">
-      <c r="A316" s="4">
-        <f t="shared" si="1"/>
-        <v>251</v>
-      </c>
-      <c r="B316" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="C316" s="13">
-        <v>45842.0</v>
-      </c>
-      <c r="D316" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="E316" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="F316" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="G316" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="H316" s="14">
-        <v>-286611.57</v>
+      <c r="A316" s="15"/>
+      <c r="B316" s="15"/>
+      <c r="C316" s="16"/>
+      <c r="D316" s="15"/>
+      <c r="E316" s="15"/>
+      <c r="F316" s="15"/>
+      <c r="G316" s="15"/>
+      <c r="H316" s="17">
+        <f>SUM(H2:H315)</f>
+        <v>60273427.85</v>
       </c>
       <c r="I316" s="4"/>
       <c r="J316" s="4"/>
@@ -15974,18 +15955,15 @@
       <c r="Y316" s="4"/>
       <c r="Z316" s="4"/>
     </row>
-    <row r="317" ht="14.25" hidden="1" customHeight="1">
-      <c r="A317" s="15"/>
-      <c r="B317" s="15"/>
-      <c r="C317" s="16"/>
-      <c r="D317" s="15"/>
-      <c r="E317" s="15"/>
-      <c r="F317" s="15"/>
-      <c r="G317" s="15"/>
-      <c r="H317" s="17">
-        <f>SUM(H2:H316)</f>
-        <v>60367496.98</v>
-      </c>
+    <row r="317" ht="14.25" customHeight="1">
+      <c r="A317" s="4"/>
+      <c r="B317" s="4"/>
+      <c r="C317" s="18"/>
+      <c r="D317" s="4"/>
+      <c r="E317" s="4"/>
+      <c r="F317" s="4"/>
+      <c r="G317" s="4"/>
+      <c r="H317" s="4"/>
       <c r="I317" s="4"/>
       <c r="J317" s="4"/>
       <c r="K317" s="4"/>
@@ -16041,7 +16019,10 @@
       <c r="E319" s="4"/>
       <c r="F319" s="4"/>
       <c r="G319" s="4"/>
-      <c r="H319" s="4"/>
+      <c r="H319" s="19">
+        <f>SUBTOTAL(9,H2:H318)</f>
+        <v>120546855.7</v>
+      </c>
       <c r="I319" s="4"/>
       <c r="J319" s="4"/>
       <c r="K319" s="4"/>
@@ -16069,10 +16050,7 @@
       <c r="E320" s="4"/>
       <c r="F320" s="4"/>
       <c r="G320" s="4"/>
-      <c r="H320" s="19">
-        <f>SUBTOTAL(9,H2:H319)</f>
-        <v>60367496.98</v>
-      </c>
+      <c r="H320" s="4"/>
       <c r="I320" s="4"/>
       <c r="J320" s="4"/>
       <c r="K320" s="4"/>
@@ -16100,7 +16078,7 @@
       <c r="E321" s="4"/>
       <c r="F321" s="4"/>
       <c r="G321" s="4"/>
-      <c r="H321" s="4"/>
+      <c r="H321" s="8"/>
       <c r="I321" s="4"/>
       <c r="J321" s="4"/>
       <c r="K321" s="4"/>
@@ -16128,7 +16106,7 @@
       <c r="E322" s="4"/>
       <c r="F322" s="4"/>
       <c r="G322" s="4"/>
-      <c r="H322" s="8"/>
+      <c r="H322" s="4"/>
       <c r="I322" s="4"/>
       <c r="J322" s="4"/>
       <c r="K322" s="4"/>
@@ -16571,12 +16549,12 @@
     <row r="338" ht="14.25" customHeight="1">
       <c r="A338" s="4"/>
       <c r="B338" s="4"/>
-      <c r="C338" s="18"/>
+      <c r="C338" s="5"/>
       <c r="D338" s="4"/>
       <c r="E338" s="4"/>
       <c r="F338" s="4"/>
       <c r="G338" s="4"/>
-      <c r="H338" s="4"/>
+      <c r="H338" s="6"/>
       <c r="I338" s="4"/>
       <c r="J338" s="4"/>
       <c r="K338" s="4"/>
@@ -21667,12 +21645,12 @@
     <row r="520" ht="14.25" customHeight="1">
       <c r="A520" s="4"/>
       <c r="B520" s="4"/>
-      <c r="C520" s="5"/>
+      <c r="C520" s="18"/>
       <c r="D520" s="4"/>
       <c r="E520" s="4"/>
       <c r="F520" s="4"/>
       <c r="G520" s="4"/>
-      <c r="H520" s="6"/>
+      <c r="H520" s="4"/>
       <c r="I520" s="4"/>
       <c r="J520" s="4"/>
       <c r="K520" s="4"/>
@@ -35048,130 +35026,8 @@
       <c r="Y997" s="4"/>
       <c r="Z997" s="4"/>
     </row>
-    <row r="998" ht="14.25" customHeight="1">
-      <c r="A998" s="4"/>
-      <c r="B998" s="4"/>
-      <c r="C998" s="18"/>
-      <c r="D998" s="4"/>
-      <c r="E998" s="4"/>
-      <c r="F998" s="4"/>
-      <c r="G998" s="4"/>
-      <c r="H998" s="4"/>
-      <c r="I998" s="4"/>
-      <c r="J998" s="4"/>
-      <c r="K998" s="4"/>
-      <c r="L998" s="4"/>
-      <c r="M998" s="4"/>
-      <c r="N998" s="4"/>
-      <c r="O998" s="4"/>
-      <c r="P998" s="4"/>
-      <c r="Q998" s="4"/>
-      <c r="R998" s="4"/>
-      <c r="S998" s="4"/>
-      <c r="T998" s="4"/>
-      <c r="U998" s="4"/>
-      <c r="V998" s="4"/>
-      <c r="W998" s="4"/>
-      <c r="X998" s="4"/>
-      <c r="Y998" s="4"/>
-      <c r="Z998" s="4"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$H$317">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Gallo Sendoya, Juan Martin"/>
-        <filter val="Montero, Hugo Hector"/>
-        <filter val="Buldain Gaston"/>
-        <filter val="Portela, Nahuel Ezequiel"/>
-        <filter val="Gonzalez, Gustavo Ariel"/>
-        <filter val="Arrieta, Maria Carolina"/>
-        <filter val="Escobar, Pablo Miguel"/>
-        <filter val="Gavalda, Mauricio Luis"/>
-        <filter val="Montalbano, Maria Camila"/>
-        <filter val="Susseret, Francisco Santiago"/>
-        <filter val="Morales, Juan Pablo"/>
-        <filter val="Anca Ezequiel"/>
-        <filter val="Gonzalez, Jose Luis"/>
-        <filter val="Pacheco Pablo Oscar"/>
-        <filter val="SOSA, HECTOR DAMIAN"/>
-        <filter val="Acuna, Santiago Martin"/>
-        <filter val="Carballo Alejandro"/>
-        <filter val="Mario Facundo Daniel"/>
-        <filter val="Castellanos, Yanina Raquel"/>
-        <filter val="Diaz, Oscar Enrique"/>
-        <filter val="Montenovo Valentino"/>
-        <filter val="Rosana Cepeda"/>
-        <filter val="Merlo Ignacio"/>
-        <filter val="Laoretani, Dalmiro Lautaro"/>
-        <filter val="CASTRO JOAQUIN EZEQUIEL"/>
-        <filter val="Retamozo Martin"/>
-        <filter val="Casas, Luciano Jesus"/>
-        <filter val="Beltran, Maximiliano"/>
-        <filter val="Pellegrotti, Raul Eduardo"/>
-        <filter val="Leunda Gabriel"/>
-        <filter val="DEL PINO MARIA SOLEDAD"/>
-        <filter val="Zola, Francisco"/>
-        <filter val="Maidana Ariana"/>
-        <filter val="Macchione, Guadalupe"/>
-        <filter val="Canepa Fernando"/>
-        <filter val="Schmidt, Aldo Walter"/>
-        <filter val="Ponce Julieta"/>
-        <filter val="Veliz, Kevin Sebastian"/>
-        <filter val="Nieto, Fabricio Ezequiel"/>
-        <filter val="Atia, Sebastian"/>
-        <filter val="Leguizamon Marcela"/>
-        <filter val="Cuadrado, Mariela Ines"/>
-        <filter val="Raimondi, Melina"/>
-        <filter val="Ercoreca Cristian"/>
-        <filter val="Bai, Sebastian"/>
-        <filter val="Giussi, Emanuel"/>
-        <filter val="GRENILLON RAUL ALBERTO"/>
-        <filter val="Pagani, Maria Laura"/>
-        <filter val="Toledo, Ignacio Martin"/>
-        <filter val="Callegaro, Diego Hernan"/>
-        <filter val="Campione, Ruth Elizabeth"/>
-        <filter val="Rodriguez, Rodrigo Emanuel"/>
-        <filter val="Toledo, Franco Martín"/>
-        <filter val="Agustina Thurler-Terceros-"/>
-        <filter val="Quiroga, Juan Diego"/>
-        <filter val="Merlo, Felix Angel"/>
-        <filter val="Medina, Jonatan Eduardo"/>
-        <filter val="Hinaypil, Jos Alberto"/>
-        <filter val="Quiroga, Franco Matias"/>
-        <filter val="Morales Fernando"/>
-        <filter val="Burela, Juan Ignacio"/>
-        <filter val="Laxagueborde, Enzo"/>
-        <filter val="Moglie Cabistañ Rafael"/>
-        <filter val="Jaime Gavalda -Terceros-"/>
-        <filter val="Cingolani, Alejandro Enrique"/>
-        <filter val="Segovia, Mario Andres"/>
-        <filter val="Maruff, Joana Alejandra"/>
-        <filter val="Dillon, Jose Maria"/>
-        <filter val="De Rosso, Humberto"/>
-        <filter val="Vazquez, Sebastian Ignacio"/>
-        <filter val="Diaz, Federico"/>
-        <filter val="Varios Terceros Otros"/>
-        <filter val="Cañas, Pablo Damian"/>
-        <filter val="Seijo, Hector Ivan"/>
-        <filter val="Galesio Francelina"/>
-        <filter val="Acuña, Mauro Hernan"/>
-        <filter val="Vanerio, Juan Pablo"/>
-        <filter val="Ongaro, Gustavo"/>
-        <filter val="Rodriguez, Franco Emmanuel"/>
-        <filter val="Barrere, Francisco"/>
-        <filter val="Cufre, Ignacio Nicolas"/>
-        <filter val="Grigera Juan-Terceros-"/>
-        <filter val="Di Vito Martin Alejandro"/>
-        <filter val="Gonzalez, Florencia Beatriz"/>
-        <filter val="Lopez, Juan Franco"/>
-        <filter val="Zega Maximiliano"/>
-        <filter val="San Agustin Terceros Otros"/>
-        <filter val="Canepa Santiago"/>
-        <filter val="Costa, Diego Daniel"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="$A$1:$H$316"/>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Actualización automática - 2025-08-19 11:21
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -15,7 +15,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="LxQuHNMPfVL1uq4s2yU6eXwz2ZXCqdZJhqiXYw89lUw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="4N0jev/vZuFcStxvpxKwkHPzMoxDjWZ+PsBzRPxMPIQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -53,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00;\(\$#,##0.00\);\$#,##0.00"/>
   </numFmts>
   <fonts count="6">

</xml_diff>

<commit_message>
Actualización automática - 2025-09-03 09:19
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -11,12 +11,12 @@
   </externalReferences>
   <definedNames>
     <definedName name="MP">'[1]MATERIA PRIMA'!$B$3:$B$135</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Descuentos para BOT '!$A$1:$H$316</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Descuentos para BOT '!$A$1:$H$367</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="hrRfP02Wa+NWbyH7jrMEVkukARwpzMndtrBANLrea7s="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="FMItia8QaPA4wxt1Nq4xwkAmwOX/0U66SRc2J2cXODQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -358,6 +358,9 @@
     <t>Gonzalez, Gustavo Ariel</t>
   </si>
   <si>
+    <t>Gonzalez, Jose Luis</t>
+  </si>
+  <si>
     <t>FGAS 6 20734</t>
   </si>
   <si>
@@ -431,9 +434,6 @@
   </si>
   <si>
     <t>Montalbano, Maria Camila</t>
-  </si>
-  <si>
-    <t>Gonzalez, Jose Luis</t>
   </si>
   <si>
     <t>LOS CINCO LEGUITOS S.R.L.</t>
@@ -1790,7 +1790,7 @@
     <col customWidth="1" min="1" max="1" width="19.71"/>
     <col customWidth="1" min="2" max="2" width="28.86"/>
     <col customWidth="1" min="3" max="3" width="13.43"/>
-    <col customWidth="1" min="4" max="4" width="38.86"/>
+    <col customWidth="1" min="4" max="4" width="45.71"/>
     <col customWidth="1" min="5" max="5" width="17.43"/>
     <col customWidth="1" min="6" max="6" width="17.0"/>
     <col customWidth="1" min="7" max="7" width="45.86"/>
@@ -3779,10 +3779,10 @@
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C45" s="6">
         <v>45853.0</v>
@@ -3791,13 +3791,13 @@
         <v>23</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H45" s="7">
         <v>77657.7</v>
@@ -3917,22 +3917,22 @@
         <v>11</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C48" s="6">
         <v>45870.0</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H48" s="7">
         <v>-45380.83</v>
@@ -3962,22 +3962,22 @@
         <v>11</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C49" s="6">
         <v>45870.0</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H49" s="7">
         <v>-5902.44</v>
@@ -4007,22 +4007,22 @@
         <v>11</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C50" s="6">
         <v>45870.0</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H50" s="7">
         <v>-10066.11</v>
@@ -4052,22 +4052,22 @@
         <v>11</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C51" s="6">
         <v>45870.0</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H51" s="7">
         <v>-77636.28</v>
@@ -4097,22 +4097,22 @@
         <v>11</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C52" s="6">
         <v>45870.0</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H52" s="7">
         <v>-5422.58</v>
@@ -4142,22 +4142,22 @@
         <v>11</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C53" s="6">
         <v>45870.0</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H53" s="7">
         <v>-9717.79</v>
@@ -4187,22 +4187,22 @@
         <v>11</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C54" s="6">
         <v>45870.0</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H54" s="7">
         <v>-4588.99</v>
@@ -4232,22 +4232,22 @@
         <v>11</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C55" s="6">
         <v>45870.0</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H55" s="7">
         <v>-1880.81</v>
@@ -4277,22 +4277,22 @@
         <v>11</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" s="6">
         <v>45871.0</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H56" s="7">
         <v>-76191.17</v>
@@ -4322,22 +4322,22 @@
         <v>11</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C57" s="6">
         <v>45871.0</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H57" s="7">
         <v>-18935.63</v>
@@ -4367,22 +4367,22 @@
         <v>11</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="6">
         <v>45883.0</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H58" s="7">
         <v>452785.0</v>
@@ -4412,22 +4412,22 @@
         <v>11</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C59" s="6">
         <v>45894.0</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H59" s="7">
         <v>1644380.8</v>
@@ -4457,7 +4457,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C60" s="6">
         <v>45839.0</v>
@@ -4502,7 +4502,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C61" s="6">
         <v>45839.0</v>
@@ -4547,7 +4547,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C62" s="6">
         <v>45867.0</v>
@@ -4592,7 +4592,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C63" s="6">
         <v>45868.0</v>
@@ -4637,7 +4637,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C64" s="6">
         <v>45869.0</v>
@@ -4682,7 +4682,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C65" s="6">
         <v>45869.0</v>
@@ -4727,7 +4727,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C66" s="6">
         <v>45869.0</v>
@@ -4772,7 +4772,7 @@
         <v>15</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C67" s="6">
         <v>45866.0</v>
@@ -4817,7 +4817,7 @@
         <v>15</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C68" s="6">
         <v>45866.0</v>
@@ -4862,7 +4862,7 @@
         <v>15</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C69" s="6">
         <v>45867.0</v>
@@ -4907,7 +4907,7 @@
         <v>15</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C70" s="6">
         <v>45869.0</v>
@@ -4952,7 +4952,7 @@
         <v>15</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C71" s="6">
         <v>45869.0</v>
@@ -6803,7 +6803,7 @@
         <v>45869.0</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>182</v>
@@ -7073,7 +7073,7 @@
         <v>45875.0</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>196</v>
@@ -7118,7 +7118,7 @@
         <v>45876.0</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>198</v>
@@ -8738,7 +8738,7 @@
         <v>45854.0</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>245</v>
@@ -9323,7 +9323,7 @@
         <v>45853.0</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>254</v>
@@ -12788,7 +12788,7 @@
         <v>45866.0</v>
       </c>
       <c r="D245" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E245" s="5" t="s">
         <v>314</v>
@@ -15668,7 +15668,7 @@
         <v>45870.0</v>
       </c>
       <c r="D309" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E309" s="5" t="s">
         <v>364</v>
@@ -15713,7 +15713,7 @@
         <v>45870.0</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E310" s="5" t="s">
         <v>364</v>
@@ -15758,7 +15758,7 @@
         <v>45871.0</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E311" s="5" t="s">
         <v>367</v>
@@ -15848,7 +15848,7 @@
         <v>45882.0</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E313" s="5" t="s">
         <v>371</v>
@@ -16523,7 +16523,7 @@
         <v>45839.0</v>
       </c>
       <c r="D328" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E328" s="5" t="s">
         <v>386</v>
@@ -16568,7 +16568,7 @@
         <v>45859.0</v>
       </c>
       <c r="D329" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E329" s="5" t="s">
         <v>388</v>
@@ -16613,7 +16613,7 @@
         <v>45866.0</v>
       </c>
       <c r="D330" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E330" s="5" t="s">
         <v>390</v>
@@ -16793,7 +16793,7 @@
         <v>45869.0</v>
       </c>
       <c r="D334" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E334" s="5" t="s">
         <v>393</v>
@@ -16838,7 +16838,7 @@
         <v>45871.0</v>
       </c>
       <c r="D335" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E335" s="5" t="s">
         <v>395</v>
@@ -17333,7 +17333,7 @@
         <v>45866.0</v>
       </c>
       <c r="D346" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E346" s="5" t="s">
         <v>419</v>
@@ -17378,7 +17378,7 @@
         <v>45870.0</v>
       </c>
       <c r="D347" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E347" s="5" t="s">
         <v>420</v>
@@ -17423,7 +17423,7 @@
         <v>45870.0</v>
       </c>
       <c r="D348" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E348" s="5" t="s">
         <v>422</v>
@@ -17468,7 +17468,7 @@
         <v>45870.0</v>
       </c>
       <c r="D349" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E349" s="5" t="s">
         <v>420</v>
@@ -17558,7 +17558,7 @@
         <v>45841.0</v>
       </c>
       <c r="D351" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E351" s="5" t="s">
         <v>428</v>
@@ -17603,7 +17603,7 @@
         <v>45845.0</v>
       </c>
       <c r="D352" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>430</v>
@@ -35952,7 +35952,7 @@
       <c r="Z997" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$H$316"/>
+  <autoFilter ref="$A$1:$H$367"/>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Actualización automática - 2025-09-30 11:42
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -15,7 +15,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="CS39eg1aGIJl2Y9NwGw672yM15u/j09bTaZSkeIExc0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="sIUkzM0vTbJAYz8CfCxAHdTDP4vibVzMyLeIAqRgrNs="/>
     </ext>
   </extLst>
 </workbook>
@@ -1559,7 +1559,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" ht="14.25" hidden="1" customHeight="1">
       <c r="A2" s="5">
         <f t="shared" ref="A2:A288" si="1">VLOOKUP(B2,'Empleados c nro legajo'!B:F,2,FALSE)</f>
         <v>1</v>
@@ -1596,7 +1596,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" ht="14.25" hidden="1" customHeight="1">
       <c r="A3" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1633,7 +1633,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" ht="14.25" hidden="1" customHeight="1">
       <c r="A4" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1670,7 +1670,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" ht="14.25" hidden="1" customHeight="1">
       <c r="A5" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1707,7 +1707,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" ht="14.25" hidden="1" customHeight="1">
       <c r="A6" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1744,7 +1744,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" ht="14.25" hidden="1" customHeight="1">
       <c r="A7" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1781,7 +1781,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" ht="14.25" hidden="1" customHeight="1">
       <c r="A8" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1818,7 +1818,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" ht="14.25" hidden="1" customHeight="1">
       <c r="A9" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1855,7 +1855,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" ht="14.25" hidden="1" customHeight="1">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1892,7 +1892,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" ht="14.25" hidden="1" customHeight="1">
       <c r="A11" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1929,7 +1929,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" ht="14.25" hidden="1" customHeight="1">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1966,7 +1966,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" ht="14.25" hidden="1" customHeight="1">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2003,7 +2003,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" ht="14.25" hidden="1" customHeight="1">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2040,7 +2040,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" ht="14.25" hidden="1" customHeight="1">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2077,7 +2077,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" ht="14.25" hidden="1" customHeight="1">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2114,7 +2114,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" ht="14.25" hidden="1" customHeight="1">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2151,7 +2151,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" ht="14.25" hidden="1" customHeight="1">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2188,7 +2188,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" ht="14.25" hidden="1" customHeight="1">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2225,7 +2225,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" ht="14.25" hidden="1" customHeight="1">
       <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2262,7 +2262,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" ht="14.25" hidden="1" customHeight="1">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2299,7 +2299,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" ht="14.25" hidden="1" customHeight="1">
       <c r="A22" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2336,7 +2336,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" ht="14.25" hidden="1" customHeight="1">
       <c r="A23" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2373,7 +2373,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" ht="14.25" hidden="1" customHeight="1">
       <c r="A24" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2410,7 +2410,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" ht="14.25" hidden="1" customHeight="1">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2447,7 +2447,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" ht="14.25" hidden="1" customHeight="1">
       <c r="A26" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2484,7 +2484,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" ht="14.25" hidden="1" customHeight="1">
       <c r="A27" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2521,7 +2521,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" ht="14.25" hidden="1" customHeight="1">
       <c r="A28" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2558,7 +2558,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" ht="14.25" hidden="1" customHeight="1">
       <c r="A29" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2593,7 +2593,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" ht="14.25" hidden="1" customHeight="1">
       <c r="A30" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2630,7 +2630,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" ht="14.25" hidden="1" customHeight="1">
       <c r="A31" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2667,7 +2667,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" ht="14.25" hidden="1" customHeight="1">
       <c r="A32" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2704,7 +2704,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" ht="14.25" hidden="1" customHeight="1">
       <c r="A33" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2741,7 +2741,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" ht="14.25" hidden="1" customHeight="1">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2778,7 +2778,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" ht="14.25" hidden="1" customHeight="1">
       <c r="A35" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2815,7 +2815,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" ht="14.25" hidden="1" customHeight="1">
       <c r="A36" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2852,7 +2852,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" ht="14.25" hidden="1" customHeight="1">
       <c r="A37" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2889,7 +2889,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" ht="14.25" hidden="1" customHeight="1">
       <c r="A38" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2926,7 +2926,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" ht="14.25" hidden="1" customHeight="1">
       <c r="A39" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2963,7 +2963,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" ht="14.25" hidden="1" customHeight="1">
       <c r="A40" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3000,7 +3000,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" ht="14.25" hidden="1" customHeight="1">
       <c r="A41" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3037,7 +3037,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" ht="14.25" hidden="1" customHeight="1">
       <c r="A42" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3074,7 +3074,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" ht="14.25" hidden="1" customHeight="1">
       <c r="A43" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3111,7 +3111,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
+    <row r="44" ht="14.25" hidden="1" customHeight="1">
       <c r="A44" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3148,7 +3148,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" ht="14.25" customHeight="1">
+    <row r="45" ht="14.25" hidden="1" customHeight="1">
       <c r="A45" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3185,7 +3185,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" ht="14.25" customHeight="1">
+    <row r="46" ht="14.25" hidden="1" customHeight="1">
       <c r="A46" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3222,7 +3222,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
+    <row r="47" ht="14.25" hidden="1" customHeight="1">
       <c r="A47" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3259,7 +3259,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
+    <row r="48" ht="14.25" hidden="1" customHeight="1">
       <c r="A48" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3296,7 +3296,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
+    <row r="49" ht="14.25" hidden="1" customHeight="1">
       <c r="A49" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3333,7 +3333,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
+    <row r="50" ht="14.25" hidden="1" customHeight="1">
       <c r="A50" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3370,7 +3370,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" ht="14.25" hidden="1" customHeight="1">
       <c r="A51" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3407,7 +3407,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" ht="14.25" customHeight="1">
+    <row r="52" ht="14.25" hidden="1" customHeight="1">
       <c r="A52" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3444,7 +3444,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
+    <row r="53" ht="14.25" hidden="1" customHeight="1">
       <c r="A53" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3481,7 +3481,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
+    <row r="54" ht="14.25" hidden="1" customHeight="1">
       <c r="A54" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3518,7 +3518,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
+    <row r="55" ht="14.25" hidden="1" customHeight="1">
       <c r="A55" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3555,7 +3555,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
+    <row r="56" ht="14.25" hidden="1" customHeight="1">
       <c r="A56" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3592,7 +3592,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
+    <row r="57" ht="14.25" hidden="1" customHeight="1">
       <c r="A57" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3629,7 +3629,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
+    <row r="58" ht="14.25" hidden="1" customHeight="1">
       <c r="A58" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3666,7 +3666,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" ht="14.25" customHeight="1">
+    <row r="59" ht="14.25" hidden="1" customHeight="1">
       <c r="A59" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3703,7 +3703,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" ht="14.25" customHeight="1">
+    <row r="60" ht="14.25" hidden="1" customHeight="1">
       <c r="A60" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3740,7 +3740,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" ht="14.25" customHeight="1">
+    <row r="61" ht="14.25" hidden="1" customHeight="1">
       <c r="A61" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3777,7 +3777,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" ht="14.25" customHeight="1">
+    <row r="62" ht="14.25" hidden="1" customHeight="1">
       <c r="A62" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3814,7 +3814,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
+    <row r="63" ht="14.25" hidden="1" customHeight="1">
       <c r="A63" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3851,7 +3851,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
+    <row r="64" ht="14.25" hidden="1" customHeight="1">
       <c r="A64" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3888,7 +3888,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
+    <row r="65" ht="14.25" hidden="1" customHeight="1">
       <c r="A65" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3925,7 +3925,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" ht="14.25" hidden="1" customHeight="1">
       <c r="A66" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3962,7 +3962,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
+    <row r="67" ht="14.25" hidden="1" customHeight="1">
       <c r="A67" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3999,7 +3999,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" ht="14.25" hidden="1" customHeight="1">
       <c r="A68" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4036,7 +4036,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
+    <row r="69" ht="14.25" hidden="1" customHeight="1">
       <c r="A69" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4073,7 +4073,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" ht="14.25" hidden="1" customHeight="1">
       <c r="A70" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4110,7 +4110,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
+    <row r="71" ht="14.25" hidden="1" customHeight="1">
       <c r="A71" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4147,7 +4147,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" ht="14.25" hidden="1" customHeight="1">
       <c r="A72" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4184,7 +4184,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
+    <row r="73" ht="14.25" hidden="1" customHeight="1">
       <c r="A73" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4221,7 +4221,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" ht="14.25" customHeight="1">
+    <row r="74" ht="14.25" hidden="1" customHeight="1">
       <c r="A74" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4258,7 +4258,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" ht="14.25" customHeight="1">
+    <row r="75" ht="14.25" hidden="1" customHeight="1">
       <c r="A75" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4295,7 +4295,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" ht="14.25" customHeight="1">
+    <row r="76" ht="14.25" hidden="1" customHeight="1">
       <c r="A76" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4332,7 +4332,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" ht="14.25" customHeight="1">
+    <row r="77" ht="14.25" hidden="1" customHeight="1">
       <c r="A77" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4369,7 +4369,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
+    <row r="78" ht="14.25" hidden="1" customHeight="1">
       <c r="A78" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4406,7 +4406,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" ht="14.25" customHeight="1">
+    <row r="79" ht="14.25" hidden="1" customHeight="1">
       <c r="A79" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4443,7 +4443,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
+    <row r="80" ht="14.25" hidden="1" customHeight="1">
       <c r="A80" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4480,7 +4480,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
+    <row r="81" ht="14.25" hidden="1" customHeight="1">
       <c r="A81" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4517,7 +4517,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
+    <row r="82" ht="14.25" hidden="1" customHeight="1">
       <c r="A82" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4552,7 +4552,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" ht="14.25" hidden="1" customHeight="1">
       <c r="A83" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4589,7 +4589,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
+    <row r="84" ht="14.25" hidden="1" customHeight="1">
       <c r="A84" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4626,7 +4626,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" ht="14.25" customHeight="1">
+    <row r="85" ht="14.25" hidden="1" customHeight="1">
       <c r="A85" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4663,7 +4663,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" ht="14.25" customHeight="1">
+    <row r="86" ht="14.25" hidden="1" customHeight="1">
       <c r="A86" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4700,7 +4700,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" ht="14.25" customHeight="1">
+    <row r="87" ht="14.25" hidden="1" customHeight="1">
       <c r="A87" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4737,7 +4737,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" ht="14.25" customHeight="1">
+    <row r="88" ht="14.25" hidden="1" customHeight="1">
       <c r="A88" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4774,7 +4774,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" ht="14.25" customHeight="1">
+    <row r="89" ht="14.25" hidden="1" customHeight="1">
       <c r="A89" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4811,7 +4811,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" ht="14.25" customHeight="1">
+    <row r="90" ht="14.25" hidden="1" customHeight="1">
       <c r="A90" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4848,7 +4848,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" ht="14.25" customHeight="1">
+    <row r="91" ht="14.25" hidden="1" customHeight="1">
       <c r="A91" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4885,7 +4885,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" ht="14.25" customHeight="1">
+    <row r="92" ht="14.25" hidden="1" customHeight="1">
       <c r="A92" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4922,7 +4922,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" ht="14.25" customHeight="1">
+    <row r="93" ht="14.25" hidden="1" customHeight="1">
       <c r="A93" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4959,7 +4959,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" ht="14.25" customHeight="1">
+    <row r="94" ht="14.25" hidden="1" customHeight="1">
       <c r="A94" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4996,7 +4996,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" ht="14.25" customHeight="1">
+    <row r="95" ht="14.25" hidden="1" customHeight="1">
       <c r="A95" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -5033,7 +5033,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" ht="14.25" customHeight="1">
+    <row r="96" ht="14.25" hidden="1" customHeight="1">
       <c r="A96" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -5070,7 +5070,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" ht="14.25" customHeight="1">
+    <row r="97" ht="14.25" hidden="1" customHeight="1">
       <c r="A97" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -5107,7 +5107,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" ht="14.25" customHeight="1">
+    <row r="98" ht="14.25" hidden="1" customHeight="1">
       <c r="A98" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -5144,7 +5144,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" ht="14.25" customHeight="1">
+    <row r="99" ht="14.25" hidden="1" customHeight="1">
       <c r="A99" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -5181,7 +5181,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" ht="14.25" customHeight="1">
+    <row r="100" ht="14.25" hidden="1" customHeight="1">
       <c r="A100" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -5218,7 +5218,7 @@
       <c r="Q100" s="4"/>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" ht="14.25" customHeight="1">
+    <row r="101" ht="14.25" hidden="1" customHeight="1">
       <c r="A101" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -5255,7 +5255,7 @@
       <c r="Q101" s="4"/>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" ht="14.25" customHeight="1">
+    <row r="102" ht="14.25" hidden="1" customHeight="1">
       <c r="A102" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -5292,7 +5292,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" ht="14.25" customHeight="1">
+    <row r="103" ht="14.25" hidden="1" customHeight="1">
       <c r="A103" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5329,7 +5329,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" ht="14.25" customHeight="1">
+    <row r="104" ht="14.25" hidden="1" customHeight="1">
       <c r="A104" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5366,7 +5366,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" ht="14.25" customHeight="1">
+    <row r="105" ht="14.25" hidden="1" customHeight="1">
       <c r="A105" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5403,7 +5403,7 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" ht="14.25" customHeight="1">
+    <row r="106" ht="14.25" hidden="1" customHeight="1">
       <c r="A106" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5440,7 +5440,7 @@
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" ht="14.25" customHeight="1">
+    <row r="107" ht="14.25" hidden="1" customHeight="1">
       <c r="A107" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5477,7 +5477,7 @@
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" ht="14.25" customHeight="1">
+    <row r="108" ht="14.25" hidden="1" customHeight="1">
       <c r="A108" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5514,7 +5514,7 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" ht="14.25" customHeight="1">
+    <row r="109" ht="14.25" hidden="1" customHeight="1">
       <c r="A109" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -5551,7 +5551,7 @@
       <c r="Q109" s="4"/>
       <c r="R109" s="4"/>
     </row>
-    <row r="110" ht="14.25" customHeight="1">
+    <row r="110" ht="14.25" hidden="1" customHeight="1">
       <c r="A110" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -5588,7 +5588,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" ht="14.25" customHeight="1">
+    <row r="111" ht="14.25" hidden="1" customHeight="1">
       <c r="A111" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -5625,7 +5625,7 @@
       <c r="Q111" s="4"/>
       <c r="R111" s="4"/>
     </row>
-    <row r="112" ht="14.25" customHeight="1">
+    <row r="112" ht="14.25" hidden="1" customHeight="1">
       <c r="A112" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5662,7 +5662,7 @@
       <c r="Q112" s="4"/>
       <c r="R112" s="4"/>
     </row>
-    <row r="113" ht="14.25" customHeight="1">
+    <row r="113" ht="14.25" hidden="1" customHeight="1">
       <c r="A113" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5699,7 +5699,7 @@
       <c r="Q113" s="4"/>
       <c r="R113" s="4"/>
     </row>
-    <row r="114" ht="14.25" customHeight="1">
+    <row r="114" ht="14.25" hidden="1" customHeight="1">
       <c r="A114" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5736,7 +5736,7 @@
       <c r="Q114" s="4"/>
       <c r="R114" s="4"/>
     </row>
-    <row r="115" ht="14.25" customHeight="1">
+    <row r="115" ht="14.25" hidden="1" customHeight="1">
       <c r="A115" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5773,7 +5773,7 @@
       <c r="Q115" s="4"/>
       <c r="R115" s="4"/>
     </row>
-    <row r="116" ht="14.25" customHeight="1">
+    <row r="116" ht="14.25" hidden="1" customHeight="1">
       <c r="A116" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5810,7 +5810,7 @@
       <c r="Q116" s="4"/>
       <c r="R116" s="4"/>
     </row>
-    <row r="117" ht="14.25" customHeight="1">
+    <row r="117" ht="14.25" hidden="1" customHeight="1">
       <c r="A117" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5847,7 +5847,7 @@
       <c r="Q117" s="4"/>
       <c r="R117" s="4"/>
     </row>
-    <row r="118" ht="14.25" customHeight="1">
+    <row r="118" ht="14.25" hidden="1" customHeight="1">
       <c r="A118" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -5884,7 +5884,7 @@
       <c r="Q118" s="4"/>
       <c r="R118" s="4"/>
     </row>
-    <row r="119" ht="14.25" customHeight="1">
+    <row r="119" ht="14.25" hidden="1" customHeight="1">
       <c r="A119" s="5">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -5921,7 +5921,7 @@
       <c r="Q119" s="4"/>
       <c r="R119" s="4"/>
     </row>
-    <row r="120" ht="14.25" customHeight="1">
+    <row r="120" ht="14.25" hidden="1" customHeight="1">
       <c r="A120" s="5">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -5958,7 +5958,7 @@
       <c r="Q120" s="4"/>
       <c r="R120" s="4"/>
     </row>
-    <row r="121" ht="14.25" customHeight="1">
+    <row r="121" ht="14.25" hidden="1" customHeight="1">
       <c r="A121" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -5995,7 +5995,7 @@
       <c r="Q121" s="4"/>
       <c r="R121" s="4"/>
     </row>
-    <row r="122" ht="14.25" customHeight="1">
+    <row r="122" ht="14.25" hidden="1" customHeight="1">
       <c r="A122" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -6032,7 +6032,7 @@
       <c r="Q122" s="4"/>
       <c r="R122" s="4"/>
     </row>
-    <row r="123" ht="14.25" customHeight="1">
+    <row r="123" ht="14.25" hidden="1" customHeight="1">
       <c r="A123" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -6069,7 +6069,7 @@
       <c r="Q123" s="4"/>
       <c r="R123" s="4"/>
     </row>
-    <row r="124" ht="14.25" customHeight="1">
+    <row r="124" ht="14.25" hidden="1" customHeight="1">
       <c r="A124" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -6106,7 +6106,7 @@
       <c r="Q124" s="4"/>
       <c r="R124" s="4"/>
     </row>
-    <row r="125" ht="14.25" customHeight="1">
+    <row r="125" ht="14.25" hidden="1" customHeight="1">
       <c r="A125" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -6143,7 +6143,7 @@
       <c r="Q125" s="4"/>
       <c r="R125" s="4"/>
     </row>
-    <row r="126" ht="14.25" customHeight="1">
+    <row r="126" ht="14.25" hidden="1" customHeight="1">
       <c r="A126" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -6180,7 +6180,7 @@
       <c r="Q126" s="4"/>
       <c r="R126" s="4"/>
     </row>
-    <row r="127" ht="14.25" customHeight="1">
+    <row r="127" ht="14.25" hidden="1" customHeight="1">
       <c r="A127" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -6217,7 +6217,7 @@
       <c r="Q127" s="4"/>
       <c r="R127" s="4"/>
     </row>
-    <row r="128" ht="14.25" customHeight="1">
+    <row r="128" ht="14.25" hidden="1" customHeight="1">
       <c r="A128" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -6254,7 +6254,7 @@
       <c r="Q128" s="4"/>
       <c r="R128" s="4"/>
     </row>
-    <row r="129" ht="14.25" customHeight="1">
+    <row r="129" ht="14.25" hidden="1" customHeight="1">
       <c r="A129" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -6291,7 +6291,7 @@
       <c r="Q129" s="4"/>
       <c r="R129" s="4"/>
     </row>
-    <row r="130" ht="14.25" customHeight="1">
+    <row r="130" ht="14.25" hidden="1" customHeight="1">
       <c r="A130" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -6328,7 +6328,7 @@
       <c r="Q130" s="4"/>
       <c r="R130" s="4"/>
     </row>
-    <row r="131" ht="14.25" customHeight="1">
+    <row r="131" ht="14.25" hidden="1" customHeight="1">
       <c r="A131" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -6365,7 +6365,7 @@
       <c r="Q131" s="4"/>
       <c r="R131" s="4"/>
     </row>
-    <row r="132" ht="14.25" customHeight="1">
+    <row r="132" ht="14.25" hidden="1" customHeight="1">
       <c r="A132" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6402,7 +6402,7 @@
       <c r="Q132" s="4"/>
       <c r="R132" s="4"/>
     </row>
-    <row r="133" ht="14.25" customHeight="1">
+    <row r="133" ht="14.25" hidden="1" customHeight="1">
       <c r="A133" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6439,7 +6439,7 @@
       <c r="Q133" s="4"/>
       <c r="R133" s="4"/>
     </row>
-    <row r="134" ht="14.25" customHeight="1">
+    <row r="134" ht="14.25" hidden="1" customHeight="1">
       <c r="A134" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6476,7 +6476,7 @@
       <c r="Q134" s="4"/>
       <c r="R134" s="4"/>
     </row>
-    <row r="135" ht="14.25" customHeight="1">
+    <row r="135" ht="14.25" hidden="1" customHeight="1">
       <c r="A135" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6513,7 +6513,7 @@
       <c r="Q135" s="4"/>
       <c r="R135" s="4"/>
     </row>
-    <row r="136" ht="14.25" customHeight="1">
+    <row r="136" ht="14.25" hidden="1" customHeight="1">
       <c r="A136" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6550,7 +6550,7 @@
       <c r="Q136" s="4"/>
       <c r="R136" s="4"/>
     </row>
-    <row r="137" ht="14.25" customHeight="1">
+    <row r="137" ht="14.25" hidden="1" customHeight="1">
       <c r="A137" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6587,7 +6587,7 @@
       <c r="Q137" s="4"/>
       <c r="R137" s="4"/>
     </row>
-    <row r="138" ht="14.25" customHeight="1">
+    <row r="138" ht="14.25" hidden="1" customHeight="1">
       <c r="A138" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6624,7 +6624,7 @@
       <c r="Q138" s="4"/>
       <c r="R138" s="4"/>
     </row>
-    <row r="139" ht="14.25" customHeight="1">
+    <row r="139" ht="14.25" hidden="1" customHeight="1">
       <c r="A139" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6661,7 +6661,7 @@
       <c r="Q139" s="4"/>
       <c r="R139" s="4"/>
     </row>
-    <row r="140" ht="14.25" customHeight="1">
+    <row r="140" ht="14.25" hidden="1" customHeight="1">
       <c r="A140" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6698,7 +6698,7 @@
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
     </row>
-    <row r="141" ht="14.25" customHeight="1">
+    <row r="141" ht="14.25" hidden="1" customHeight="1">
       <c r="A141" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6735,7 +6735,7 @@
       <c r="Q141" s="4"/>
       <c r="R141" s="4"/>
     </row>
-    <row r="142" ht="14.25" customHeight="1">
+    <row r="142" ht="14.25" hidden="1" customHeight="1">
       <c r="A142" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6772,7 +6772,7 @@
       <c r="Q142" s="4"/>
       <c r="R142" s="4"/>
     </row>
-    <row r="143" ht="14.25" customHeight="1">
+    <row r="143" ht="14.25" hidden="1" customHeight="1">
       <c r="A143" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6809,7 +6809,7 @@
       <c r="Q143" s="4"/>
       <c r="R143" s="4"/>
     </row>
-    <row r="144" ht="14.25" customHeight="1">
+    <row r="144" ht="14.25" hidden="1" customHeight="1">
       <c r="A144" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6846,7 +6846,7 @@
       <c r="Q144" s="4"/>
       <c r="R144" s="4"/>
     </row>
-    <row r="145" ht="14.25" customHeight="1">
+    <row r="145" ht="14.25" hidden="1" customHeight="1">
       <c r="A145" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -6883,7 +6883,7 @@
       <c r="Q145" s="4"/>
       <c r="R145" s="4"/>
     </row>
-    <row r="146" ht="14.25" customHeight="1">
+    <row r="146" ht="14.25" hidden="1" customHeight="1">
       <c r="A146" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6920,7 +6920,7 @@
       <c r="Q146" s="4"/>
       <c r="R146" s="4"/>
     </row>
-    <row r="147" ht="14.25" customHeight="1">
+    <row r="147" ht="14.25" hidden="1" customHeight="1">
       <c r="A147" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6957,7 +6957,7 @@
       <c r="Q147" s="4"/>
       <c r="R147" s="4"/>
     </row>
-    <row r="148" ht="14.25" customHeight="1">
+    <row r="148" ht="14.25" hidden="1" customHeight="1">
       <c r="A148" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6994,7 +6994,7 @@
       <c r="Q148" s="4"/>
       <c r="R148" s="4"/>
     </row>
-    <row r="149" ht="14.25" customHeight="1">
+    <row r="149" ht="14.25" hidden="1" customHeight="1">
       <c r="A149" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7031,7 +7031,7 @@
       <c r="Q149" s="4"/>
       <c r="R149" s="4"/>
     </row>
-    <row r="150" ht="14.25" customHeight="1">
+    <row r="150" ht="14.25" hidden="1" customHeight="1">
       <c r="A150" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7068,7 +7068,7 @@
       <c r="Q150" s="4"/>
       <c r="R150" s="4"/>
     </row>
-    <row r="151" ht="14.25" customHeight="1">
+    <row r="151" ht="14.25" hidden="1" customHeight="1">
       <c r="A151" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7105,7 +7105,7 @@
       <c r="Q151" s="4"/>
       <c r="R151" s="4"/>
     </row>
-    <row r="152" ht="14.25" customHeight="1">
+    <row r="152" ht="14.25" hidden="1" customHeight="1">
       <c r="A152" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7142,7 +7142,7 @@
       <c r="Q152" s="4"/>
       <c r="R152" s="4"/>
     </row>
-    <row r="153" ht="14.25" customHeight="1">
+    <row r="153" ht="14.25" hidden="1" customHeight="1">
       <c r="A153" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7179,7 +7179,7 @@
       <c r="Q153" s="4"/>
       <c r="R153" s="4"/>
     </row>
-    <row r="154" ht="14.25" customHeight="1">
+    <row r="154" ht="14.25" hidden="1" customHeight="1">
       <c r="A154" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7216,7 +7216,7 @@
       <c r="Q154" s="4"/>
       <c r="R154" s="4"/>
     </row>
-    <row r="155" ht="14.25" customHeight="1">
+    <row r="155" ht="14.25" hidden="1" customHeight="1">
       <c r="A155" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7253,7 +7253,7 @@
       <c r="Q155" s="4"/>
       <c r="R155" s="4"/>
     </row>
-    <row r="156" ht="14.25" customHeight="1">
+    <row r="156" ht="14.25" hidden="1" customHeight="1">
       <c r="A156" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7290,7 +7290,7 @@
       <c r="Q156" s="4"/>
       <c r="R156" s="4"/>
     </row>
-    <row r="157" ht="14.25" customHeight="1">
+    <row r="157" ht="14.25" hidden="1" customHeight="1">
       <c r="A157" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7327,7 +7327,7 @@
       <c r="Q157" s="4"/>
       <c r="R157" s="4"/>
     </row>
-    <row r="158" ht="14.25" customHeight="1">
+    <row r="158" ht="14.25" hidden="1" customHeight="1">
       <c r="A158" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7364,7 +7364,7 @@
       <c r="Q158" s="4"/>
       <c r="R158" s="4"/>
     </row>
-    <row r="159" ht="14.25" customHeight="1">
+    <row r="159" ht="14.25" hidden="1" customHeight="1">
       <c r="A159" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7401,7 +7401,7 @@
       <c r="Q159" s="4"/>
       <c r="R159" s="4"/>
     </row>
-    <row r="160" ht="14.25" customHeight="1">
+    <row r="160" ht="14.25" hidden="1" customHeight="1">
       <c r="A160" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7438,7 +7438,7 @@
       <c r="Q160" s="4"/>
       <c r="R160" s="4"/>
     </row>
-    <row r="161" ht="14.25" customHeight="1">
+    <row r="161" ht="14.25" hidden="1" customHeight="1">
       <c r="A161" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7475,7 +7475,7 @@
       <c r="Q161" s="4"/>
       <c r="R161" s="4"/>
     </row>
-    <row r="162" ht="14.25" customHeight="1">
+    <row r="162" ht="14.25" hidden="1" customHeight="1">
       <c r="A162" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7512,7 +7512,7 @@
       <c r="Q162" s="4"/>
       <c r="R162" s="4"/>
     </row>
-    <row r="163" ht="14.25" customHeight="1">
+    <row r="163" ht="14.25" hidden="1" customHeight="1">
       <c r="A163" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7549,7 +7549,7 @@
       <c r="Q163" s="4"/>
       <c r="R163" s="4"/>
     </row>
-    <row r="164" ht="14.25" customHeight="1">
+    <row r="164" ht="14.25" hidden="1" customHeight="1">
       <c r="A164" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7586,7 +7586,7 @@
       <c r="Q164" s="4"/>
       <c r="R164" s="4"/>
     </row>
-    <row r="165" ht="14.25" customHeight="1">
+    <row r="165" ht="14.25" hidden="1" customHeight="1">
       <c r="A165" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7623,7 +7623,7 @@
       <c r="Q165" s="4"/>
       <c r="R165" s="4"/>
     </row>
-    <row r="166" ht="14.25" customHeight="1">
+    <row r="166" ht="14.25" hidden="1" customHeight="1">
       <c r="A166" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7660,7 +7660,7 @@
       <c r="Q166" s="4"/>
       <c r="R166" s="4"/>
     </row>
-    <row r="167" ht="14.25" customHeight="1">
+    <row r="167" ht="14.25" hidden="1" customHeight="1">
       <c r="A167" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7697,7 +7697,7 @@
       <c r="Q167" s="4"/>
       <c r="R167" s="4"/>
     </row>
-    <row r="168" ht="14.25" customHeight="1">
+    <row r="168" ht="14.25" hidden="1" customHeight="1">
       <c r="A168" s="5">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -7734,7 +7734,7 @@
       <c r="Q168" s="4"/>
       <c r="R168" s="4"/>
     </row>
-    <row r="169" ht="14.25" customHeight="1">
+    <row r="169" ht="14.25" hidden="1" customHeight="1">
       <c r="A169" s="5">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -7771,7 +7771,7 @@
       <c r="Q169" s="4"/>
       <c r="R169" s="4"/>
     </row>
-    <row r="170" ht="14.25" customHeight="1">
+    <row r="170" ht="14.25" hidden="1" customHeight="1">
       <c r="A170" s="5">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -7808,7 +7808,7 @@
       <c r="Q170" s="4"/>
       <c r="R170" s="4"/>
     </row>
-    <row r="171" ht="14.25" customHeight="1">
+    <row r="171" ht="14.25" hidden="1" customHeight="1">
       <c r="A171" s="5">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -7845,7 +7845,7 @@
       <c r="Q171" s="4"/>
       <c r="R171" s="4"/>
     </row>
-    <row r="172" ht="14.25" customHeight="1">
+    <row r="172" ht="14.25" hidden="1" customHeight="1">
       <c r="A172" s="5">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -7882,7 +7882,7 @@
       <c r="Q172" s="4"/>
       <c r="R172" s="4"/>
     </row>
-    <row r="173" ht="14.25" customHeight="1">
+    <row r="173" ht="14.25" hidden="1" customHeight="1">
       <c r="A173" s="5">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -7919,7 +7919,7 @@
       <c r="Q173" s="4"/>
       <c r="R173" s="4"/>
     </row>
-    <row r="174" ht="14.25" customHeight="1">
+    <row r="174" ht="14.25" hidden="1" customHeight="1">
       <c r="A174" s="5">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -7956,7 +7956,7 @@
       <c r="Q174" s="4"/>
       <c r="R174" s="4"/>
     </row>
-    <row r="175" ht="14.25" customHeight="1">
+    <row r="175" ht="14.25" hidden="1" customHeight="1">
       <c r="A175" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -7993,7 +7993,7 @@
       <c r="Q175" s="4"/>
       <c r="R175" s="4"/>
     </row>
-    <row r="176" ht="14.25" customHeight="1">
+    <row r="176" ht="14.25" hidden="1" customHeight="1">
       <c r="A176" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -8030,7 +8030,7 @@
       <c r="Q176" s="4"/>
       <c r="R176" s="4"/>
     </row>
-    <row r="177" ht="14.25" customHeight="1">
+    <row r="177" ht="14.25" hidden="1" customHeight="1">
       <c r="A177" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -8067,7 +8067,7 @@
       <c r="Q177" s="4"/>
       <c r="R177" s="4"/>
     </row>
-    <row r="178" ht="14.25" customHeight="1">
+    <row r="178" ht="14.25" hidden="1" customHeight="1">
       <c r="A178" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -8104,7 +8104,7 @@
       <c r="Q178" s="4"/>
       <c r="R178" s="4"/>
     </row>
-    <row r="179" ht="14.25" customHeight="1">
+    <row r="179" ht="14.25" hidden="1" customHeight="1">
       <c r="A179" s="5">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -8141,7 +8141,7 @@
       <c r="Q179" s="4"/>
       <c r="R179" s="4"/>
     </row>
-    <row r="180" ht="14.25" customHeight="1">
+    <row r="180" ht="14.25" hidden="1" customHeight="1">
       <c r="A180" s="5">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -8178,7 +8178,7 @@
       <c r="Q180" s="4"/>
       <c r="R180" s="4"/>
     </row>
-    <row r="181" ht="14.25" customHeight="1">
+    <row r="181" ht="14.25" hidden="1" customHeight="1">
       <c r="A181" s="5">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -8215,7 +8215,7 @@
       <c r="Q181" s="4"/>
       <c r="R181" s="4"/>
     </row>
-    <row r="182" ht="14.25" customHeight="1">
+    <row r="182" ht="14.25" hidden="1" customHeight="1">
       <c r="A182" s="5">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -8252,7 +8252,7 @@
       <c r="Q182" s="4"/>
       <c r="R182" s="4"/>
     </row>
-    <row r="183" ht="14.25" customHeight="1">
+    <row r="183" ht="14.25" hidden="1" customHeight="1">
       <c r="A183" s="5">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -8289,7 +8289,7 @@
       <c r="Q183" s="4"/>
       <c r="R183" s="4"/>
     </row>
-    <row r="184" ht="14.25" customHeight="1">
+    <row r="184" ht="14.25" hidden="1" customHeight="1">
       <c r="A184" s="5">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -8326,7 +8326,7 @@
       <c r="Q184" s="4"/>
       <c r="R184" s="4"/>
     </row>
-    <row r="185" ht="14.25" customHeight="1">
+    <row r="185" ht="14.25" hidden="1" customHeight="1">
       <c r="A185" s="5">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -8363,7 +8363,7 @@
       <c r="Q185" s="4"/>
       <c r="R185" s="4"/>
     </row>
-    <row r="186" ht="14.25" customHeight="1">
+    <row r="186" ht="14.25" hidden="1" customHeight="1">
       <c r="A186" s="5">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -8400,7 +8400,7 @@
       <c r="Q186" s="4"/>
       <c r="R186" s="4"/>
     </row>
-    <row r="187" ht="14.25" customHeight="1">
+    <row r="187" ht="14.25" hidden="1" customHeight="1">
       <c r="A187" s="5">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -8437,7 +8437,7 @@
       <c r="Q187" s="4"/>
       <c r="R187" s="4"/>
     </row>
-    <row r="188" ht="14.25" customHeight="1">
+    <row r="188" ht="14.25" hidden="1" customHeight="1">
       <c r="A188" s="5">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -8474,7 +8474,7 @@
       <c r="Q188" s="4"/>
       <c r="R188" s="4"/>
     </row>
-    <row r="189" ht="14.25" customHeight="1">
+    <row r="189" ht="14.25" hidden="1" customHeight="1">
       <c r="A189" s="5">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -8511,7 +8511,7 @@
       <c r="Q189" s="4"/>
       <c r="R189" s="4"/>
     </row>
-    <row r="190" ht="14.25" customHeight="1">
+    <row r="190" ht="14.25" hidden="1" customHeight="1">
       <c r="A190" s="5">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -8548,7 +8548,7 @@
       <c r="Q190" s="4"/>
       <c r="R190" s="4"/>
     </row>
-    <row r="191" ht="14.25" customHeight="1">
+    <row r="191" ht="14.25" hidden="1" customHeight="1">
       <c r="A191" s="5">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -8585,7 +8585,7 @@
       <c r="Q191" s="4"/>
       <c r="R191" s="4"/>
     </row>
-    <row r="192" ht="14.25" customHeight="1">
+    <row r="192" ht="14.25" hidden="1" customHeight="1">
       <c r="A192" s="5">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -8622,7 +8622,7 @@
       <c r="Q192" s="4"/>
       <c r="R192" s="4"/>
     </row>
-    <row r="193" ht="14.25" customHeight="1">
+    <row r="193" ht="14.25" hidden="1" customHeight="1">
       <c r="A193" s="5">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -8659,7 +8659,7 @@
       <c r="Q193" s="4"/>
       <c r="R193" s="4"/>
     </row>
-    <row r="194" ht="14.25" customHeight="1">
+    <row r="194" ht="14.25" hidden="1" customHeight="1">
       <c r="A194" s="5">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -8696,7 +8696,7 @@
       <c r="Q194" s="4"/>
       <c r="R194" s="4"/>
     </row>
-    <row r="195" ht="14.25" customHeight="1">
+    <row r="195" ht="14.25" hidden="1" customHeight="1">
       <c r="A195" s="5">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -8733,7 +8733,7 @@
       <c r="Q195" s="4"/>
       <c r="R195" s="4"/>
     </row>
-    <row r="196" ht="14.25" customHeight="1">
+    <row r="196" ht="14.25" hidden="1" customHeight="1">
       <c r="A196" s="5">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -8770,7 +8770,7 @@
       <c r="Q196" s="4"/>
       <c r="R196" s="4"/>
     </row>
-    <row r="197" ht="14.25" customHeight="1">
+    <row r="197" ht="14.25" hidden="1" customHeight="1">
       <c r="A197" s="5">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -8807,7 +8807,7 @@
       <c r="Q197" s="4"/>
       <c r="R197" s="4"/>
     </row>
-    <row r="198" ht="14.25" customHeight="1">
+    <row r="198" ht="14.25" hidden="1" customHeight="1">
       <c r="A198" s="5">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -9362,7 +9362,7 @@
       <c r="Q212" s="4"/>
       <c r="R212" s="4"/>
     </row>
-    <row r="213" ht="14.25" customHeight="1">
+    <row r="213" ht="14.25" hidden="1" customHeight="1">
       <c r="A213" s="5">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -9399,7 +9399,7 @@
       <c r="Q213" s="4"/>
       <c r="R213" s="4"/>
     </row>
-    <row r="214" ht="14.25" customHeight="1">
+    <row r="214" ht="14.25" hidden="1" customHeight="1">
       <c r="A214" s="5">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -9436,7 +9436,7 @@
       <c r="Q214" s="4"/>
       <c r="R214" s="4"/>
     </row>
-    <row r="215" ht="14.25" customHeight="1">
+    <row r="215" ht="14.25" hidden="1" customHeight="1">
       <c r="A215" s="5">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -9473,7 +9473,7 @@
       <c r="Q215" s="4"/>
       <c r="R215" s="4"/>
     </row>
-    <row r="216" ht="14.25" customHeight="1">
+    <row r="216" ht="14.25" hidden="1" customHeight="1">
       <c r="A216" s="5">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -9510,7 +9510,7 @@
       <c r="Q216" s="4"/>
       <c r="R216" s="4"/>
     </row>
-    <row r="217" ht="14.25" customHeight="1">
+    <row r="217" ht="14.25" hidden="1" customHeight="1">
       <c r="A217" s="5">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -9547,7 +9547,7 @@
       <c r="Q217" s="4"/>
       <c r="R217" s="4"/>
     </row>
-    <row r="218" ht="14.25" customHeight="1">
+    <row r="218" ht="14.25" hidden="1" customHeight="1">
       <c r="A218" s="5">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -9584,7 +9584,7 @@
       <c r="Q218" s="4"/>
       <c r="R218" s="4"/>
     </row>
-    <row r="219" ht="14.25" customHeight="1">
+    <row r="219" ht="14.25" hidden="1" customHeight="1">
       <c r="A219" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9621,7 +9621,7 @@
       <c r="Q219" s="4"/>
       <c r="R219" s="4"/>
     </row>
-    <row r="220" ht="14.25" customHeight="1">
+    <row r="220" ht="14.25" hidden="1" customHeight="1">
       <c r="A220" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9658,7 +9658,7 @@
       <c r="Q220" s="4"/>
       <c r="R220" s="4"/>
     </row>
-    <row r="221" ht="14.25" customHeight="1">
+    <row r="221" ht="14.25" hidden="1" customHeight="1">
       <c r="A221" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9695,7 +9695,7 @@
       <c r="Q221" s="4"/>
       <c r="R221" s="4"/>
     </row>
-    <row r="222" ht="14.25" customHeight="1">
+    <row r="222" ht="14.25" hidden="1" customHeight="1">
       <c r="A222" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9732,7 +9732,7 @@
       <c r="Q222" s="4"/>
       <c r="R222" s="4"/>
     </row>
-    <row r="223" ht="14.25" customHeight="1">
+    <row r="223" ht="14.25" hidden="1" customHeight="1">
       <c r="A223" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9769,7 +9769,7 @@
       <c r="Q223" s="4"/>
       <c r="R223" s="4"/>
     </row>
-    <row r="224" ht="14.25" customHeight="1">
+    <row r="224" ht="14.25" hidden="1" customHeight="1">
       <c r="A224" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9806,7 +9806,7 @@
       <c r="Q224" s="4"/>
       <c r="R224" s="4"/>
     </row>
-    <row r="225" ht="14.25" customHeight="1">
+    <row r="225" ht="14.25" hidden="1" customHeight="1">
       <c r="A225" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9843,7 +9843,7 @@
       <c r="Q225" s="4"/>
       <c r="R225" s="4"/>
     </row>
-    <row r="226" ht="14.25" customHeight="1">
+    <row r="226" ht="14.25" hidden="1" customHeight="1">
       <c r="A226" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9880,7 +9880,7 @@
       <c r="Q226" s="4"/>
       <c r="R226" s="4"/>
     </row>
-    <row r="227" ht="14.25" customHeight="1">
+    <row r="227" ht="14.25" hidden="1" customHeight="1">
       <c r="A227" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9917,7 +9917,7 @@
       <c r="Q227" s="4"/>
       <c r="R227" s="4"/>
     </row>
-    <row r="228" ht="14.25" customHeight="1">
+    <row r="228" ht="14.25" hidden="1" customHeight="1">
       <c r="A228" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -9954,7 +9954,7 @@
       <c r="Q228" s="4"/>
       <c r="R228" s="4"/>
     </row>
-    <row r="229" ht="14.25" customHeight="1">
+    <row r="229" ht="14.25" hidden="1" customHeight="1">
       <c r="A229" s="5">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -9991,7 +9991,7 @@
       <c r="Q229" s="4"/>
       <c r="R229" s="4"/>
     </row>
-    <row r="230" ht="14.25" customHeight="1">
+    <row r="230" ht="14.25" hidden="1" customHeight="1">
       <c r="A230" s="5">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -10028,7 +10028,7 @@
       <c r="Q230" s="4"/>
       <c r="R230" s="4"/>
     </row>
-    <row r="231" ht="14.25" customHeight="1">
+    <row r="231" ht="14.25" hidden="1" customHeight="1">
       <c r="A231" s="5">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -10065,7 +10065,7 @@
       <c r="Q231" s="4"/>
       <c r="R231" s="4"/>
     </row>
-    <row r="232" ht="14.25" customHeight="1">
+    <row r="232" ht="14.25" hidden="1" customHeight="1">
       <c r="A232" s="5">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -10102,7 +10102,7 @@
       <c r="Q232" s="4"/>
       <c r="R232" s="4"/>
     </row>
-    <row r="233" ht="14.25" customHeight="1">
+    <row r="233" ht="14.25" hidden="1" customHeight="1">
       <c r="A233" s="5">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -10139,7 +10139,7 @@
       <c r="Q233" s="4"/>
       <c r="R233" s="4"/>
     </row>
-    <row r="234" ht="14.25" customHeight="1">
+    <row r="234" ht="14.25" hidden="1" customHeight="1">
       <c r="A234" s="5">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -10176,7 +10176,7 @@
       <c r="Q234" s="4"/>
       <c r="R234" s="4"/>
     </row>
-    <row r="235" ht="14.25" customHeight="1">
+    <row r="235" ht="14.25" hidden="1" customHeight="1">
       <c r="A235" s="5">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -10213,7 +10213,7 @@
       <c r="Q235" s="4"/>
       <c r="R235" s="4"/>
     </row>
-    <row r="236" ht="14.25" customHeight="1">
+    <row r="236" ht="14.25" hidden="1" customHeight="1">
       <c r="A236" s="5">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -10250,7 +10250,7 @@
       <c r="Q236" s="4"/>
       <c r="R236" s="4"/>
     </row>
-    <row r="237" ht="14.25" customHeight="1">
+    <row r="237" ht="14.25" hidden="1" customHeight="1">
       <c r="A237" s="5">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -10287,7 +10287,7 @@
       <c r="Q237" s="4"/>
       <c r="R237" s="4"/>
     </row>
-    <row r="238" ht="14.25" customHeight="1">
+    <row r="238" ht="14.25" hidden="1" customHeight="1">
       <c r="A238" s="5">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -10324,7 +10324,7 @@
       <c r="Q238" s="4"/>
       <c r="R238" s="4"/>
     </row>
-    <row r="239" ht="14.25" customHeight="1">
+    <row r="239" ht="14.25" hidden="1" customHeight="1">
       <c r="A239" s="5">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -10361,7 +10361,7 @@
       <c r="Q239" s="4"/>
       <c r="R239" s="4"/>
     </row>
-    <row r="240" ht="14.25" customHeight="1">
+    <row r="240" ht="14.25" hidden="1" customHeight="1">
       <c r="A240" s="5">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -10398,7 +10398,7 @@
       <c r="Q240" s="4"/>
       <c r="R240" s="4"/>
     </row>
-    <row r="241" ht="14.25" customHeight="1">
+    <row r="241" ht="14.25" hidden="1" customHeight="1">
       <c r="A241" s="5">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -10435,7 +10435,7 @@
       <c r="Q241" s="4"/>
       <c r="R241" s="4"/>
     </row>
-    <row r="242" ht="14.25" customHeight="1">
+    <row r="242" ht="14.25" hidden="1" customHeight="1">
       <c r="A242" s="5">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -10472,7 +10472,7 @@
       <c r="Q242" s="4"/>
       <c r="R242" s="4"/>
     </row>
-    <row r="243" ht="14.25" customHeight="1">
+    <row r="243" ht="14.25" hidden="1" customHeight="1">
       <c r="A243" s="5">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -10509,7 +10509,7 @@
       <c r="Q243" s="4"/>
       <c r="R243" s="4"/>
     </row>
-    <row r="244" ht="14.25" customHeight="1">
+    <row r="244" ht="14.25" hidden="1" customHeight="1">
       <c r="A244" s="5">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -10546,7 +10546,7 @@
       <c r="Q244" s="4"/>
       <c r="R244" s="4"/>
     </row>
-    <row r="245" ht="14.25" customHeight="1">
+    <row r="245" ht="14.25" hidden="1" customHeight="1">
       <c r="A245" s="5">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -10583,7 +10583,7 @@
       <c r="Q245" s="4"/>
       <c r="R245" s="4"/>
     </row>
-    <row r="246" ht="14.25" customHeight="1">
+    <row r="246" ht="14.25" hidden="1" customHeight="1">
       <c r="A246" s="5">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -10620,7 +10620,7 @@
       <c r="Q246" s="4"/>
       <c r="R246" s="4"/>
     </row>
-    <row r="247" ht="14.25" customHeight="1">
+    <row r="247" ht="14.25" hidden="1" customHeight="1">
       <c r="A247" s="5">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -10657,7 +10657,7 @@
       <c r="Q247" s="4"/>
       <c r="R247" s="4"/>
     </row>
-    <row r="248" ht="14.25" customHeight="1">
+    <row r="248" ht="14.25" hidden="1" customHeight="1">
       <c r="A248" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -10694,7 +10694,7 @@
       <c r="Q248" s="4"/>
       <c r="R248" s="4"/>
     </row>
-    <row r="249" ht="14.25" customHeight="1">
+    <row r="249" ht="14.25" hidden="1" customHeight="1">
       <c r="A249" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -10731,7 +10731,7 @@
       <c r="Q249" s="4"/>
       <c r="R249" s="4"/>
     </row>
-    <row r="250" ht="14.25" customHeight="1">
+    <row r="250" ht="14.25" hidden="1" customHeight="1">
       <c r="A250" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -10768,7 +10768,7 @@
       <c r="Q250" s="4"/>
       <c r="R250" s="4"/>
     </row>
-    <row r="251" ht="14.25" customHeight="1">
+    <row r="251" ht="14.25" hidden="1" customHeight="1">
       <c r="A251" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -10805,7 +10805,7 @@
       <c r="Q251" s="4"/>
       <c r="R251" s="4"/>
     </row>
-    <row r="252" ht="14.25" customHeight="1">
+    <row r="252" ht="14.25" hidden="1" customHeight="1">
       <c r="A252" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -10842,7 +10842,7 @@
       <c r="Q252" s="4"/>
       <c r="R252" s="4"/>
     </row>
-    <row r="253" ht="14.25" customHeight="1">
+    <row r="253" ht="14.25" hidden="1" customHeight="1">
       <c r="A253" s="5">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -10879,7 +10879,7 @@
       <c r="Q253" s="4"/>
       <c r="R253" s="4"/>
     </row>
-    <row r="254" ht="14.25" customHeight="1">
+    <row r="254" ht="14.25" hidden="1" customHeight="1">
       <c r="A254" s="5">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -10916,7 +10916,7 @@
       <c r="Q254" s="4"/>
       <c r="R254" s="4"/>
     </row>
-    <row r="255" ht="14.25" customHeight="1">
+    <row r="255" ht="14.25" hidden="1" customHeight="1">
       <c r="A255" s="5">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -10953,7 +10953,7 @@
       <c r="Q255" s="4"/>
       <c r="R255" s="4"/>
     </row>
-    <row r="256" ht="14.25" customHeight="1">
+    <row r="256" ht="14.25" hidden="1" customHeight="1">
       <c r="A256" s="5">
         <f t="shared" si="1"/>
         <v>136</v>
@@ -10990,7 +10990,7 @@
       <c r="Q256" s="4"/>
       <c r="R256" s="4"/>
     </row>
-    <row r="257" ht="14.25" customHeight="1">
+    <row r="257" ht="14.25" hidden="1" customHeight="1">
       <c r="A257" s="5">
         <f t="shared" si="1"/>
         <v>136</v>
@@ -11027,7 +11027,7 @@
       <c r="Q257" s="4"/>
       <c r="R257" s="4"/>
     </row>
-    <row r="258" ht="14.25" customHeight="1">
+    <row r="258" ht="14.25" hidden="1" customHeight="1">
       <c r="A258" s="5">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -11064,7 +11064,7 @@
       <c r="Q258" s="4"/>
       <c r="R258" s="4"/>
     </row>
-    <row r="259" ht="14.25" customHeight="1">
+    <row r="259" ht="14.25" hidden="1" customHeight="1">
       <c r="A259" s="5">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -11101,7 +11101,7 @@
       <c r="Q259" s="4"/>
       <c r="R259" s="4"/>
     </row>
-    <row r="260" ht="14.25" customHeight="1">
+    <row r="260" ht="14.25" hidden="1" customHeight="1">
       <c r="A260" s="5">
         <f t="shared" si="1"/>
         <v>139</v>
@@ -11138,7 +11138,7 @@
       <c r="Q260" s="4"/>
       <c r="R260" s="4"/>
     </row>
-    <row r="261" ht="14.25" customHeight="1">
+    <row r="261" ht="14.25" hidden="1" customHeight="1">
       <c r="A261" s="5">
         <f t="shared" si="1"/>
         <v>141</v>
@@ -11175,7 +11175,7 @@
       <c r="Q261" s="4"/>
       <c r="R261" s="4"/>
     </row>
-    <row r="262" ht="14.25" customHeight="1">
+    <row r="262" ht="14.25" hidden="1" customHeight="1">
       <c r="A262" s="5">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -11212,7 +11212,7 @@
       <c r="Q262" s="4"/>
       <c r="R262" s="4"/>
     </row>
-    <row r="263" ht="14.25" customHeight="1">
+    <row r="263" ht="14.25" hidden="1" customHeight="1">
       <c r="A263" s="5">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -11249,7 +11249,7 @@
       <c r="Q263" s="4"/>
       <c r="R263" s="4"/>
     </row>
-    <row r="264" ht="14.25" customHeight="1">
+    <row r="264" ht="14.25" hidden="1" customHeight="1">
       <c r="A264" s="5">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -11286,7 +11286,7 @@
       <c r="Q264" s="4"/>
       <c r="R264" s="4"/>
     </row>
-    <row r="265" ht="14.25" customHeight="1">
+    <row r="265" ht="14.25" hidden="1" customHeight="1">
       <c r="A265" s="5">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -11323,7 +11323,7 @@
       <c r="Q265" s="4"/>
       <c r="R265" s="4"/>
     </row>
-    <row r="266" ht="14.25" customHeight="1">
+    <row r="266" ht="14.25" hidden="1" customHeight="1">
       <c r="A266" s="5">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -11360,7 +11360,7 @@
       <c r="Q266" s="4"/>
       <c r="R266" s="4"/>
     </row>
-    <row r="267" ht="14.25" customHeight="1">
+    <row r="267" ht="14.25" hidden="1" customHeight="1">
       <c r="A267" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11397,7 +11397,7 @@
       <c r="Q267" s="4"/>
       <c r="R267" s="4"/>
     </row>
-    <row r="268" ht="14.25" customHeight="1">
+    <row r="268" ht="14.25" hidden="1" customHeight="1">
       <c r="A268" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11434,7 +11434,7 @@
       <c r="Q268" s="4"/>
       <c r="R268" s="4"/>
     </row>
-    <row r="269" ht="14.25" customHeight="1">
+    <row r="269" ht="14.25" hidden="1" customHeight="1">
       <c r="A269" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11471,7 +11471,7 @@
       <c r="Q269" s="4"/>
       <c r="R269" s="4"/>
     </row>
-    <row r="270" ht="14.25" customHeight="1">
+    <row r="270" ht="14.25" hidden="1" customHeight="1">
       <c r="A270" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11508,7 +11508,7 @@
       <c r="Q270" s="4"/>
       <c r="R270" s="4"/>
     </row>
-    <row r="271" ht="14.25" customHeight="1">
+    <row r="271" ht="14.25" hidden="1" customHeight="1">
       <c r="A271" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11545,7 +11545,7 @@
       <c r="Q271" s="4"/>
       <c r="R271" s="4"/>
     </row>
-    <row r="272" ht="14.25" customHeight="1">
+    <row r="272" ht="14.25" hidden="1" customHeight="1">
       <c r="A272" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11582,7 +11582,7 @@
       <c r="Q272" s="4"/>
       <c r="R272" s="4"/>
     </row>
-    <row r="273" ht="14.25" customHeight="1">
+    <row r="273" ht="14.25" hidden="1" customHeight="1">
       <c r="A273" s="5">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -11619,7 +11619,7 @@
       <c r="Q273" s="4"/>
       <c r="R273" s="4"/>
     </row>
-    <row r="274" ht="14.25" customHeight="1">
+    <row r="274" ht="14.25" hidden="1" customHeight="1">
       <c r="A274" s="5">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -11656,7 +11656,7 @@
       <c r="Q274" s="4"/>
       <c r="R274" s="4"/>
     </row>
-    <row r="275" ht="14.25" customHeight="1">
+    <row r="275" ht="14.25" hidden="1" customHeight="1">
       <c r="A275" s="5">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -11693,7 +11693,7 @@
       <c r="Q275" s="4"/>
       <c r="R275" s="4"/>
     </row>
-    <row r="276" ht="14.25" customHeight="1">
+    <row r="276" ht="14.25" hidden="1" customHeight="1">
       <c r="A276" s="5">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -11730,7 +11730,7 @@
       <c r="Q276" s="4"/>
       <c r="R276" s="4"/>
     </row>
-    <row r="277" ht="14.25" customHeight="1">
+    <row r="277" ht="14.25" hidden="1" customHeight="1">
       <c r="A277" s="5">
         <f t="shared" si="1"/>
         <v>163</v>
@@ -11767,7 +11767,7 @@
       <c r="Q277" s="4"/>
       <c r="R277" s="4"/>
     </row>
-    <row r="278" ht="14.25" customHeight="1">
+    <row r="278" ht="14.25" hidden="1" customHeight="1">
       <c r="A278" s="5">
         <f t="shared" si="1"/>
         <v>163</v>
@@ -11804,7 +11804,7 @@
       <c r="Q278" s="4"/>
       <c r="R278" s="4"/>
     </row>
-    <row r="279" ht="14.25" customHeight="1">
+    <row r="279" ht="14.25" hidden="1" customHeight="1">
       <c r="A279" s="5">
         <f t="shared" si="1"/>
         <v>166</v>
@@ -11841,7 +11841,7 @@
       <c r="Q279" s="4"/>
       <c r="R279" s="4"/>
     </row>
-    <row r="280" ht="14.25" customHeight="1">
+    <row r="280" ht="14.25" hidden="1" customHeight="1">
       <c r="A280" s="5">
         <f t="shared" si="1"/>
         <v>166</v>
@@ -11878,7 +11878,7 @@
       <c r="Q280" s="4"/>
       <c r="R280" s="4"/>
     </row>
-    <row r="281" ht="14.25" customHeight="1">
+    <row r="281" ht="14.25" hidden="1" customHeight="1">
       <c r="A281" s="5">
         <f t="shared" si="1"/>
         <v>166</v>
@@ -11915,7 +11915,7 @@
       <c r="Q281" s="4"/>
       <c r="R281" s="4"/>
     </row>
-    <row r="282" ht="14.25" customHeight="1">
+    <row r="282" ht="14.25" hidden="1" customHeight="1">
       <c r="A282" s="5">
         <f t="shared" si="1"/>
         <v>169</v>
@@ -11952,7 +11952,7 @@
       <c r="Q282" s="4"/>
       <c r="R282" s="4"/>
     </row>
-    <row r="283" ht="14.25" customHeight="1">
+    <row r="283" ht="14.25" hidden="1" customHeight="1">
       <c r="A283" s="5">
         <f t="shared" si="1"/>
         <v>179</v>
@@ -11989,7 +11989,7 @@
       <c r="Q283" s="4"/>
       <c r="R283" s="4"/>
     </row>
-    <row r="284" ht="14.25" customHeight="1">
+    <row r="284" ht="14.25" hidden="1" customHeight="1">
       <c r="A284" s="5">
         <f t="shared" si="1"/>
         <v>194</v>
@@ -12026,7 +12026,7 @@
       <c r="Q284" s="4"/>
       <c r="R284" s="4"/>
     </row>
-    <row r="285" ht="14.25" customHeight="1">
+    <row r="285" ht="14.25" hidden="1" customHeight="1">
       <c r="A285" s="5">
         <f t="shared" si="1"/>
         <v>194</v>
@@ -12063,7 +12063,7 @@
       <c r="Q285" s="4"/>
       <c r="R285" s="4"/>
     </row>
-    <row r="286" ht="14.25" customHeight="1">
+    <row r="286" ht="14.25" hidden="1" customHeight="1">
       <c r="A286" s="5">
         <f t="shared" si="1"/>
         <v>194</v>
@@ -12100,7 +12100,7 @@
       <c r="Q286" s="4"/>
       <c r="R286" s="4"/>
     </row>
-    <row r="287" ht="14.25" customHeight="1">
+    <row r="287" ht="14.25" hidden="1" customHeight="1">
       <c r="A287" s="5">
         <f t="shared" si="1"/>
         <v>196</v>
@@ -12137,7 +12137,7 @@
       <c r="Q287" s="4"/>
       <c r="R287" s="4"/>
     </row>
-    <row r="288" ht="14.25" customHeight="1">
+    <row r="288" ht="14.25" hidden="1" customHeight="1">
       <c r="A288" s="5">
         <f t="shared" si="1"/>
         <v>196</v>
@@ -12174,7 +12174,7 @@
       <c r="Q288" s="4"/>
       <c r="R288" s="4"/>
     </row>
-    <row r="289" ht="14.25" customHeight="1">
+    <row r="289" ht="14.25" hidden="1" customHeight="1">
       <c r="A289" s="5"/>
       <c r="B289" s="5"/>
       <c r="C289" s="5"/>
@@ -12194,7 +12194,7 @@
       <c r="Q289" s="4"/>
       <c r="R289" s="4"/>
     </row>
-    <row r="290" ht="14.25" customHeight="1">
+    <row r="290" ht="14.25" hidden="1" customHeight="1">
       <c r="A290" s="4"/>
       <c r="B290" s="4"/>
       <c r="C290" s="4"/>
@@ -12214,7 +12214,7 @@
       <c r="Q290" s="4"/>
       <c r="R290" s="4"/>
     </row>
-    <row r="291" ht="14.25" customHeight="1">
+    <row r="291" ht="14.25" hidden="1" customHeight="1">
       <c r="A291" s="4"/>
       <c r="B291" s="4"/>
       <c r="C291" s="4"/>
@@ -12234,7 +12234,7 @@
       <c r="Q291" s="4"/>
       <c r="R291" s="4"/>
     </row>
-    <row r="292" ht="14.25" customHeight="1">
+    <row r="292" ht="14.25" hidden="1" customHeight="1">
       <c r="A292" s="4"/>
       <c r="B292" s="4"/>
       <c r="C292" s="4"/>
@@ -12254,7 +12254,7 @@
       <c r="Q292" s="4"/>
       <c r="R292" s="4"/>
     </row>
-    <row r="293" ht="14.25" customHeight="1">
+    <row r="293" ht="14.25" hidden="1" customHeight="1">
       <c r="A293" s="4"/>
       <c r="B293" s="4"/>
       <c r="C293" s="4"/>
@@ -12274,7 +12274,7 @@
       <c r="Q293" s="4"/>
       <c r="R293" s="4"/>
     </row>
-    <row r="294" ht="14.25" customHeight="1">
+    <row r="294" ht="14.25" hidden="1" customHeight="1">
       <c r="A294" s="4"/>
       <c r="B294" s="4"/>
       <c r="C294" s="4"/>
@@ -12294,7 +12294,7 @@
       <c r="Q294" s="4"/>
       <c r="R294" s="4"/>
     </row>
-    <row r="295" ht="14.25" customHeight="1">
+    <row r="295" ht="14.25" hidden="1" customHeight="1">
       <c r="A295" s="4"/>
       <c r="B295" s="4"/>
       <c r="C295" s="4"/>
@@ -12314,7 +12314,7 @@
       <c r="Q295" s="4"/>
       <c r="R295" s="4"/>
     </row>
-    <row r="296" ht="14.25" customHeight="1">
+    <row r="296" ht="14.25" hidden="1" customHeight="1">
       <c r="A296" s="4"/>
       <c r="B296" s="4"/>
       <c r="C296" s="4"/>
@@ -12334,7 +12334,7 @@
       <c r="Q296" s="4"/>
       <c r="R296" s="4"/>
     </row>
-    <row r="297" ht="14.25" customHeight="1">
+    <row r="297" ht="14.25" hidden="1" customHeight="1">
       <c r="A297" s="4"/>
       <c r="B297" s="4"/>
       <c r="C297" s="4"/>
@@ -12354,7 +12354,7 @@
       <c r="Q297" s="4"/>
       <c r="R297" s="4"/>
     </row>
-    <row r="298" ht="14.25" customHeight="1">
+    <row r="298" ht="14.25" hidden="1" customHeight="1">
       <c r="A298" s="4"/>
       <c r="B298" s="4"/>
       <c r="C298" s="4"/>
@@ -12374,7 +12374,7 @@
       <c r="Q298" s="4"/>
       <c r="R298" s="4"/>
     </row>
-    <row r="299" ht="14.25" customHeight="1">
+    <row r="299" ht="14.25" hidden="1" customHeight="1">
       <c r="A299" s="4"/>
       <c r="B299" s="4"/>
       <c r="C299" s="4"/>
@@ -12394,7 +12394,7 @@
       <c r="Q299" s="4"/>
       <c r="R299" s="4"/>
     </row>
-    <row r="300" ht="14.25" customHeight="1">
+    <row r="300" ht="14.25" hidden="1" customHeight="1">
       <c r="A300" s="4"/>
       <c r="B300" s="4"/>
       <c r="C300" s="4"/>
@@ -12414,7 +12414,7 @@
       <c r="Q300" s="4"/>
       <c r="R300" s="4"/>
     </row>
-    <row r="301" ht="14.25" customHeight="1">
+    <row r="301" ht="14.25" hidden="1" customHeight="1">
       <c r="A301" s="4"/>
       <c r="B301" s="4"/>
       <c r="C301" s="4"/>
@@ -12434,7 +12434,7 @@
       <c r="Q301" s="4"/>
       <c r="R301" s="4"/>
     </row>
-    <row r="302" ht="14.25" customHeight="1">
+    <row r="302" ht="14.25" hidden="1" customHeight="1">
       <c r="A302" s="4"/>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
@@ -12454,7 +12454,7 @@
       <c r="Q302" s="4"/>
       <c r="R302" s="4"/>
     </row>
-    <row r="303" ht="14.25" customHeight="1">
+    <row r="303" ht="14.25" hidden="1" customHeight="1">
       <c r="A303" s="4"/>
       <c r="B303" s="4"/>
       <c r="C303" s="4"/>
@@ -12474,7 +12474,7 @@
       <c r="Q303" s="4"/>
       <c r="R303" s="4"/>
     </row>
-    <row r="304" ht="14.25" customHeight="1">
+    <row r="304" ht="14.25" hidden="1" customHeight="1">
       <c r="A304" s="4"/>
       <c r="B304" s="4"/>
       <c r="C304" s="4"/>
@@ -12494,7 +12494,7 @@
       <c r="Q304" s="4"/>
       <c r="R304" s="4"/>
     </row>
-    <row r="305" ht="14.25" customHeight="1">
+    <row r="305" ht="14.25" hidden="1" customHeight="1">
       <c r="A305" s="4"/>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
@@ -12514,7 +12514,7 @@
       <c r="Q305" s="4"/>
       <c r="R305" s="4"/>
     </row>
-    <row r="306" ht="14.25" customHeight="1">
+    <row r="306" ht="14.25" hidden="1" customHeight="1">
       <c r="A306" s="4"/>
       <c r="B306" s="4"/>
       <c r="C306" s="4"/>
@@ -12534,7 +12534,7 @@
       <c r="Q306" s="4"/>
       <c r="R306" s="4"/>
     </row>
-    <row r="307" ht="14.25" customHeight="1">
+    <row r="307" ht="14.25" hidden="1" customHeight="1">
       <c r="A307" s="4"/>
       <c r="B307" s="4"/>
       <c r="C307" s="4"/>
@@ -12554,7 +12554,7 @@
       <c r="Q307" s="4"/>
       <c r="R307" s="4"/>
     </row>
-    <row r="308" ht="14.25" customHeight="1">
+    <row r="308" ht="14.25" hidden="1" customHeight="1">
       <c r="A308" s="4"/>
       <c r="B308" s="4"/>
       <c r="C308" s="4"/>
@@ -12574,7 +12574,7 @@
       <c r="Q308" s="4"/>
       <c r="R308" s="4"/>
     </row>
-    <row r="309" ht="14.25" customHeight="1">
+    <row r="309" ht="14.25" hidden="1" customHeight="1">
       <c r="A309" s="4"/>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
@@ -12594,7 +12594,7 @@
       <c r="Q309" s="4"/>
       <c r="R309" s="4"/>
     </row>
-    <row r="310" ht="14.25" customHeight="1">
+    <row r="310" ht="14.25" hidden="1" customHeight="1">
       <c r="A310" s="4"/>
       <c r="B310" s="4"/>
       <c r="C310" s="4"/>
@@ -12614,7 +12614,7 @@
       <c r="Q310" s="4"/>
       <c r="R310" s="4"/>
     </row>
-    <row r="311" ht="14.25" customHeight="1">
+    <row r="311" ht="14.25" hidden="1" customHeight="1">
       <c r="A311" s="4"/>
       <c r="B311" s="4"/>
       <c r="C311" s="4"/>
@@ -12634,7 +12634,7 @@
       <c r="Q311" s="4"/>
       <c r="R311" s="4"/>
     </row>
-    <row r="312" ht="14.25" customHeight="1">
+    <row r="312" ht="14.25" hidden="1" customHeight="1">
       <c r="A312" s="4"/>
       <c r="B312" s="4"/>
       <c r="C312" s="4"/>
@@ -12654,7 +12654,7 @@
       <c r="Q312" s="4"/>
       <c r="R312" s="4"/>
     </row>
-    <row r="313" ht="14.25" customHeight="1">
+    <row r="313" ht="14.25" hidden="1" customHeight="1">
       <c r="A313" s="11"/>
       <c r="B313" s="11"/>
       <c r="C313" s="11"/>
@@ -12674,7 +12674,7 @@
       <c r="Q313" s="11"/>
       <c r="R313" s="11"/>
     </row>
-    <row r="314" ht="14.25" customHeight="1">
+    <row r="314" ht="14.25" hidden="1" customHeight="1">
       <c r="A314" s="4"/>
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
@@ -12694,7 +12694,7 @@
       <c r="Q314" s="4"/>
       <c r="R314" s="4"/>
     </row>
-    <row r="315" ht="14.25" customHeight="1">
+    <row r="315" ht="14.25" hidden="1" customHeight="1">
       <c r="A315" s="4"/>
       <c r="B315" s="4"/>
       <c r="C315" s="4"/>
@@ -12714,7 +12714,7 @@
       <c r="Q315" s="4"/>
       <c r="R315" s="4"/>
     </row>
-    <row r="316" ht="14.25" customHeight="1">
+    <row r="316" ht="14.25" hidden="1" customHeight="1">
       <c r="A316" s="4"/>
       <c r="B316" s="4"/>
       <c r="C316" s="4"/>
@@ -12734,7 +12734,7 @@
       <c r="Q316" s="4"/>
       <c r="R316" s="4"/>
     </row>
-    <row r="317" ht="14.25" customHeight="1">
+    <row r="317" ht="14.25" hidden="1" customHeight="1">
       <c r="A317" s="4"/>
       <c r="B317" s="4"/>
       <c r="C317" s="4"/>
@@ -12754,7 +12754,7 @@
       <c r="Q317" s="4"/>
       <c r="R317" s="4"/>
     </row>
-    <row r="318" ht="14.25" customHeight="1">
+    <row r="318" ht="14.25" hidden="1" customHeight="1">
       <c r="A318" s="4"/>
       <c r="B318" s="4"/>
       <c r="C318" s="4"/>
@@ -12774,7 +12774,7 @@
       <c r="Q318" s="4"/>
       <c r="R318" s="4"/>
     </row>
-    <row r="319" ht="14.25" customHeight="1">
+    <row r="319" ht="14.25" hidden="1" customHeight="1">
       <c r="A319" s="4"/>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -12794,7 +12794,7 @@
       <c r="Q319" s="4"/>
       <c r="R319" s="4"/>
     </row>
-    <row r="320" ht="14.25" customHeight="1">
+    <row r="320" ht="14.25" hidden="1" customHeight="1">
       <c r="A320" s="4"/>
       <c r="B320" s="4"/>
       <c r="C320" s="4"/>
@@ -12814,7 +12814,7 @@
       <c r="Q320" s="4"/>
       <c r="R320" s="4"/>
     </row>
-    <row r="321" ht="14.25" customHeight="1">
+    <row r="321" ht="14.25" hidden="1" customHeight="1">
       <c r="A321" s="4"/>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -12834,7 +12834,7 @@
       <c r="Q321" s="4"/>
       <c r="R321" s="4"/>
     </row>
-    <row r="322" ht="14.25" customHeight="1">
+    <row r="322" ht="14.25" hidden="1" customHeight="1">
       <c r="A322" s="4"/>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -12854,7 +12854,7 @@
       <c r="Q322" s="4"/>
       <c r="R322" s="4"/>
     </row>
-    <row r="323" ht="14.25" customHeight="1">
+    <row r="323" ht="14.25" hidden="1" customHeight="1">
       <c r="A323" s="4"/>
       <c r="B323" s="4"/>
       <c r="C323" s="4"/>
@@ -12874,7 +12874,7 @@
       <c r="Q323" s="4"/>
       <c r="R323" s="4"/>
     </row>
-    <row r="324" ht="14.25" customHeight="1">
+    <row r="324" ht="14.25" hidden="1" customHeight="1">
       <c r="A324" s="4"/>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -12894,7 +12894,7 @@
       <c r="Q324" s="4"/>
       <c r="R324" s="4"/>
     </row>
-    <row r="325" ht="14.25" customHeight="1">
+    <row r="325" ht="14.25" hidden="1" customHeight="1">
       <c r="A325" s="4"/>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -12914,7 +12914,7 @@
       <c r="Q325" s="4"/>
       <c r="R325" s="4"/>
     </row>
-    <row r="326" ht="14.25" customHeight="1">
+    <row r="326" ht="14.25" hidden="1" customHeight="1">
       <c r="A326" s="4"/>
       <c r="B326" s="4"/>
       <c r="C326" s="4"/>
@@ -12934,7 +12934,7 @@
       <c r="Q326" s="4"/>
       <c r="R326" s="4"/>
     </row>
-    <row r="327" ht="14.25" customHeight="1">
+    <row r="327" ht="14.25" hidden="1" customHeight="1">
       <c r="A327" s="4"/>
       <c r="B327" s="4"/>
       <c r="C327" s="4"/>
@@ -12954,7 +12954,7 @@
       <c r="Q327" s="4"/>
       <c r="R327" s="4"/>
     </row>
-    <row r="328" ht="14.25" customHeight="1">
+    <row r="328" ht="14.25" hidden="1" customHeight="1">
       <c r="A328" s="4"/>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -12974,7 +12974,7 @@
       <c r="Q328" s="4"/>
       <c r="R328" s="4"/>
     </row>
-    <row r="329" ht="14.25" customHeight="1">
+    <row r="329" ht="14.25" hidden="1" customHeight="1">
       <c r="A329" s="4"/>
       <c r="B329" s="4"/>
       <c r="C329" s="4"/>
@@ -12994,7 +12994,7 @@
       <c r="Q329" s="4"/>
       <c r="R329" s="4"/>
     </row>
-    <row r="330" ht="14.25" customHeight="1">
+    <row r="330" ht="14.25" hidden="1" customHeight="1">
       <c r="A330" s="4"/>
       <c r="B330" s="4"/>
       <c r="C330" s="4"/>
@@ -13014,7 +13014,7 @@
       <c r="Q330" s="4"/>
       <c r="R330" s="4"/>
     </row>
-    <row r="331" ht="14.25" customHeight="1">
+    <row r="331" ht="14.25" hidden="1" customHeight="1">
       <c r="A331" s="4"/>
       <c r="B331" s="4"/>
       <c r="C331" s="4"/>
@@ -13034,7 +13034,7 @@
       <c r="Q331" s="4"/>
       <c r="R331" s="4"/>
     </row>
-    <row r="332" ht="14.25" customHeight="1">
+    <row r="332" ht="14.25" hidden="1" customHeight="1">
       <c r="A332" s="4"/>
       <c r="B332" s="4"/>
       <c r="C332" s="4"/>
@@ -13054,7 +13054,7 @@
       <c r="Q332" s="4"/>
       <c r="R332" s="4"/>
     </row>
-    <row r="333" ht="14.25" customHeight="1">
+    <row r="333" ht="14.25" hidden="1" customHeight="1">
       <c r="A333" s="4"/>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -13074,7 +13074,7 @@
       <c r="Q333" s="4"/>
       <c r="R333" s="4"/>
     </row>
-    <row r="334" ht="14.25" customHeight="1">
+    <row r="334" ht="14.25" hidden="1" customHeight="1">
       <c r="A334" s="4"/>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -13094,7 +13094,7 @@
       <c r="Q334" s="4"/>
       <c r="R334" s="4"/>
     </row>
-    <row r="335" ht="14.25" customHeight="1">
+    <row r="335" ht="14.25" hidden="1" customHeight="1">
       <c r="A335" s="4"/>
       <c r="B335" s="4"/>
       <c r="C335" s="4"/>
@@ -13114,7 +13114,7 @@
       <c r="Q335" s="4"/>
       <c r="R335" s="4"/>
     </row>
-    <row r="336" ht="14.25" customHeight="1">
+    <row r="336" ht="14.25" hidden="1" customHeight="1">
       <c r="A336" s="4"/>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
@@ -13134,7 +13134,7 @@
       <c r="Q336" s="4"/>
       <c r="R336" s="4"/>
     </row>
-    <row r="337" ht="14.25" customHeight="1">
+    <row r="337" ht="14.25" hidden="1" customHeight="1">
       <c r="A337" s="4"/>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
@@ -13154,7 +13154,7 @@
       <c r="Q337" s="4"/>
       <c r="R337" s="4"/>
     </row>
-    <row r="338" ht="14.25" customHeight="1">
+    <row r="338" ht="14.25" hidden="1" customHeight="1">
       <c r="A338" s="4"/>
       <c r="B338" s="4"/>
       <c r="C338" s="4"/>
@@ -13174,7 +13174,7 @@
       <c r="Q338" s="4"/>
       <c r="R338" s="4"/>
     </row>
-    <row r="339" ht="14.25" customHeight="1">
+    <row r="339" ht="14.25" hidden="1" customHeight="1">
       <c r="A339" s="4"/>
       <c r="B339" s="4"/>
       <c r="C339" s="4"/>
@@ -13194,7 +13194,7 @@
       <c r="Q339" s="4"/>
       <c r="R339" s="4"/>
     </row>
-    <row r="340" ht="14.25" customHeight="1">
+    <row r="340" ht="14.25" hidden="1" customHeight="1">
       <c r="A340" s="4"/>
       <c r="B340" s="4"/>
       <c r="C340" s="4"/>
@@ -13214,7 +13214,7 @@
       <c r="Q340" s="4"/>
       <c r="R340" s="4"/>
     </row>
-    <row r="341" ht="14.25" customHeight="1">
+    <row r="341" ht="14.25" hidden="1" customHeight="1">
       <c r="A341" s="4"/>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
@@ -13234,7 +13234,7 @@
       <c r="Q341" s="4"/>
       <c r="R341" s="4"/>
     </row>
-    <row r="342" ht="14.25" customHeight="1">
+    <row r="342" ht="14.25" hidden="1" customHeight="1">
       <c r="A342" s="4"/>
       <c r="B342" s="4"/>
       <c r="C342" s="4"/>
@@ -13254,7 +13254,7 @@
       <c r="Q342" s="4"/>
       <c r="R342" s="4"/>
     </row>
-    <row r="343" ht="14.25" customHeight="1">
+    <row r="343" ht="14.25" hidden="1" customHeight="1">
       <c r="A343" s="4"/>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
@@ -13274,7 +13274,7 @@
       <c r="Q343" s="4"/>
       <c r="R343" s="4"/>
     </row>
-    <row r="344" ht="14.25" customHeight="1">
+    <row r="344" ht="14.25" hidden="1" customHeight="1">
       <c r="A344" s="4"/>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>
@@ -13294,7 +13294,7 @@
       <c r="Q344" s="4"/>
       <c r="R344" s="4"/>
     </row>
-    <row r="345" ht="14.25" customHeight="1">
+    <row r="345" ht="14.25" hidden="1" customHeight="1">
       <c r="A345" s="4"/>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -13314,7 +13314,7 @@
       <c r="Q345" s="4"/>
       <c r="R345" s="4"/>
     </row>
-    <row r="346" ht="14.25" customHeight="1">
+    <row r="346" ht="14.25" hidden="1" customHeight="1">
       <c r="A346" s="4"/>
       <c r="B346" s="4"/>
       <c r="C346" s="4"/>
@@ -13334,7 +13334,7 @@
       <c r="Q346" s="4"/>
       <c r="R346" s="4"/>
     </row>
-    <row r="347" ht="14.25" customHeight="1">
+    <row r="347" ht="14.25" hidden="1" customHeight="1">
       <c r="A347" s="4"/>
       <c r="B347" s="4"/>
       <c r="C347" s="4"/>
@@ -13354,7 +13354,7 @@
       <c r="Q347" s="4"/>
       <c r="R347" s="4"/>
     </row>
-    <row r="348" ht="14.25" customHeight="1">
+    <row r="348" ht="14.25" hidden="1" customHeight="1">
       <c r="A348" s="4"/>
       <c r="B348" s="4"/>
       <c r="C348" s="4"/>
@@ -13374,7 +13374,7 @@
       <c r="Q348" s="4"/>
       <c r="R348" s="4"/>
     </row>
-    <row r="349" ht="14.25" customHeight="1">
+    <row r="349" ht="14.25" hidden="1" customHeight="1">
       <c r="A349" s="4"/>
       <c r="B349" s="4"/>
       <c r="C349" s="4"/>
@@ -13394,7 +13394,7 @@
       <c r="Q349" s="4"/>
       <c r="R349" s="4"/>
     </row>
-    <row r="350" ht="14.25" customHeight="1">
+    <row r="350" ht="14.25" hidden="1" customHeight="1">
       <c r="A350" s="4"/>
       <c r="B350" s="4"/>
       <c r="C350" s="4"/>
@@ -13414,7 +13414,7 @@
       <c r="Q350" s="4"/>
       <c r="R350" s="4"/>
     </row>
-    <row r="351" ht="14.25" customHeight="1">
+    <row r="351" ht="14.25" hidden="1" customHeight="1">
       <c r="A351" s="4"/>
       <c r="B351" s="4"/>
       <c r="C351" s="4"/>
@@ -13434,7 +13434,7 @@
       <c r="Q351" s="4"/>
       <c r="R351" s="4"/>
     </row>
-    <row r="352" ht="14.25" customHeight="1">
+    <row r="352" ht="14.25" hidden="1" customHeight="1">
       <c r="A352" s="4"/>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -13454,7 +13454,7 @@
       <c r="Q352" s="4"/>
       <c r="R352" s="4"/>
     </row>
-    <row r="353" ht="14.25" customHeight="1">
+    <row r="353" ht="14.25" hidden="1" customHeight="1">
       <c r="A353" s="4"/>
       <c r="B353" s="4"/>
       <c r="C353" s="4"/>
@@ -13474,7 +13474,7 @@
       <c r="Q353" s="4"/>
       <c r="R353" s="4"/>
     </row>
-    <row r="354" ht="14.25" customHeight="1">
+    <row r="354" ht="14.25" hidden="1" customHeight="1">
       <c r="A354" s="4"/>
       <c r="B354" s="4"/>
       <c r="C354" s="4"/>
@@ -13494,7 +13494,7 @@
       <c r="Q354" s="4"/>
       <c r="R354" s="4"/>
     </row>
-    <row r="355" ht="14.25" customHeight="1">
+    <row r="355" ht="14.25" hidden="1" customHeight="1">
       <c r="A355" s="4"/>
       <c r="B355" s="4"/>
       <c r="C355" s="4"/>
@@ -13514,7 +13514,7 @@
       <c r="Q355" s="4"/>
       <c r="R355" s="4"/>
     </row>
-    <row r="356" ht="14.25" customHeight="1">
+    <row r="356" ht="14.25" hidden="1" customHeight="1">
       <c r="A356" s="4"/>
       <c r="B356" s="4"/>
       <c r="C356" s="4"/>
@@ -13534,7 +13534,7 @@
       <c r="Q356" s="4"/>
       <c r="R356" s="4"/>
     </row>
-    <row r="357" ht="14.25" customHeight="1">
+    <row r="357" ht="14.25" hidden="1" customHeight="1">
       <c r="A357" s="4"/>
       <c r="B357" s="4"/>
       <c r="C357" s="4"/>
@@ -13554,7 +13554,7 @@
       <c r="Q357" s="4"/>
       <c r="R357" s="4"/>
     </row>
-    <row r="358" ht="14.25" customHeight="1">
+    <row r="358" ht="14.25" hidden="1" customHeight="1">
       <c r="A358" s="4"/>
       <c r="B358" s="4"/>
       <c r="C358" s="4"/>
@@ -13574,7 +13574,7 @@
       <c r="Q358" s="4"/>
       <c r="R358" s="4"/>
     </row>
-    <row r="359" ht="14.25" customHeight="1">
+    <row r="359" ht="14.25" hidden="1" customHeight="1">
       <c r="A359" s="4"/>
       <c r="B359" s="4"/>
       <c r="C359" s="4"/>
@@ -13594,7 +13594,7 @@
       <c r="Q359" s="4"/>
       <c r="R359" s="4"/>
     </row>
-    <row r="360" ht="14.25" customHeight="1">
+    <row r="360" ht="14.25" hidden="1" customHeight="1">
       <c r="A360" s="4"/>
       <c r="B360" s="4"/>
       <c r="C360" s="4"/>
@@ -13614,7 +13614,7 @@
       <c r="Q360" s="4"/>
       <c r="R360" s="4"/>
     </row>
-    <row r="361" ht="14.25" customHeight="1">
+    <row r="361" ht="14.25" hidden="1" customHeight="1">
       <c r="A361" s="4"/>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
@@ -13634,7 +13634,7 @@
       <c r="Q361" s="4"/>
       <c r="R361" s="4"/>
     </row>
-    <row r="362" ht="14.25" customHeight="1">
+    <row r="362" ht="14.25" hidden="1" customHeight="1">
       <c r="A362" s="4"/>
       <c r="B362" s="4"/>
       <c r="C362" s="4"/>
@@ -13654,7 +13654,7 @@
       <c r="Q362" s="4"/>
       <c r="R362" s="4"/>
     </row>
-    <row r="363" ht="14.25" customHeight="1">
+    <row r="363" ht="14.25" hidden="1" customHeight="1">
       <c r="A363" s="4"/>
       <c r="B363" s="4"/>
       <c r="C363" s="4"/>
@@ -13674,7 +13674,7 @@
       <c r="Q363" s="4"/>
       <c r="R363" s="4"/>
     </row>
-    <row r="364" ht="14.25" customHeight="1">
+    <row r="364" ht="14.25" hidden="1" customHeight="1">
       <c r="A364" s="4"/>
       <c r="B364" s="4"/>
       <c r="C364" s="4"/>
@@ -13694,7 +13694,7 @@
       <c r="Q364" s="4"/>
       <c r="R364" s="4"/>
     </row>
-    <row r="365" ht="14.25" customHeight="1">
+    <row r="365" ht="14.25" hidden="1" customHeight="1">
       <c r="A365" s="4"/>
       <c r="B365" s="4"/>
       <c r="C365" s="4"/>
@@ -13714,7 +13714,7 @@
       <c r="Q365" s="4"/>
       <c r="R365" s="4"/>
     </row>
-    <row r="366" ht="14.25" customHeight="1">
+    <row r="366" ht="14.25" hidden="1" customHeight="1">
       <c r="A366" s="4"/>
       <c r="B366" s="4"/>
       <c r="C366" s="4"/>
@@ -31367,7 +31367,13 @@
       <c r="Z996" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$H$366"/>
+  <autoFilter ref="$A$1:$H$366">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Vazquez, Sebastian Ignacio"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Actualización automática - 2025-10-01 10:16
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -15,7 +15,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="ay9WolQA5uKxQqkrSyeHmwx059QVjAayQfPdRWDFzbI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="UgepXM4+o4zN/2W73SOBnJ05ynlfjcTKIvBl6ElTvIg="/>
     </ext>
   </extLst>
 </workbook>
@@ -1704,7 +1704,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1726,8 +1726,6 @@
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -19878,14 +19876,14 @@
       <c r="Z462" s="4"/>
     </row>
     <row r="463" ht="14.25" customHeight="1">
-      <c r="A463" s="5"/>
-      <c r="B463" s="8"/>
+      <c r="A463" s="4"/>
+      <c r="B463" s="4"/>
       <c r="C463" s="13"/>
-      <c r="D463" s="8"/>
-      <c r="E463" s="8"/>
-      <c r="F463" s="8"/>
-      <c r="G463" s="8"/>
-      <c r="H463" s="14"/>
+      <c r="D463" s="4"/>
+      <c r="E463" s="4"/>
+      <c r="F463" s="4"/>
+      <c r="G463" s="4"/>
+      <c r="H463" s="4"/>
       <c r="I463" s="4"/>
       <c r="J463" s="4"/>
       <c r="K463" s="4"/>
@@ -19906,14 +19904,14 @@
       <c r="Z463" s="4"/>
     </row>
     <row r="464" ht="14.25" customHeight="1">
-      <c r="A464" s="5"/>
-      <c r="B464" s="8"/>
+      <c r="A464" s="4"/>
+      <c r="B464" s="4"/>
       <c r="C464" s="13"/>
-      <c r="D464" s="8"/>
-      <c r="E464" s="8"/>
-      <c r="F464" s="8"/>
-      <c r="G464" s="8"/>
-      <c r="H464" s="14"/>
+      <c r="D464" s="4"/>
+      <c r="E464" s="4"/>
+      <c r="F464" s="4"/>
+      <c r="G464" s="4"/>
+      <c r="H464" s="4"/>
       <c r="I464" s="4"/>
       <c r="J464" s="4"/>
       <c r="K464" s="4"/>
@@ -19934,14 +19932,14 @@
       <c r="Z464" s="4"/>
     </row>
     <row r="465" ht="14.25" customHeight="1">
-      <c r="A465" s="5"/>
-      <c r="B465" s="8"/>
+      <c r="A465" s="4"/>
+      <c r="B465" s="4"/>
       <c r="C465" s="13"/>
-      <c r="D465" s="8"/>
-      <c r="E465" s="8"/>
-      <c r="F465" s="8"/>
-      <c r="G465" s="8"/>
-      <c r="H465" s="14"/>
+      <c r="D465" s="4"/>
+      <c r="E465" s="4"/>
+      <c r="F465" s="4"/>
+      <c r="G465" s="4"/>
+      <c r="H465" s="4"/>
       <c r="I465" s="4"/>
       <c r="J465" s="4"/>
       <c r="K465" s="4"/>
@@ -19964,12 +19962,12 @@
     <row r="466" ht="14.25" customHeight="1">
       <c r="A466" s="4"/>
       <c r="B466" s="4"/>
-      <c r="C466" s="6"/>
+      <c r="C466" s="13"/>
       <c r="D466" s="4"/>
       <c r="E466" s="4"/>
       <c r="F466" s="4"/>
       <c r="G466" s="4"/>
-      <c r="H466" s="7"/>
+      <c r="H466" s="4"/>
       <c r="I466" s="4"/>
       <c r="J466" s="4"/>
       <c r="K466" s="4"/>
@@ -19992,7 +19990,7 @@
     <row r="467" ht="14.25" customHeight="1">
       <c r="A467" s="4"/>
       <c r="B467" s="4"/>
-      <c r="C467" s="15"/>
+      <c r="C467" s="13"/>
       <c r="D467" s="4"/>
       <c r="E467" s="4"/>
       <c r="F467" s="4"/>
@@ -20020,7 +20018,7 @@
     <row r="468" ht="14.25" customHeight="1">
       <c r="A468" s="4"/>
       <c r="B468" s="4"/>
-      <c r="C468" s="15"/>
+      <c r="C468" s="13"/>
       <c r="D468" s="4"/>
       <c r="E468" s="4"/>
       <c r="F468" s="4"/>
@@ -20048,7 +20046,7 @@
     <row r="469" ht="14.25" customHeight="1">
       <c r="A469" s="4"/>
       <c r="B469" s="4"/>
-      <c r="C469" s="15"/>
+      <c r="C469" s="13"/>
       <c r="D469" s="4"/>
       <c r="E469" s="4"/>
       <c r="F469" s="4"/>
@@ -20076,7 +20074,7 @@
     <row r="470" ht="14.25" customHeight="1">
       <c r="A470" s="4"/>
       <c r="B470" s="4"/>
-      <c r="C470" s="15"/>
+      <c r="C470" s="13"/>
       <c r="D470" s="4"/>
       <c r="E470" s="4"/>
       <c r="F470" s="4"/>
@@ -20104,7 +20102,7 @@
     <row r="471" ht="14.25" customHeight="1">
       <c r="A471" s="4"/>
       <c r="B471" s="4"/>
-      <c r="C471" s="15"/>
+      <c r="C471" s="13"/>
       <c r="D471" s="4"/>
       <c r="E471" s="4"/>
       <c r="F471" s="4"/>
@@ -20132,7 +20130,7 @@
     <row r="472" ht="14.25" customHeight="1">
       <c r="A472" s="4"/>
       <c r="B472" s="4"/>
-      <c r="C472" s="15"/>
+      <c r="C472" s="13"/>
       <c r="D472" s="4"/>
       <c r="E472" s="4"/>
       <c r="F472" s="4"/>
@@ -20160,7 +20158,7 @@
     <row r="473" ht="14.25" customHeight="1">
       <c r="A473" s="4"/>
       <c r="B473" s="4"/>
-      <c r="C473" s="15"/>
+      <c r="C473" s="13"/>
       <c r="D473" s="4"/>
       <c r="E473" s="4"/>
       <c r="F473" s="4"/>
@@ -20188,7 +20186,7 @@
     <row r="474" ht="14.25" customHeight="1">
       <c r="A474" s="4"/>
       <c r="B474" s="4"/>
-      <c r="C474" s="15"/>
+      <c r="C474" s="13"/>
       <c r="D474" s="4"/>
       <c r="E474" s="4"/>
       <c r="F474" s="4"/>
@@ -20216,7 +20214,7 @@
     <row r="475" ht="14.25" customHeight="1">
       <c r="A475" s="4"/>
       <c r="B475" s="4"/>
-      <c r="C475" s="15"/>
+      <c r="C475" s="13"/>
       <c r="D475" s="4"/>
       <c r="E475" s="4"/>
       <c r="F475" s="4"/>
@@ -20244,7 +20242,7 @@
     <row r="476" ht="14.25" customHeight="1">
       <c r="A476" s="4"/>
       <c r="B476" s="4"/>
-      <c r="C476" s="15"/>
+      <c r="C476" s="13"/>
       <c r="D476" s="4"/>
       <c r="E476" s="4"/>
       <c r="F476" s="4"/>
@@ -20272,7 +20270,7 @@
     <row r="477" ht="14.25" customHeight="1">
       <c r="A477" s="4"/>
       <c r="B477" s="4"/>
-      <c r="C477" s="15"/>
+      <c r="C477" s="13"/>
       <c r="D477" s="4"/>
       <c r="E477" s="4"/>
       <c r="F477" s="4"/>
@@ -20300,7 +20298,7 @@
     <row r="478" ht="14.25" customHeight="1">
       <c r="A478" s="4"/>
       <c r="B478" s="4"/>
-      <c r="C478" s="15"/>
+      <c r="C478" s="13"/>
       <c r="D478" s="4"/>
       <c r="E478" s="4"/>
       <c r="F478" s="4"/>
@@ -20328,7 +20326,7 @@
     <row r="479" ht="14.25" customHeight="1">
       <c r="A479" s="4"/>
       <c r="B479" s="4"/>
-      <c r="C479" s="15"/>
+      <c r="C479" s="13"/>
       <c r="D479" s="4"/>
       <c r="E479" s="4"/>
       <c r="F479" s="4"/>
@@ -20356,7 +20354,7 @@
     <row r="480" ht="14.25" customHeight="1">
       <c r="A480" s="4"/>
       <c r="B480" s="4"/>
-      <c r="C480" s="15"/>
+      <c r="C480" s="13"/>
       <c r="D480" s="4"/>
       <c r="E480" s="4"/>
       <c r="F480" s="4"/>
@@ -20384,7 +20382,7 @@
     <row r="481" ht="14.25" customHeight="1">
       <c r="A481" s="4"/>
       <c r="B481" s="4"/>
-      <c r="C481" s="15"/>
+      <c r="C481" s="13"/>
       <c r="D481" s="4"/>
       <c r="E481" s="4"/>
       <c r="F481" s="4"/>
@@ -20412,7 +20410,7 @@
     <row r="482" ht="14.25" customHeight="1">
       <c r="A482" s="4"/>
       <c r="B482" s="4"/>
-      <c r="C482" s="15"/>
+      <c r="C482" s="13"/>
       <c r="D482" s="4"/>
       <c r="E482" s="4"/>
       <c r="F482" s="4"/>
@@ -20440,7 +20438,7 @@
     <row r="483" ht="14.25" customHeight="1">
       <c r="A483" s="4"/>
       <c r="B483" s="4"/>
-      <c r="C483" s="15"/>
+      <c r="C483" s="13"/>
       <c r="D483" s="4"/>
       <c r="E483" s="4"/>
       <c r="F483" s="4"/>
@@ -20468,7 +20466,7 @@
     <row r="484" ht="14.25" customHeight="1">
       <c r="A484" s="4"/>
       <c r="B484" s="4"/>
-      <c r="C484" s="15"/>
+      <c r="C484" s="13"/>
       <c r="D484" s="4"/>
       <c r="E484" s="4"/>
       <c r="F484" s="4"/>
@@ -20496,7 +20494,7 @@
     <row r="485" ht="14.25" customHeight="1">
       <c r="A485" s="4"/>
       <c r="B485" s="4"/>
-      <c r="C485" s="15"/>
+      <c r="C485" s="13"/>
       <c r="D485" s="4"/>
       <c r="E485" s="4"/>
       <c r="F485" s="4"/>
@@ -20524,7 +20522,7 @@
     <row r="486" ht="14.25" customHeight="1">
       <c r="A486" s="4"/>
       <c r="B486" s="4"/>
-      <c r="C486" s="15"/>
+      <c r="C486" s="13"/>
       <c r="D486" s="4"/>
       <c r="E486" s="4"/>
       <c r="F486" s="4"/>
@@ -20552,7 +20550,7 @@
     <row r="487" ht="14.25" customHeight="1">
       <c r="A487" s="4"/>
       <c r="B487" s="4"/>
-      <c r="C487" s="15"/>
+      <c r="C487" s="13"/>
       <c r="D487" s="4"/>
       <c r="E487" s="4"/>
       <c r="F487" s="4"/>
@@ -20580,7 +20578,7 @@
     <row r="488" ht="14.25" customHeight="1">
       <c r="A488" s="4"/>
       <c r="B488" s="4"/>
-      <c r="C488" s="15"/>
+      <c r="C488" s="13"/>
       <c r="D488" s="4"/>
       <c r="E488" s="4"/>
       <c r="F488" s="4"/>
@@ -20608,7 +20606,7 @@
     <row r="489" ht="14.25" customHeight="1">
       <c r="A489" s="4"/>
       <c r="B489" s="4"/>
-      <c r="C489" s="15"/>
+      <c r="C489" s="13"/>
       <c r="D489" s="4"/>
       <c r="E489" s="4"/>
       <c r="F489" s="4"/>
@@ -20636,7 +20634,7 @@
     <row r="490" ht="14.25" customHeight="1">
       <c r="A490" s="4"/>
       <c r="B490" s="4"/>
-      <c r="C490" s="15"/>
+      <c r="C490" s="13"/>
       <c r="D490" s="4"/>
       <c r="E490" s="4"/>
       <c r="F490" s="4"/>
@@ -20664,7 +20662,7 @@
     <row r="491" ht="14.25" customHeight="1">
       <c r="A491" s="4"/>
       <c r="B491" s="4"/>
-      <c r="C491" s="15"/>
+      <c r="C491" s="13"/>
       <c r="D491" s="4"/>
       <c r="E491" s="4"/>
       <c r="F491" s="4"/>
@@ -20692,7 +20690,7 @@
     <row r="492" ht="14.25" customHeight="1">
       <c r="A492" s="4"/>
       <c r="B492" s="4"/>
-      <c r="C492" s="15"/>
+      <c r="C492" s="13"/>
       <c r="D492" s="4"/>
       <c r="E492" s="4"/>
       <c r="F492" s="4"/>
@@ -20720,7 +20718,7 @@
     <row r="493" ht="14.25" customHeight="1">
       <c r="A493" s="4"/>
       <c r="B493" s="4"/>
-      <c r="C493" s="15"/>
+      <c r="C493" s="13"/>
       <c r="D493" s="4"/>
       <c r="E493" s="4"/>
       <c r="F493" s="4"/>
@@ -20748,7 +20746,7 @@
     <row r="494" ht="14.25" customHeight="1">
       <c r="A494" s="4"/>
       <c r="B494" s="4"/>
-      <c r="C494" s="15"/>
+      <c r="C494" s="13"/>
       <c r="D494" s="4"/>
       <c r="E494" s="4"/>
       <c r="F494" s="4"/>
@@ -20776,7 +20774,7 @@
     <row r="495" ht="14.25" customHeight="1">
       <c r="A495" s="4"/>
       <c r="B495" s="4"/>
-      <c r="C495" s="15"/>
+      <c r="C495" s="13"/>
       <c r="D495" s="4"/>
       <c r="E495" s="4"/>
       <c r="F495" s="4"/>
@@ -20804,7 +20802,7 @@
     <row r="496" ht="14.25" customHeight="1">
       <c r="A496" s="4"/>
       <c r="B496" s="4"/>
-      <c r="C496" s="15"/>
+      <c r="C496" s="13"/>
       <c r="D496" s="4"/>
       <c r="E496" s="4"/>
       <c r="F496" s="4"/>
@@ -20832,7 +20830,7 @@
     <row r="497" ht="14.25" customHeight="1">
       <c r="A497" s="4"/>
       <c r="B497" s="4"/>
-      <c r="C497" s="15"/>
+      <c r="C497" s="13"/>
       <c r="D497" s="4"/>
       <c r="E497" s="4"/>
       <c r="F497" s="4"/>
@@ -20860,7 +20858,7 @@
     <row r="498" ht="14.25" customHeight="1">
       <c r="A498" s="4"/>
       <c r="B498" s="4"/>
-      <c r="C498" s="15"/>
+      <c r="C498" s="13"/>
       <c r="D498" s="4"/>
       <c r="E498" s="4"/>
       <c r="F498" s="4"/>
@@ -20888,7 +20886,7 @@
     <row r="499" ht="14.25" customHeight="1">
       <c r="A499" s="4"/>
       <c r="B499" s="4"/>
-      <c r="C499" s="15"/>
+      <c r="C499" s="13"/>
       <c r="D499" s="4"/>
       <c r="E499" s="4"/>
       <c r="F499" s="4"/>
@@ -20916,7 +20914,7 @@
     <row r="500" ht="14.25" customHeight="1">
       <c r="A500" s="4"/>
       <c r="B500" s="4"/>
-      <c r="C500" s="15"/>
+      <c r="C500" s="13"/>
       <c r="D500" s="4"/>
       <c r="E500" s="4"/>
       <c r="F500" s="4"/>
@@ -20944,7 +20942,7 @@
     <row r="501" ht="14.25" customHeight="1">
       <c r="A501" s="4"/>
       <c r="B501" s="4"/>
-      <c r="C501" s="15"/>
+      <c r="C501" s="13"/>
       <c r="D501" s="4"/>
       <c r="E501" s="4"/>
       <c r="F501" s="4"/>
@@ -20972,7 +20970,7 @@
     <row r="502" ht="14.25" customHeight="1">
       <c r="A502" s="4"/>
       <c r="B502" s="4"/>
-      <c r="C502" s="15"/>
+      <c r="C502" s="13"/>
       <c r="D502" s="4"/>
       <c r="E502" s="4"/>
       <c r="F502" s="4"/>
@@ -21000,7 +20998,7 @@
     <row r="503" ht="14.25" customHeight="1">
       <c r="A503" s="4"/>
       <c r="B503" s="4"/>
-      <c r="C503" s="15"/>
+      <c r="C503" s="13"/>
       <c r="D503" s="4"/>
       <c r="E503" s="4"/>
       <c r="F503" s="4"/>
@@ -21028,7 +21026,7 @@
     <row r="504" ht="14.25" customHeight="1">
       <c r="A504" s="4"/>
       <c r="B504" s="4"/>
-      <c r="C504" s="15"/>
+      <c r="C504" s="13"/>
       <c r="D504" s="4"/>
       <c r="E504" s="4"/>
       <c r="F504" s="4"/>
@@ -21056,7 +21054,7 @@
     <row r="505" ht="14.25" customHeight="1">
       <c r="A505" s="4"/>
       <c r="B505" s="4"/>
-      <c r="C505" s="15"/>
+      <c r="C505" s="13"/>
       <c r="D505" s="4"/>
       <c r="E505" s="4"/>
       <c r="F505" s="4"/>
@@ -21084,7 +21082,7 @@
     <row r="506" ht="14.25" customHeight="1">
       <c r="A506" s="4"/>
       <c r="B506" s="4"/>
-      <c r="C506" s="15"/>
+      <c r="C506" s="13"/>
       <c r="D506" s="4"/>
       <c r="E506" s="4"/>
       <c r="F506" s="4"/>
@@ -21112,7 +21110,7 @@
     <row r="507" ht="14.25" customHeight="1">
       <c r="A507" s="4"/>
       <c r="B507" s="4"/>
-      <c r="C507" s="15"/>
+      <c r="C507" s="13"/>
       <c r="D507" s="4"/>
       <c r="E507" s="4"/>
       <c r="F507" s="4"/>
@@ -21140,7 +21138,7 @@
     <row r="508" ht="14.25" customHeight="1">
       <c r="A508" s="4"/>
       <c r="B508" s="4"/>
-      <c r="C508" s="15"/>
+      <c r="C508" s="13"/>
       <c r="D508" s="4"/>
       <c r="E508" s="4"/>
       <c r="F508" s="4"/>
@@ -21168,7 +21166,7 @@
     <row r="509" ht="14.25" customHeight="1">
       <c r="A509" s="4"/>
       <c r="B509" s="4"/>
-      <c r="C509" s="15"/>
+      <c r="C509" s="13"/>
       <c r="D509" s="4"/>
       <c r="E509" s="4"/>
       <c r="F509" s="4"/>
@@ -21196,7 +21194,7 @@
     <row r="510" ht="14.25" customHeight="1">
       <c r="A510" s="4"/>
       <c r="B510" s="4"/>
-      <c r="C510" s="15"/>
+      <c r="C510" s="13"/>
       <c r="D510" s="4"/>
       <c r="E510" s="4"/>
       <c r="F510" s="4"/>
@@ -21224,7 +21222,7 @@
     <row r="511" ht="14.25" customHeight="1">
       <c r="A511" s="4"/>
       <c r="B511" s="4"/>
-      <c r="C511" s="15"/>
+      <c r="C511" s="13"/>
       <c r="D511" s="4"/>
       <c r="E511" s="4"/>
       <c r="F511" s="4"/>
@@ -21252,7 +21250,7 @@
     <row r="512" ht="14.25" customHeight="1">
       <c r="A512" s="4"/>
       <c r="B512" s="4"/>
-      <c r="C512" s="15"/>
+      <c r="C512" s="13"/>
       <c r="D512" s="4"/>
       <c r="E512" s="4"/>
       <c r="F512" s="4"/>
@@ -21280,7 +21278,7 @@
     <row r="513" ht="14.25" customHeight="1">
       <c r="A513" s="4"/>
       <c r="B513" s="4"/>
-      <c r="C513" s="15"/>
+      <c r="C513" s="13"/>
       <c r="D513" s="4"/>
       <c r="E513" s="4"/>
       <c r="F513" s="4"/>
@@ -21308,7 +21306,7 @@
     <row r="514" ht="14.25" customHeight="1">
       <c r="A514" s="4"/>
       <c r="B514" s="4"/>
-      <c r="C514" s="15"/>
+      <c r="C514" s="13"/>
       <c r="D514" s="4"/>
       <c r="E514" s="4"/>
       <c r="F514" s="4"/>
@@ -21336,7 +21334,7 @@
     <row r="515" ht="14.25" customHeight="1">
       <c r="A515" s="4"/>
       <c r="B515" s="4"/>
-      <c r="C515" s="15"/>
+      <c r="C515" s="13"/>
       <c r="D515" s="4"/>
       <c r="E515" s="4"/>
       <c r="F515" s="4"/>
@@ -21364,7 +21362,7 @@
     <row r="516" ht="14.25" customHeight="1">
       <c r="A516" s="4"/>
       <c r="B516" s="4"/>
-      <c r="C516" s="15"/>
+      <c r="C516" s="13"/>
       <c r="D516" s="4"/>
       <c r="E516" s="4"/>
       <c r="F516" s="4"/>
@@ -21392,7 +21390,7 @@
     <row r="517" ht="14.25" customHeight="1">
       <c r="A517" s="4"/>
       <c r="B517" s="4"/>
-      <c r="C517" s="15"/>
+      <c r="C517" s="13"/>
       <c r="D517" s="4"/>
       <c r="E517" s="4"/>
       <c r="F517" s="4"/>
@@ -21420,7 +21418,7 @@
     <row r="518" ht="14.25" customHeight="1">
       <c r="A518" s="4"/>
       <c r="B518" s="4"/>
-      <c r="C518" s="15"/>
+      <c r="C518" s="13"/>
       <c r="D518" s="4"/>
       <c r="E518" s="4"/>
       <c r="F518" s="4"/>
@@ -21448,7 +21446,7 @@
     <row r="519" ht="14.25" customHeight="1">
       <c r="A519" s="4"/>
       <c r="B519" s="4"/>
-      <c r="C519" s="15"/>
+      <c r="C519" s="13"/>
       <c r="D519" s="4"/>
       <c r="E519" s="4"/>
       <c r="F519" s="4"/>
@@ -21476,7 +21474,7 @@
     <row r="520" ht="14.25" customHeight="1">
       <c r="A520" s="4"/>
       <c r="B520" s="4"/>
-      <c r="C520" s="15"/>
+      <c r="C520" s="13"/>
       <c r="D520" s="4"/>
       <c r="E520" s="4"/>
       <c r="F520" s="4"/>
@@ -21504,7 +21502,7 @@
     <row r="521" ht="14.25" customHeight="1">
       <c r="A521" s="4"/>
       <c r="B521" s="4"/>
-      <c r="C521" s="15"/>
+      <c r="C521" s="13"/>
       <c r="D521" s="4"/>
       <c r="E521" s="4"/>
       <c r="F521" s="4"/>
@@ -21532,7 +21530,7 @@
     <row r="522" ht="14.25" customHeight="1">
       <c r="A522" s="4"/>
       <c r="B522" s="4"/>
-      <c r="C522" s="15"/>
+      <c r="C522" s="13"/>
       <c r="D522" s="4"/>
       <c r="E522" s="4"/>
       <c r="F522" s="4"/>
@@ -21560,7 +21558,7 @@
     <row r="523" ht="14.25" customHeight="1">
       <c r="A523" s="4"/>
       <c r="B523" s="4"/>
-      <c r="C523" s="15"/>
+      <c r="C523" s="13"/>
       <c r="D523" s="4"/>
       <c r="E523" s="4"/>
       <c r="F523" s="4"/>
@@ -21588,7 +21586,7 @@
     <row r="524" ht="14.25" customHeight="1">
       <c r="A524" s="4"/>
       <c r="B524" s="4"/>
-      <c r="C524" s="15"/>
+      <c r="C524" s="13"/>
       <c r="D524" s="4"/>
       <c r="E524" s="4"/>
       <c r="F524" s="4"/>
@@ -21616,7 +21614,7 @@
     <row r="525" ht="14.25" customHeight="1">
       <c r="A525" s="4"/>
       <c r="B525" s="4"/>
-      <c r="C525" s="15"/>
+      <c r="C525" s="13"/>
       <c r="D525" s="4"/>
       <c r="E525" s="4"/>
       <c r="F525" s="4"/>
@@ -21644,7 +21642,7 @@
     <row r="526" ht="14.25" customHeight="1">
       <c r="A526" s="4"/>
       <c r="B526" s="4"/>
-      <c r="C526" s="15"/>
+      <c r="C526" s="13"/>
       <c r="D526" s="4"/>
       <c r="E526" s="4"/>
       <c r="F526" s="4"/>
@@ -21672,7 +21670,7 @@
     <row r="527" ht="14.25" customHeight="1">
       <c r="A527" s="4"/>
       <c r="B527" s="4"/>
-      <c r="C527" s="15"/>
+      <c r="C527" s="13"/>
       <c r="D527" s="4"/>
       <c r="E527" s="4"/>
       <c r="F527" s="4"/>
@@ -21700,7 +21698,7 @@
     <row r="528" ht="14.25" customHeight="1">
       <c r="A528" s="4"/>
       <c r="B528" s="4"/>
-      <c r="C528" s="15"/>
+      <c r="C528" s="13"/>
       <c r="D528" s="4"/>
       <c r="E528" s="4"/>
       <c r="F528" s="4"/>
@@ -21728,7 +21726,7 @@
     <row r="529" ht="14.25" customHeight="1">
       <c r="A529" s="4"/>
       <c r="B529" s="4"/>
-      <c r="C529" s="15"/>
+      <c r="C529" s="13"/>
       <c r="D529" s="4"/>
       <c r="E529" s="4"/>
       <c r="F529" s="4"/>
@@ -21756,7 +21754,7 @@
     <row r="530" ht="14.25" customHeight="1">
       <c r="A530" s="4"/>
       <c r="B530" s="4"/>
-      <c r="C530" s="15"/>
+      <c r="C530" s="13"/>
       <c r="D530" s="4"/>
       <c r="E530" s="4"/>
       <c r="F530" s="4"/>
@@ -21784,7 +21782,7 @@
     <row r="531" ht="14.25" customHeight="1">
       <c r="A531" s="4"/>
       <c r="B531" s="4"/>
-      <c r="C531" s="15"/>
+      <c r="C531" s="13"/>
       <c r="D531" s="4"/>
       <c r="E531" s="4"/>
       <c r="F531" s="4"/>
@@ -21812,7 +21810,7 @@
     <row r="532" ht="14.25" customHeight="1">
       <c r="A532" s="4"/>
       <c r="B532" s="4"/>
-      <c r="C532" s="15"/>
+      <c r="C532" s="13"/>
       <c r="D532" s="4"/>
       <c r="E532" s="4"/>
       <c r="F532" s="4"/>
@@ -21840,7 +21838,7 @@
     <row r="533" ht="14.25" customHeight="1">
       <c r="A533" s="4"/>
       <c r="B533" s="4"/>
-      <c r="C533" s="15"/>
+      <c r="C533" s="13"/>
       <c r="D533" s="4"/>
       <c r="E533" s="4"/>
       <c r="F533" s="4"/>
@@ -21868,7 +21866,7 @@
     <row r="534" ht="14.25" customHeight="1">
       <c r="A534" s="4"/>
       <c r="B534" s="4"/>
-      <c r="C534" s="15"/>
+      <c r="C534" s="13"/>
       <c r="D534" s="4"/>
       <c r="E534" s="4"/>
       <c r="F534" s="4"/>
@@ -21896,7 +21894,7 @@
     <row r="535" ht="14.25" customHeight="1">
       <c r="A535" s="4"/>
       <c r="B535" s="4"/>
-      <c r="C535" s="15"/>
+      <c r="C535" s="13"/>
       <c r="D535" s="4"/>
       <c r="E535" s="4"/>
       <c r="F535" s="4"/>
@@ -21924,7 +21922,7 @@
     <row r="536" ht="14.25" customHeight="1">
       <c r="A536" s="4"/>
       <c r="B536" s="4"/>
-      <c r="C536" s="15"/>
+      <c r="C536" s="13"/>
       <c r="D536" s="4"/>
       <c r="E536" s="4"/>
       <c r="F536" s="4"/>
@@ -21952,7 +21950,7 @@
     <row r="537" ht="14.25" customHeight="1">
       <c r="A537" s="4"/>
       <c r="B537" s="4"/>
-      <c r="C537" s="15"/>
+      <c r="C537" s="13"/>
       <c r="D537" s="4"/>
       <c r="E537" s="4"/>
       <c r="F537" s="4"/>
@@ -21980,7 +21978,7 @@
     <row r="538" ht="14.25" customHeight="1">
       <c r="A538" s="4"/>
       <c r="B538" s="4"/>
-      <c r="C538" s="15"/>
+      <c r="C538" s="13"/>
       <c r="D538" s="4"/>
       <c r="E538" s="4"/>
       <c r="F538" s="4"/>
@@ -22008,7 +22006,7 @@
     <row r="539" ht="14.25" customHeight="1">
       <c r="A539" s="4"/>
       <c r="B539" s="4"/>
-      <c r="C539" s="15"/>
+      <c r="C539" s="13"/>
       <c r="D539" s="4"/>
       <c r="E539" s="4"/>
       <c r="F539" s="4"/>
@@ -22036,7 +22034,7 @@
     <row r="540" ht="14.25" customHeight="1">
       <c r="A540" s="4"/>
       <c r="B540" s="4"/>
-      <c r="C540" s="15"/>
+      <c r="C540" s="13"/>
       <c r="D540" s="4"/>
       <c r="E540" s="4"/>
       <c r="F540" s="4"/>
@@ -22064,7 +22062,7 @@
     <row r="541" ht="14.25" customHeight="1">
       <c r="A541" s="4"/>
       <c r="B541" s="4"/>
-      <c r="C541" s="15"/>
+      <c r="C541" s="13"/>
       <c r="D541" s="4"/>
       <c r="E541" s="4"/>
       <c r="F541" s="4"/>
@@ -22092,7 +22090,7 @@
     <row r="542" ht="14.25" customHeight="1">
       <c r="A542" s="4"/>
       <c r="B542" s="4"/>
-      <c r="C542" s="15"/>
+      <c r="C542" s="13"/>
       <c r="D542" s="4"/>
       <c r="E542" s="4"/>
       <c r="F542" s="4"/>
@@ -22120,7 +22118,7 @@
     <row r="543" ht="14.25" customHeight="1">
       <c r="A543" s="4"/>
       <c r="B543" s="4"/>
-      <c r="C543" s="15"/>
+      <c r="C543" s="13"/>
       <c r="D543" s="4"/>
       <c r="E543" s="4"/>
       <c r="F543" s="4"/>
@@ -22148,7 +22146,7 @@
     <row r="544" ht="14.25" customHeight="1">
       <c r="A544" s="4"/>
       <c r="B544" s="4"/>
-      <c r="C544" s="15"/>
+      <c r="C544" s="13"/>
       <c r="D544" s="4"/>
       <c r="E544" s="4"/>
       <c r="F544" s="4"/>
@@ -22176,7 +22174,7 @@
     <row r="545" ht="14.25" customHeight="1">
       <c r="A545" s="4"/>
       <c r="B545" s="4"/>
-      <c r="C545" s="15"/>
+      <c r="C545" s="13"/>
       <c r="D545" s="4"/>
       <c r="E545" s="4"/>
       <c r="F545" s="4"/>
@@ -22204,7 +22202,7 @@
     <row r="546" ht="14.25" customHeight="1">
       <c r="A546" s="4"/>
       <c r="B546" s="4"/>
-      <c r="C546" s="15"/>
+      <c r="C546" s="13"/>
       <c r="D546" s="4"/>
       <c r="E546" s="4"/>
       <c r="F546" s="4"/>
@@ -22232,7 +22230,7 @@
     <row r="547" ht="14.25" customHeight="1">
       <c r="A547" s="4"/>
       <c r="B547" s="4"/>
-      <c r="C547" s="15"/>
+      <c r="C547" s="13"/>
       <c r="D547" s="4"/>
       <c r="E547" s="4"/>
       <c r="F547" s="4"/>
@@ -22260,7 +22258,7 @@
     <row r="548" ht="14.25" customHeight="1">
       <c r="A548" s="4"/>
       <c r="B548" s="4"/>
-      <c r="C548" s="15"/>
+      <c r="C548" s="13"/>
       <c r="D548" s="4"/>
       <c r="E548" s="4"/>
       <c r="F548" s="4"/>
@@ -22288,7 +22286,7 @@
     <row r="549" ht="14.25" customHeight="1">
       <c r="A549" s="4"/>
       <c r="B549" s="4"/>
-      <c r="C549" s="15"/>
+      <c r="C549" s="13"/>
       <c r="D549" s="4"/>
       <c r="E549" s="4"/>
       <c r="F549" s="4"/>
@@ -22316,7 +22314,7 @@
     <row r="550" ht="14.25" customHeight="1">
       <c r="A550" s="4"/>
       <c r="B550" s="4"/>
-      <c r="C550" s="15"/>
+      <c r="C550" s="13"/>
       <c r="D550" s="4"/>
       <c r="E550" s="4"/>
       <c r="F550" s="4"/>
@@ -22344,7 +22342,7 @@
     <row r="551" ht="14.25" customHeight="1">
       <c r="A551" s="4"/>
       <c r="B551" s="4"/>
-      <c r="C551" s="15"/>
+      <c r="C551" s="13"/>
       <c r="D551" s="4"/>
       <c r="E551" s="4"/>
       <c r="F551" s="4"/>
@@ -22372,7 +22370,7 @@
     <row r="552" ht="14.25" customHeight="1">
       <c r="A552" s="4"/>
       <c r="B552" s="4"/>
-      <c r="C552" s="15"/>
+      <c r="C552" s="13"/>
       <c r="D552" s="4"/>
       <c r="E552" s="4"/>
       <c r="F552" s="4"/>
@@ -22400,7 +22398,7 @@
     <row r="553" ht="14.25" customHeight="1">
       <c r="A553" s="4"/>
       <c r="B553" s="4"/>
-      <c r="C553" s="15"/>
+      <c r="C553" s="13"/>
       <c r="D553" s="4"/>
       <c r="E553" s="4"/>
       <c r="F553" s="4"/>
@@ -22428,7 +22426,7 @@
     <row r="554" ht="14.25" customHeight="1">
       <c r="A554" s="4"/>
       <c r="B554" s="4"/>
-      <c r="C554" s="15"/>
+      <c r="C554" s="13"/>
       <c r="D554" s="4"/>
       <c r="E554" s="4"/>
       <c r="F554" s="4"/>
@@ -22456,7 +22454,7 @@
     <row r="555" ht="14.25" customHeight="1">
       <c r="A555" s="4"/>
       <c r="B555" s="4"/>
-      <c r="C555" s="15"/>
+      <c r="C555" s="13"/>
       <c r="D555" s="4"/>
       <c r="E555" s="4"/>
       <c r="F555" s="4"/>
@@ -22484,7 +22482,7 @@
     <row r="556" ht="14.25" customHeight="1">
       <c r="A556" s="4"/>
       <c r="B556" s="4"/>
-      <c r="C556" s="15"/>
+      <c r="C556" s="13"/>
       <c r="D556" s="4"/>
       <c r="E556" s="4"/>
       <c r="F556" s="4"/>
@@ -22512,7 +22510,7 @@
     <row r="557" ht="14.25" customHeight="1">
       <c r="A557" s="4"/>
       <c r="B557" s="4"/>
-      <c r="C557" s="15"/>
+      <c r="C557" s="13"/>
       <c r="D557" s="4"/>
       <c r="E557" s="4"/>
       <c r="F557" s="4"/>
@@ -22540,7 +22538,7 @@
     <row r="558" ht="14.25" customHeight="1">
       <c r="A558" s="4"/>
       <c r="B558" s="4"/>
-      <c r="C558" s="15"/>
+      <c r="C558" s="13"/>
       <c r="D558" s="4"/>
       <c r="E558" s="4"/>
       <c r="F558" s="4"/>
@@ -22568,7 +22566,7 @@
     <row r="559" ht="14.25" customHeight="1">
       <c r="A559" s="4"/>
       <c r="B559" s="4"/>
-      <c r="C559" s="15"/>
+      <c r="C559" s="13"/>
       <c r="D559" s="4"/>
       <c r="E559" s="4"/>
       <c r="F559" s="4"/>
@@ -22596,7 +22594,7 @@
     <row r="560" ht="14.25" customHeight="1">
       <c r="A560" s="4"/>
       <c r="B560" s="4"/>
-      <c r="C560" s="15"/>
+      <c r="C560" s="13"/>
       <c r="D560" s="4"/>
       <c r="E560" s="4"/>
       <c r="F560" s="4"/>
@@ -22624,7 +22622,7 @@
     <row r="561" ht="14.25" customHeight="1">
       <c r="A561" s="4"/>
       <c r="B561" s="4"/>
-      <c r="C561" s="15"/>
+      <c r="C561" s="13"/>
       <c r="D561" s="4"/>
       <c r="E561" s="4"/>
       <c r="F561" s="4"/>
@@ -22652,7 +22650,7 @@
     <row r="562" ht="14.25" customHeight="1">
       <c r="A562" s="4"/>
       <c r="B562" s="4"/>
-      <c r="C562" s="15"/>
+      <c r="C562" s="13"/>
       <c r="D562" s="4"/>
       <c r="E562" s="4"/>
       <c r="F562" s="4"/>
@@ -22680,7 +22678,7 @@
     <row r="563" ht="14.25" customHeight="1">
       <c r="A563" s="4"/>
       <c r="B563" s="4"/>
-      <c r="C563" s="15"/>
+      <c r="C563" s="13"/>
       <c r="D563" s="4"/>
       <c r="E563" s="4"/>
       <c r="F563" s="4"/>
@@ -22708,7 +22706,7 @@
     <row r="564" ht="14.25" customHeight="1">
       <c r="A564" s="4"/>
       <c r="B564" s="4"/>
-      <c r="C564" s="15"/>
+      <c r="C564" s="13"/>
       <c r="D564" s="4"/>
       <c r="E564" s="4"/>
       <c r="F564" s="4"/>
@@ -22736,7 +22734,7 @@
     <row r="565" ht="14.25" customHeight="1">
       <c r="A565" s="4"/>
       <c r="B565" s="4"/>
-      <c r="C565" s="15"/>
+      <c r="C565" s="13"/>
       <c r="D565" s="4"/>
       <c r="E565" s="4"/>
       <c r="F565" s="4"/>
@@ -22764,7 +22762,7 @@
     <row r="566" ht="14.25" customHeight="1">
       <c r="A566" s="4"/>
       <c r="B566" s="4"/>
-      <c r="C566" s="15"/>
+      <c r="C566" s="13"/>
       <c r="D566" s="4"/>
       <c r="E566" s="4"/>
       <c r="F566" s="4"/>
@@ -22792,7 +22790,7 @@
     <row r="567" ht="14.25" customHeight="1">
       <c r="A567" s="4"/>
       <c r="B567" s="4"/>
-      <c r="C567" s="15"/>
+      <c r="C567" s="13"/>
       <c r="D567" s="4"/>
       <c r="E567" s="4"/>
       <c r="F567" s="4"/>
@@ -22820,7 +22818,7 @@
     <row r="568" ht="14.25" customHeight="1">
       <c r="A568" s="4"/>
       <c r="B568" s="4"/>
-      <c r="C568" s="15"/>
+      <c r="C568" s="13"/>
       <c r="D568" s="4"/>
       <c r="E568" s="4"/>
       <c r="F568" s="4"/>
@@ -22848,7 +22846,7 @@
     <row r="569" ht="14.25" customHeight="1">
       <c r="A569" s="4"/>
       <c r="B569" s="4"/>
-      <c r="C569" s="15"/>
+      <c r="C569" s="13"/>
       <c r="D569" s="4"/>
       <c r="E569" s="4"/>
       <c r="F569" s="4"/>
@@ -22876,7 +22874,7 @@
     <row r="570" ht="14.25" customHeight="1">
       <c r="A570" s="4"/>
       <c r="B570" s="4"/>
-      <c r="C570" s="15"/>
+      <c r="C570" s="13"/>
       <c r="D570" s="4"/>
       <c r="E570" s="4"/>
       <c r="F570" s="4"/>
@@ -22904,7 +22902,7 @@
     <row r="571" ht="14.25" customHeight="1">
       <c r="A571" s="4"/>
       <c r="B571" s="4"/>
-      <c r="C571" s="15"/>
+      <c r="C571" s="13"/>
       <c r="D571" s="4"/>
       <c r="E571" s="4"/>
       <c r="F571" s="4"/>
@@ -22932,7 +22930,7 @@
     <row r="572" ht="14.25" customHeight="1">
       <c r="A572" s="4"/>
       <c r="B572" s="4"/>
-      <c r="C572" s="15"/>
+      <c r="C572" s="13"/>
       <c r="D572" s="4"/>
       <c r="E572" s="4"/>
       <c r="F572" s="4"/>
@@ -22960,7 +22958,7 @@
     <row r="573" ht="14.25" customHeight="1">
       <c r="A573" s="4"/>
       <c r="B573" s="4"/>
-      <c r="C573" s="15"/>
+      <c r="C573" s="13"/>
       <c r="D573" s="4"/>
       <c r="E573" s="4"/>
       <c r="F573" s="4"/>
@@ -22988,7 +22986,7 @@
     <row r="574" ht="14.25" customHeight="1">
       <c r="A574" s="4"/>
       <c r="B574" s="4"/>
-      <c r="C574" s="15"/>
+      <c r="C574" s="13"/>
       <c r="D574" s="4"/>
       <c r="E574" s="4"/>
       <c r="F574" s="4"/>
@@ -23016,7 +23014,7 @@
     <row r="575" ht="14.25" customHeight="1">
       <c r="A575" s="4"/>
       <c r="B575" s="4"/>
-      <c r="C575" s="15"/>
+      <c r="C575" s="13"/>
       <c r="D575" s="4"/>
       <c r="E575" s="4"/>
       <c r="F575" s="4"/>
@@ -23044,7 +23042,7 @@
     <row r="576" ht="14.25" customHeight="1">
       <c r="A576" s="4"/>
       <c r="B576" s="4"/>
-      <c r="C576" s="15"/>
+      <c r="C576" s="13"/>
       <c r="D576" s="4"/>
       <c r="E576" s="4"/>
       <c r="F576" s="4"/>
@@ -23072,7 +23070,7 @@
     <row r="577" ht="14.25" customHeight="1">
       <c r="A577" s="4"/>
       <c r="B577" s="4"/>
-      <c r="C577" s="15"/>
+      <c r="C577" s="13"/>
       <c r="D577" s="4"/>
       <c r="E577" s="4"/>
       <c r="F577" s="4"/>
@@ -23100,7 +23098,7 @@
     <row r="578" ht="14.25" customHeight="1">
       <c r="A578" s="4"/>
       <c r="B578" s="4"/>
-      <c r="C578" s="15"/>
+      <c r="C578" s="13"/>
       <c r="D578" s="4"/>
       <c r="E578" s="4"/>
       <c r="F578" s="4"/>
@@ -23128,7 +23126,7 @@
     <row r="579" ht="14.25" customHeight="1">
       <c r="A579" s="4"/>
       <c r="B579" s="4"/>
-      <c r="C579" s="15"/>
+      <c r="C579" s="13"/>
       <c r="D579" s="4"/>
       <c r="E579" s="4"/>
       <c r="F579" s="4"/>
@@ -23156,7 +23154,7 @@
     <row r="580" ht="14.25" customHeight="1">
       <c r="A580" s="4"/>
       <c r="B580" s="4"/>
-      <c r="C580" s="15"/>
+      <c r="C580" s="13"/>
       <c r="D580" s="4"/>
       <c r="E580" s="4"/>
       <c r="F580" s="4"/>
@@ -23184,7 +23182,7 @@
     <row r="581" ht="14.25" customHeight="1">
       <c r="A581" s="4"/>
       <c r="B581" s="4"/>
-      <c r="C581" s="15"/>
+      <c r="C581" s="13"/>
       <c r="D581" s="4"/>
       <c r="E581" s="4"/>
       <c r="F581" s="4"/>
@@ -23212,7 +23210,7 @@
     <row r="582" ht="14.25" customHeight="1">
       <c r="A582" s="4"/>
       <c r="B582" s="4"/>
-      <c r="C582" s="15"/>
+      <c r="C582" s="13"/>
       <c r="D582" s="4"/>
       <c r="E582" s="4"/>
       <c r="F582" s="4"/>
@@ -23240,7 +23238,7 @@
     <row r="583" ht="14.25" customHeight="1">
       <c r="A583" s="4"/>
       <c r="B583" s="4"/>
-      <c r="C583" s="15"/>
+      <c r="C583" s="13"/>
       <c r="D583" s="4"/>
       <c r="E583" s="4"/>
       <c r="F583" s="4"/>
@@ -23268,7 +23266,7 @@
     <row r="584" ht="14.25" customHeight="1">
       <c r="A584" s="4"/>
       <c r="B584" s="4"/>
-      <c r="C584" s="15"/>
+      <c r="C584" s="13"/>
       <c r="D584" s="4"/>
       <c r="E584" s="4"/>
       <c r="F584" s="4"/>
@@ -23296,7 +23294,7 @@
     <row r="585" ht="14.25" customHeight="1">
       <c r="A585" s="4"/>
       <c r="B585" s="4"/>
-      <c r="C585" s="15"/>
+      <c r="C585" s="13"/>
       <c r="D585" s="4"/>
       <c r="E585" s="4"/>
       <c r="F585" s="4"/>
@@ -23324,7 +23322,7 @@
     <row r="586" ht="14.25" customHeight="1">
       <c r="A586" s="4"/>
       <c r="B586" s="4"/>
-      <c r="C586" s="15"/>
+      <c r="C586" s="13"/>
       <c r="D586" s="4"/>
       <c r="E586" s="4"/>
       <c r="F586" s="4"/>
@@ -23352,7 +23350,7 @@
     <row r="587" ht="14.25" customHeight="1">
       <c r="A587" s="4"/>
       <c r="B587" s="4"/>
-      <c r="C587" s="15"/>
+      <c r="C587" s="13"/>
       <c r="D587" s="4"/>
       <c r="E587" s="4"/>
       <c r="F587" s="4"/>
@@ -23380,7 +23378,7 @@
     <row r="588" ht="14.25" customHeight="1">
       <c r="A588" s="4"/>
       <c r="B588" s="4"/>
-      <c r="C588" s="15"/>
+      <c r="C588" s="13"/>
       <c r="D588" s="4"/>
       <c r="E588" s="4"/>
       <c r="F588" s="4"/>
@@ -23408,7 +23406,7 @@
     <row r="589" ht="14.25" customHeight="1">
       <c r="A589" s="4"/>
       <c r="B589" s="4"/>
-      <c r="C589" s="15"/>
+      <c r="C589" s="13"/>
       <c r="D589" s="4"/>
       <c r="E589" s="4"/>
       <c r="F589" s="4"/>
@@ -23436,7 +23434,7 @@
     <row r="590" ht="14.25" customHeight="1">
       <c r="A590" s="4"/>
       <c r="B590" s="4"/>
-      <c r="C590" s="15"/>
+      <c r="C590" s="13"/>
       <c r="D590" s="4"/>
       <c r="E590" s="4"/>
       <c r="F590" s="4"/>
@@ -23464,7 +23462,7 @@
     <row r="591" ht="14.25" customHeight="1">
       <c r="A591" s="4"/>
       <c r="B591" s="4"/>
-      <c r="C591" s="15"/>
+      <c r="C591" s="13"/>
       <c r="D591" s="4"/>
       <c r="E591" s="4"/>
       <c r="F591" s="4"/>
@@ -23492,7 +23490,7 @@
     <row r="592" ht="14.25" customHeight="1">
       <c r="A592" s="4"/>
       <c r="B592" s="4"/>
-      <c r="C592" s="15"/>
+      <c r="C592" s="13"/>
       <c r="D592" s="4"/>
       <c r="E592" s="4"/>
       <c r="F592" s="4"/>
@@ -23520,7 +23518,7 @@
     <row r="593" ht="14.25" customHeight="1">
       <c r="A593" s="4"/>
       <c r="B593" s="4"/>
-      <c r="C593" s="15"/>
+      <c r="C593" s="13"/>
       <c r="D593" s="4"/>
       <c r="E593" s="4"/>
       <c r="F593" s="4"/>
@@ -23548,7 +23546,7 @@
     <row r="594" ht="14.25" customHeight="1">
       <c r="A594" s="4"/>
       <c r="B594" s="4"/>
-      <c r="C594" s="15"/>
+      <c r="C594" s="13"/>
       <c r="D594" s="4"/>
       <c r="E594" s="4"/>
       <c r="F594" s="4"/>
@@ -23576,7 +23574,7 @@
     <row r="595" ht="14.25" customHeight="1">
       <c r="A595" s="4"/>
       <c r="B595" s="4"/>
-      <c r="C595" s="15"/>
+      <c r="C595" s="13"/>
       <c r="D595" s="4"/>
       <c r="E595" s="4"/>
       <c r="F595" s="4"/>
@@ -23604,7 +23602,7 @@
     <row r="596" ht="14.25" customHeight="1">
       <c r="A596" s="4"/>
       <c r="B596" s="4"/>
-      <c r="C596" s="15"/>
+      <c r="C596" s="13"/>
       <c r="D596" s="4"/>
       <c r="E596" s="4"/>
       <c r="F596" s="4"/>
@@ -23632,7 +23630,7 @@
     <row r="597" ht="14.25" customHeight="1">
       <c r="A597" s="4"/>
       <c r="B597" s="4"/>
-      <c r="C597" s="15"/>
+      <c r="C597" s="13"/>
       <c r="D597" s="4"/>
       <c r="E597" s="4"/>
       <c r="F597" s="4"/>
@@ -23660,7 +23658,7 @@
     <row r="598" ht="14.25" customHeight="1">
       <c r="A598" s="4"/>
       <c r="B598" s="4"/>
-      <c r="C598" s="15"/>
+      <c r="C598" s="13"/>
       <c r="D598" s="4"/>
       <c r="E598" s="4"/>
       <c r="F598" s="4"/>
@@ -23688,7 +23686,7 @@
     <row r="599" ht="14.25" customHeight="1">
       <c r="A599" s="4"/>
       <c r="B599" s="4"/>
-      <c r="C599" s="15"/>
+      <c r="C599" s="13"/>
       <c r="D599" s="4"/>
       <c r="E599" s="4"/>
       <c r="F599" s="4"/>
@@ -23716,7 +23714,7 @@
     <row r="600" ht="14.25" customHeight="1">
       <c r="A600" s="4"/>
       <c r="B600" s="4"/>
-      <c r="C600" s="15"/>
+      <c r="C600" s="13"/>
       <c r="D600" s="4"/>
       <c r="E600" s="4"/>
       <c r="F600" s="4"/>
@@ -23744,7 +23742,7 @@
     <row r="601" ht="14.25" customHeight="1">
       <c r="A601" s="4"/>
       <c r="B601" s="4"/>
-      <c r="C601" s="15"/>
+      <c r="C601" s="13"/>
       <c r="D601" s="4"/>
       <c r="E601" s="4"/>
       <c r="F601" s="4"/>
@@ -23772,7 +23770,7 @@
     <row r="602" ht="14.25" customHeight="1">
       <c r="A602" s="4"/>
       <c r="B602" s="4"/>
-      <c r="C602" s="15"/>
+      <c r="C602" s="13"/>
       <c r="D602" s="4"/>
       <c r="E602" s="4"/>
       <c r="F602" s="4"/>
@@ -23800,7 +23798,7 @@
     <row r="603" ht="14.25" customHeight="1">
       <c r="A603" s="4"/>
       <c r="B603" s="4"/>
-      <c r="C603" s="15"/>
+      <c r="C603" s="13"/>
       <c r="D603" s="4"/>
       <c r="E603" s="4"/>
       <c r="F603" s="4"/>
@@ -23828,7 +23826,7 @@
     <row r="604" ht="14.25" customHeight="1">
       <c r="A604" s="4"/>
       <c r="B604" s="4"/>
-      <c r="C604" s="15"/>
+      <c r="C604" s="13"/>
       <c r="D604" s="4"/>
       <c r="E604" s="4"/>
       <c r="F604" s="4"/>
@@ -23856,7 +23854,7 @@
     <row r="605" ht="14.25" customHeight="1">
       <c r="A605" s="4"/>
       <c r="B605" s="4"/>
-      <c r="C605" s="15"/>
+      <c r="C605" s="13"/>
       <c r="D605" s="4"/>
       <c r="E605" s="4"/>
       <c r="F605" s="4"/>
@@ -23884,7 +23882,7 @@
     <row r="606" ht="14.25" customHeight="1">
       <c r="A606" s="4"/>
       <c r="B606" s="4"/>
-      <c r="C606" s="15"/>
+      <c r="C606" s="13"/>
       <c r="D606" s="4"/>
       <c r="E606" s="4"/>
       <c r="F606" s="4"/>
@@ -23912,7 +23910,7 @@
     <row r="607" ht="14.25" customHeight="1">
       <c r="A607" s="4"/>
       <c r="B607" s="4"/>
-      <c r="C607" s="15"/>
+      <c r="C607" s="13"/>
       <c r="D607" s="4"/>
       <c r="E607" s="4"/>
       <c r="F607" s="4"/>
@@ -23940,7 +23938,7 @@
     <row r="608" ht="14.25" customHeight="1">
       <c r="A608" s="4"/>
       <c r="B608" s="4"/>
-      <c r="C608" s="15"/>
+      <c r="C608" s="13"/>
       <c r="D608" s="4"/>
       <c r="E608" s="4"/>
       <c r="F608" s="4"/>
@@ -23968,7 +23966,7 @@
     <row r="609" ht="14.25" customHeight="1">
       <c r="A609" s="4"/>
       <c r="B609" s="4"/>
-      <c r="C609" s="15"/>
+      <c r="C609" s="13"/>
       <c r="D609" s="4"/>
       <c r="E609" s="4"/>
       <c r="F609" s="4"/>
@@ -23996,7 +23994,7 @@
     <row r="610" ht="14.25" customHeight="1">
       <c r="A610" s="4"/>
       <c r="B610" s="4"/>
-      <c r="C610" s="15"/>
+      <c r="C610" s="13"/>
       <c r="D610" s="4"/>
       <c r="E610" s="4"/>
       <c r="F610" s="4"/>
@@ -24024,7 +24022,7 @@
     <row r="611" ht="14.25" customHeight="1">
       <c r="A611" s="4"/>
       <c r="B611" s="4"/>
-      <c r="C611" s="15"/>
+      <c r="C611" s="13"/>
       <c r="D611" s="4"/>
       <c r="E611" s="4"/>
       <c r="F611" s="4"/>
@@ -24052,7 +24050,7 @@
     <row r="612" ht="14.25" customHeight="1">
       <c r="A612" s="4"/>
       <c r="B612" s="4"/>
-      <c r="C612" s="15"/>
+      <c r="C612" s="13"/>
       <c r="D612" s="4"/>
       <c r="E612" s="4"/>
       <c r="F612" s="4"/>
@@ -24080,7 +24078,7 @@
     <row r="613" ht="14.25" customHeight="1">
       <c r="A613" s="4"/>
       <c r="B613" s="4"/>
-      <c r="C613" s="15"/>
+      <c r="C613" s="13"/>
       <c r="D613" s="4"/>
       <c r="E613" s="4"/>
       <c r="F613" s="4"/>
@@ -24108,7 +24106,7 @@
     <row r="614" ht="14.25" customHeight="1">
       <c r="A614" s="4"/>
       <c r="B614" s="4"/>
-      <c r="C614" s="15"/>
+      <c r="C614" s="13"/>
       <c r="D614" s="4"/>
       <c r="E614" s="4"/>
       <c r="F614" s="4"/>
@@ -24136,7 +24134,7 @@
     <row r="615" ht="14.25" customHeight="1">
       <c r="A615" s="4"/>
       <c r="B615" s="4"/>
-      <c r="C615" s="15"/>
+      <c r="C615" s="13"/>
       <c r="D615" s="4"/>
       <c r="E615" s="4"/>
       <c r="F615" s="4"/>
@@ -24164,7 +24162,7 @@
     <row r="616" ht="14.25" customHeight="1">
       <c r="A616" s="4"/>
       <c r="B616" s="4"/>
-      <c r="C616" s="15"/>
+      <c r="C616" s="13"/>
       <c r="D616" s="4"/>
       <c r="E616" s="4"/>
       <c r="F616" s="4"/>
@@ -24192,7 +24190,7 @@
     <row r="617" ht="14.25" customHeight="1">
       <c r="A617" s="4"/>
       <c r="B617" s="4"/>
-      <c r="C617" s="15"/>
+      <c r="C617" s="13"/>
       <c r="D617" s="4"/>
       <c r="E617" s="4"/>
       <c r="F617" s="4"/>
@@ -24220,7 +24218,7 @@
     <row r="618" ht="14.25" customHeight="1">
       <c r="A618" s="4"/>
       <c r="B618" s="4"/>
-      <c r="C618" s="15"/>
+      <c r="C618" s="13"/>
       <c r="D618" s="4"/>
       <c r="E618" s="4"/>
       <c r="F618" s="4"/>
@@ -24248,7 +24246,7 @@
     <row r="619" ht="14.25" customHeight="1">
       <c r="A619" s="4"/>
       <c r="B619" s="4"/>
-      <c r="C619" s="15"/>
+      <c r="C619" s="13"/>
       <c r="D619" s="4"/>
       <c r="E619" s="4"/>
       <c r="F619" s="4"/>
@@ -24276,7 +24274,7 @@
     <row r="620" ht="14.25" customHeight="1">
       <c r="A620" s="4"/>
       <c r="B620" s="4"/>
-      <c r="C620" s="15"/>
+      <c r="C620" s="13"/>
       <c r="D620" s="4"/>
       <c r="E620" s="4"/>
       <c r="F620" s="4"/>
@@ -24304,7 +24302,7 @@
     <row r="621" ht="14.25" customHeight="1">
       <c r="A621" s="4"/>
       <c r="B621" s="4"/>
-      <c r="C621" s="15"/>
+      <c r="C621" s="13"/>
       <c r="D621" s="4"/>
       <c r="E621" s="4"/>
       <c r="F621" s="4"/>
@@ -24332,7 +24330,7 @@
     <row r="622" ht="14.25" customHeight="1">
       <c r="A622" s="4"/>
       <c r="B622" s="4"/>
-      <c r="C622" s="15"/>
+      <c r="C622" s="13"/>
       <c r="D622" s="4"/>
       <c r="E622" s="4"/>
       <c r="F622" s="4"/>
@@ -24360,7 +24358,7 @@
     <row r="623" ht="14.25" customHeight="1">
       <c r="A623" s="4"/>
       <c r="B623" s="4"/>
-      <c r="C623" s="15"/>
+      <c r="C623" s="13"/>
       <c r="D623" s="4"/>
       <c r="E623" s="4"/>
       <c r="F623" s="4"/>
@@ -24388,7 +24386,7 @@
     <row r="624" ht="14.25" customHeight="1">
       <c r="A624" s="4"/>
       <c r="B624" s="4"/>
-      <c r="C624" s="15"/>
+      <c r="C624" s="13"/>
       <c r="D624" s="4"/>
       <c r="E624" s="4"/>
       <c r="F624" s="4"/>
@@ -24416,7 +24414,7 @@
     <row r="625" ht="14.25" customHeight="1">
       <c r="A625" s="4"/>
       <c r="B625" s="4"/>
-      <c r="C625" s="15"/>
+      <c r="C625" s="13"/>
       <c r="D625" s="4"/>
       <c r="E625" s="4"/>
       <c r="F625" s="4"/>
@@ -24444,7 +24442,7 @@
     <row r="626" ht="14.25" customHeight="1">
       <c r="A626" s="4"/>
       <c r="B626" s="4"/>
-      <c r="C626" s="15"/>
+      <c r="C626" s="13"/>
       <c r="D626" s="4"/>
       <c r="E626" s="4"/>
       <c r="F626" s="4"/>
@@ -24472,7 +24470,7 @@
     <row r="627" ht="14.25" customHeight="1">
       <c r="A627" s="4"/>
       <c r="B627" s="4"/>
-      <c r="C627" s="15"/>
+      <c r="C627" s="13"/>
       <c r="D627" s="4"/>
       <c r="E627" s="4"/>
       <c r="F627" s="4"/>
@@ -24500,7 +24498,7 @@
     <row r="628" ht="14.25" customHeight="1">
       <c r="A628" s="4"/>
       <c r="B628" s="4"/>
-      <c r="C628" s="15"/>
+      <c r="C628" s="13"/>
       <c r="D628" s="4"/>
       <c r="E628" s="4"/>
       <c r="F628" s="4"/>
@@ -24528,7 +24526,7 @@
     <row r="629" ht="14.25" customHeight="1">
       <c r="A629" s="4"/>
       <c r="B629" s="4"/>
-      <c r="C629" s="15"/>
+      <c r="C629" s="13"/>
       <c r="D629" s="4"/>
       <c r="E629" s="4"/>
       <c r="F629" s="4"/>
@@ -24556,7 +24554,7 @@
     <row r="630" ht="14.25" customHeight="1">
       <c r="A630" s="4"/>
       <c r="B630" s="4"/>
-      <c r="C630" s="15"/>
+      <c r="C630" s="13"/>
       <c r="D630" s="4"/>
       <c r="E630" s="4"/>
       <c r="F630" s="4"/>
@@ -24584,7 +24582,7 @@
     <row r="631" ht="14.25" customHeight="1">
       <c r="A631" s="4"/>
       <c r="B631" s="4"/>
-      <c r="C631" s="15"/>
+      <c r="C631" s="13"/>
       <c r="D631" s="4"/>
       <c r="E631" s="4"/>
       <c r="F631" s="4"/>
@@ -24612,7 +24610,7 @@
     <row r="632" ht="14.25" customHeight="1">
       <c r="A632" s="4"/>
       <c r="B632" s="4"/>
-      <c r="C632" s="15"/>
+      <c r="C632" s="13"/>
       <c r="D632" s="4"/>
       <c r="E632" s="4"/>
       <c r="F632" s="4"/>
@@ -24640,7 +24638,7 @@
     <row r="633" ht="14.25" customHeight="1">
       <c r="A633" s="4"/>
       <c r="B633" s="4"/>
-      <c r="C633" s="15"/>
+      <c r="C633" s="13"/>
       <c r="D633" s="4"/>
       <c r="E633" s="4"/>
       <c r="F633" s="4"/>
@@ -24668,7 +24666,7 @@
     <row r="634" ht="14.25" customHeight="1">
       <c r="A634" s="4"/>
       <c r="B634" s="4"/>
-      <c r="C634" s="15"/>
+      <c r="C634" s="13"/>
       <c r="D634" s="4"/>
       <c r="E634" s="4"/>
       <c r="F634" s="4"/>
@@ -24696,7 +24694,7 @@
     <row r="635" ht="14.25" customHeight="1">
       <c r="A635" s="4"/>
       <c r="B635" s="4"/>
-      <c r="C635" s="15"/>
+      <c r="C635" s="13"/>
       <c r="D635" s="4"/>
       <c r="E635" s="4"/>
       <c r="F635" s="4"/>
@@ -24724,7 +24722,7 @@
     <row r="636" ht="14.25" customHeight="1">
       <c r="A636" s="4"/>
       <c r="B636" s="4"/>
-      <c r="C636" s="15"/>
+      <c r="C636" s="13"/>
       <c r="D636" s="4"/>
       <c r="E636" s="4"/>
       <c r="F636" s="4"/>
@@ -24752,7 +24750,7 @@
     <row r="637" ht="14.25" customHeight="1">
       <c r="A637" s="4"/>
       <c r="B637" s="4"/>
-      <c r="C637" s="15"/>
+      <c r="C637" s="13"/>
       <c r="D637" s="4"/>
       <c r="E637" s="4"/>
       <c r="F637" s="4"/>
@@ -24780,7 +24778,7 @@
     <row r="638" ht="14.25" customHeight="1">
       <c r="A638" s="4"/>
       <c r="B638" s="4"/>
-      <c r="C638" s="15"/>
+      <c r="C638" s="13"/>
       <c r="D638" s="4"/>
       <c r="E638" s="4"/>
       <c r="F638" s="4"/>
@@ -24808,7 +24806,7 @@
     <row r="639" ht="14.25" customHeight="1">
       <c r="A639" s="4"/>
       <c r="B639" s="4"/>
-      <c r="C639" s="15"/>
+      <c r="C639" s="13"/>
       <c r="D639" s="4"/>
       <c r="E639" s="4"/>
       <c r="F639" s="4"/>
@@ -24836,7 +24834,7 @@
     <row r="640" ht="14.25" customHeight="1">
       <c r="A640" s="4"/>
       <c r="B640" s="4"/>
-      <c r="C640" s="15"/>
+      <c r="C640" s="13"/>
       <c r="D640" s="4"/>
       <c r="E640" s="4"/>
       <c r="F640" s="4"/>
@@ -24864,7 +24862,7 @@
     <row r="641" ht="14.25" customHeight="1">
       <c r="A641" s="4"/>
       <c r="B641" s="4"/>
-      <c r="C641" s="15"/>
+      <c r="C641" s="13"/>
       <c r="D641" s="4"/>
       <c r="E641" s="4"/>
       <c r="F641" s="4"/>
@@ -24892,7 +24890,7 @@
     <row r="642" ht="14.25" customHeight="1">
       <c r="A642" s="4"/>
       <c r="B642" s="4"/>
-      <c r="C642" s="15"/>
+      <c r="C642" s="13"/>
       <c r="D642" s="4"/>
       <c r="E642" s="4"/>
       <c r="F642" s="4"/>
@@ -24920,7 +24918,7 @@
     <row r="643" ht="14.25" customHeight="1">
       <c r="A643" s="4"/>
       <c r="B643" s="4"/>
-      <c r="C643" s="15"/>
+      <c r="C643" s="13"/>
       <c r="D643" s="4"/>
       <c r="E643" s="4"/>
       <c r="F643" s="4"/>
@@ -24948,7 +24946,7 @@
     <row r="644" ht="14.25" customHeight="1">
       <c r="A644" s="4"/>
       <c r="B644" s="4"/>
-      <c r="C644" s="15"/>
+      <c r="C644" s="13"/>
       <c r="D644" s="4"/>
       <c r="E644" s="4"/>
       <c r="F644" s="4"/>
@@ -24976,7 +24974,7 @@
     <row r="645" ht="14.25" customHeight="1">
       <c r="A645" s="4"/>
       <c r="B645" s="4"/>
-      <c r="C645" s="15"/>
+      <c r="C645" s="13"/>
       <c r="D645" s="4"/>
       <c r="E645" s="4"/>
       <c r="F645" s="4"/>
@@ -25004,7 +25002,7 @@
     <row r="646" ht="14.25" customHeight="1">
       <c r="A646" s="4"/>
       <c r="B646" s="4"/>
-      <c r="C646" s="15"/>
+      <c r="C646" s="13"/>
       <c r="D646" s="4"/>
       <c r="E646" s="4"/>
       <c r="F646" s="4"/>
@@ -25032,7 +25030,7 @@
     <row r="647" ht="14.25" customHeight="1">
       <c r="A647" s="4"/>
       <c r="B647" s="4"/>
-      <c r="C647" s="15"/>
+      <c r="C647" s="13"/>
       <c r="D647" s="4"/>
       <c r="E647" s="4"/>
       <c r="F647" s="4"/>
@@ -25060,7 +25058,7 @@
     <row r="648" ht="14.25" customHeight="1">
       <c r="A648" s="4"/>
       <c r="B648" s="4"/>
-      <c r="C648" s="15"/>
+      <c r="C648" s="13"/>
       <c r="D648" s="4"/>
       <c r="E648" s="4"/>
       <c r="F648" s="4"/>
@@ -25088,7 +25086,7 @@
     <row r="649" ht="14.25" customHeight="1">
       <c r="A649" s="4"/>
       <c r="B649" s="4"/>
-      <c r="C649" s="15"/>
+      <c r="C649" s="13"/>
       <c r="D649" s="4"/>
       <c r="E649" s="4"/>
       <c r="F649" s="4"/>
@@ -25116,7 +25114,7 @@
     <row r="650" ht="14.25" customHeight="1">
       <c r="A650" s="4"/>
       <c r="B650" s="4"/>
-      <c r="C650" s="15"/>
+      <c r="C650" s="13"/>
       <c r="D650" s="4"/>
       <c r="E650" s="4"/>
       <c r="F650" s="4"/>
@@ -25144,7 +25142,7 @@
     <row r="651" ht="14.25" customHeight="1">
       <c r="A651" s="4"/>
       <c r="B651" s="4"/>
-      <c r="C651" s="15"/>
+      <c r="C651" s="13"/>
       <c r="D651" s="4"/>
       <c r="E651" s="4"/>
       <c r="F651" s="4"/>
@@ -25172,7 +25170,7 @@
     <row r="652" ht="14.25" customHeight="1">
       <c r="A652" s="4"/>
       <c r="B652" s="4"/>
-      <c r="C652" s="15"/>
+      <c r="C652" s="13"/>
       <c r="D652" s="4"/>
       <c r="E652" s="4"/>
       <c r="F652" s="4"/>
@@ -25200,7 +25198,7 @@
     <row r="653" ht="14.25" customHeight="1">
       <c r="A653" s="4"/>
       <c r="B653" s="4"/>
-      <c r="C653" s="15"/>
+      <c r="C653" s="13"/>
       <c r="D653" s="4"/>
       <c r="E653" s="4"/>
       <c r="F653" s="4"/>
@@ -25228,7 +25226,7 @@
     <row r="654" ht="14.25" customHeight="1">
       <c r="A654" s="4"/>
       <c r="B654" s="4"/>
-      <c r="C654" s="15"/>
+      <c r="C654" s="13"/>
       <c r="D654" s="4"/>
       <c r="E654" s="4"/>
       <c r="F654" s="4"/>
@@ -25256,7 +25254,7 @@
     <row r="655" ht="14.25" customHeight="1">
       <c r="A655" s="4"/>
       <c r="B655" s="4"/>
-      <c r="C655" s="15"/>
+      <c r="C655" s="13"/>
       <c r="D655" s="4"/>
       <c r="E655" s="4"/>
       <c r="F655" s="4"/>
@@ -25284,7 +25282,7 @@
     <row r="656" ht="14.25" customHeight="1">
       <c r="A656" s="4"/>
       <c r="B656" s="4"/>
-      <c r="C656" s="15"/>
+      <c r="C656" s="13"/>
       <c r="D656" s="4"/>
       <c r="E656" s="4"/>
       <c r="F656" s="4"/>
@@ -25312,7 +25310,7 @@
     <row r="657" ht="14.25" customHeight="1">
       <c r="A657" s="4"/>
       <c r="B657" s="4"/>
-      <c r="C657" s="15"/>
+      <c r="C657" s="13"/>
       <c r="D657" s="4"/>
       <c r="E657" s="4"/>
       <c r="F657" s="4"/>
@@ -25340,7 +25338,7 @@
     <row r="658" ht="14.25" customHeight="1">
       <c r="A658" s="4"/>
       <c r="B658" s="4"/>
-      <c r="C658" s="15"/>
+      <c r="C658" s="13"/>
       <c r="D658" s="4"/>
       <c r="E658" s="4"/>
       <c r="F658" s="4"/>
@@ -25368,7 +25366,7 @@
     <row r="659" ht="14.25" customHeight="1">
       <c r="A659" s="4"/>
       <c r="B659" s="4"/>
-      <c r="C659" s="15"/>
+      <c r="C659" s="13"/>
       <c r="D659" s="4"/>
       <c r="E659" s="4"/>
       <c r="F659" s="4"/>
@@ -25396,7 +25394,7 @@
     <row r="660" ht="14.25" customHeight="1">
       <c r="A660" s="4"/>
       <c r="B660" s="4"/>
-      <c r="C660" s="15"/>
+      <c r="C660" s="13"/>
       <c r="D660" s="4"/>
       <c r="E660" s="4"/>
       <c r="F660" s="4"/>
@@ -25424,7 +25422,7 @@
     <row r="661" ht="14.25" customHeight="1">
       <c r="A661" s="4"/>
       <c r="B661" s="4"/>
-      <c r="C661" s="15"/>
+      <c r="C661" s="13"/>
       <c r="D661" s="4"/>
       <c r="E661" s="4"/>
       <c r="F661" s="4"/>
@@ -25452,7 +25450,7 @@
     <row r="662" ht="14.25" customHeight="1">
       <c r="A662" s="4"/>
       <c r="B662" s="4"/>
-      <c r="C662" s="15"/>
+      <c r="C662" s="13"/>
       <c r="D662" s="4"/>
       <c r="E662" s="4"/>
       <c r="F662" s="4"/>
@@ -25480,7 +25478,7 @@
     <row r="663" ht="14.25" customHeight="1">
       <c r="A663" s="4"/>
       <c r="B663" s="4"/>
-      <c r="C663" s="15"/>
+      <c r="C663" s="13"/>
       <c r="D663" s="4"/>
       <c r="E663" s="4"/>
       <c r="F663" s="4"/>
@@ -25508,7 +25506,7 @@
     <row r="664" ht="14.25" customHeight="1">
       <c r="A664" s="4"/>
       <c r="B664" s="4"/>
-      <c r="C664" s="15"/>
+      <c r="C664" s="13"/>
       <c r="D664" s="4"/>
       <c r="E664" s="4"/>
       <c r="F664" s="4"/>
@@ -25536,7 +25534,7 @@
     <row r="665" ht="14.25" customHeight="1">
       <c r="A665" s="4"/>
       <c r="B665" s="4"/>
-      <c r="C665" s="15"/>
+      <c r="C665" s="13"/>
       <c r="D665" s="4"/>
       <c r="E665" s="4"/>
       <c r="F665" s="4"/>
@@ -25564,7 +25562,7 @@
     <row r="666" ht="14.25" customHeight="1">
       <c r="A666" s="4"/>
       <c r="B666" s="4"/>
-      <c r="C666" s="15"/>
+      <c r="C666" s="13"/>
       <c r="D666" s="4"/>
       <c r="E666" s="4"/>
       <c r="F666" s="4"/>
@@ -25592,7 +25590,7 @@
     <row r="667" ht="14.25" customHeight="1">
       <c r="A667" s="4"/>
       <c r="B667" s="4"/>
-      <c r="C667" s="15"/>
+      <c r="C667" s="13"/>
       <c r="D667" s="4"/>
       <c r="E667" s="4"/>
       <c r="F667" s="4"/>
@@ -25620,7 +25618,7 @@
     <row r="668" ht="14.25" customHeight="1">
       <c r="A668" s="4"/>
       <c r="B668" s="4"/>
-      <c r="C668" s="15"/>
+      <c r="C668" s="13"/>
       <c r="D668" s="4"/>
       <c r="E668" s="4"/>
       <c r="F668" s="4"/>
@@ -25648,7 +25646,7 @@
     <row r="669" ht="14.25" customHeight="1">
       <c r="A669" s="4"/>
       <c r="B669" s="4"/>
-      <c r="C669" s="15"/>
+      <c r="C669" s="13"/>
       <c r="D669" s="4"/>
       <c r="E669" s="4"/>
       <c r="F669" s="4"/>
@@ -25676,7 +25674,7 @@
     <row r="670" ht="14.25" customHeight="1">
       <c r="A670" s="4"/>
       <c r="B670" s="4"/>
-      <c r="C670" s="15"/>
+      <c r="C670" s="13"/>
       <c r="D670" s="4"/>
       <c r="E670" s="4"/>
       <c r="F670" s="4"/>
@@ -25704,7 +25702,7 @@
     <row r="671" ht="14.25" customHeight="1">
       <c r="A671" s="4"/>
       <c r="B671" s="4"/>
-      <c r="C671" s="15"/>
+      <c r="C671" s="13"/>
       <c r="D671" s="4"/>
       <c r="E671" s="4"/>
       <c r="F671" s="4"/>
@@ -25732,7 +25730,7 @@
     <row r="672" ht="14.25" customHeight="1">
       <c r="A672" s="4"/>
       <c r="B672" s="4"/>
-      <c r="C672" s="15"/>
+      <c r="C672" s="13"/>
       <c r="D672" s="4"/>
       <c r="E672" s="4"/>
       <c r="F672" s="4"/>
@@ -25760,7 +25758,7 @@
     <row r="673" ht="14.25" customHeight="1">
       <c r="A673" s="4"/>
       <c r="B673" s="4"/>
-      <c r="C673" s="15"/>
+      <c r="C673" s="13"/>
       <c r="D673" s="4"/>
       <c r="E673" s="4"/>
       <c r="F673" s="4"/>
@@ -25788,7 +25786,7 @@
     <row r="674" ht="14.25" customHeight="1">
       <c r="A674" s="4"/>
       <c r="B674" s="4"/>
-      <c r="C674" s="15"/>
+      <c r="C674" s="13"/>
       <c r="D674" s="4"/>
       <c r="E674" s="4"/>
       <c r="F674" s="4"/>
@@ -25816,7 +25814,7 @@
     <row r="675" ht="14.25" customHeight="1">
       <c r="A675" s="4"/>
       <c r="B675" s="4"/>
-      <c r="C675" s="15"/>
+      <c r="C675" s="13"/>
       <c r="D675" s="4"/>
       <c r="E675" s="4"/>
       <c r="F675" s="4"/>
@@ -25844,7 +25842,7 @@
     <row r="676" ht="14.25" customHeight="1">
       <c r="A676" s="4"/>
       <c r="B676" s="4"/>
-      <c r="C676" s="15"/>
+      <c r="C676" s="13"/>
       <c r="D676" s="4"/>
       <c r="E676" s="4"/>
       <c r="F676" s="4"/>
@@ -25872,7 +25870,7 @@
     <row r="677" ht="14.25" customHeight="1">
       <c r="A677" s="4"/>
       <c r="B677" s="4"/>
-      <c r="C677" s="15"/>
+      <c r="C677" s="13"/>
       <c r="D677" s="4"/>
       <c r="E677" s="4"/>
       <c r="F677" s="4"/>
@@ -25900,7 +25898,7 @@
     <row r="678" ht="14.25" customHeight="1">
       <c r="A678" s="4"/>
       <c r="B678" s="4"/>
-      <c r="C678" s="15"/>
+      <c r="C678" s="13"/>
       <c r="D678" s="4"/>
       <c r="E678" s="4"/>
       <c r="F678" s="4"/>
@@ -25928,7 +25926,7 @@
     <row r="679" ht="14.25" customHeight="1">
       <c r="A679" s="4"/>
       <c r="B679" s="4"/>
-      <c r="C679" s="15"/>
+      <c r="C679" s="13"/>
       <c r="D679" s="4"/>
       <c r="E679" s="4"/>
       <c r="F679" s="4"/>
@@ -25956,7 +25954,7 @@
     <row r="680" ht="14.25" customHeight="1">
       <c r="A680" s="4"/>
       <c r="B680" s="4"/>
-      <c r="C680" s="15"/>
+      <c r="C680" s="13"/>
       <c r="D680" s="4"/>
       <c r="E680" s="4"/>
       <c r="F680" s="4"/>
@@ -25984,7 +25982,7 @@
     <row r="681" ht="14.25" customHeight="1">
       <c r="A681" s="4"/>
       <c r="B681" s="4"/>
-      <c r="C681" s="15"/>
+      <c r="C681" s="13"/>
       <c r="D681" s="4"/>
       <c r="E681" s="4"/>
       <c r="F681" s="4"/>
@@ -26012,7 +26010,7 @@
     <row r="682" ht="14.25" customHeight="1">
       <c r="A682" s="4"/>
       <c r="B682" s="4"/>
-      <c r="C682" s="15"/>
+      <c r="C682" s="13"/>
       <c r="D682" s="4"/>
       <c r="E682" s="4"/>
       <c r="F682" s="4"/>
@@ -26040,7 +26038,7 @@
     <row r="683" ht="14.25" customHeight="1">
       <c r="A683" s="4"/>
       <c r="B683" s="4"/>
-      <c r="C683" s="15"/>
+      <c r="C683" s="13"/>
       <c r="D683" s="4"/>
       <c r="E683" s="4"/>
       <c r="F683" s="4"/>
@@ -26068,7 +26066,7 @@
     <row r="684" ht="14.25" customHeight="1">
       <c r="A684" s="4"/>
       <c r="B684" s="4"/>
-      <c r="C684" s="15"/>
+      <c r="C684" s="13"/>
       <c r="D684" s="4"/>
       <c r="E684" s="4"/>
       <c r="F684" s="4"/>
@@ -26096,7 +26094,7 @@
     <row r="685" ht="14.25" customHeight="1">
       <c r="A685" s="4"/>
       <c r="B685" s="4"/>
-      <c r="C685" s="15"/>
+      <c r="C685" s="13"/>
       <c r="D685" s="4"/>
       <c r="E685" s="4"/>
       <c r="F685" s="4"/>
@@ -26124,7 +26122,7 @@
     <row r="686" ht="14.25" customHeight="1">
       <c r="A686" s="4"/>
       <c r="B686" s="4"/>
-      <c r="C686" s="15"/>
+      <c r="C686" s="13"/>
       <c r="D686" s="4"/>
       <c r="E686" s="4"/>
       <c r="F686" s="4"/>
@@ -26152,7 +26150,7 @@
     <row r="687" ht="14.25" customHeight="1">
       <c r="A687" s="4"/>
       <c r="B687" s="4"/>
-      <c r="C687" s="15"/>
+      <c r="C687" s="13"/>
       <c r="D687" s="4"/>
       <c r="E687" s="4"/>
       <c r="F687" s="4"/>
@@ -26180,7 +26178,7 @@
     <row r="688" ht="14.25" customHeight="1">
       <c r="A688" s="4"/>
       <c r="B688" s="4"/>
-      <c r="C688" s="15"/>
+      <c r="C688" s="13"/>
       <c r="D688" s="4"/>
       <c r="E688" s="4"/>
       <c r="F688" s="4"/>
@@ -26208,7 +26206,7 @@
     <row r="689" ht="14.25" customHeight="1">
       <c r="A689" s="4"/>
       <c r="B689" s="4"/>
-      <c r="C689" s="15"/>
+      <c r="C689" s="13"/>
       <c r="D689" s="4"/>
       <c r="E689" s="4"/>
       <c r="F689" s="4"/>
@@ -26236,7 +26234,7 @@
     <row r="690" ht="14.25" customHeight="1">
       <c r="A690" s="4"/>
       <c r="B690" s="4"/>
-      <c r="C690" s="15"/>
+      <c r="C690" s="13"/>
       <c r="D690" s="4"/>
       <c r="E690" s="4"/>
       <c r="F690" s="4"/>
@@ -26264,7 +26262,7 @@
     <row r="691" ht="14.25" customHeight="1">
       <c r="A691" s="4"/>
       <c r="B691" s="4"/>
-      <c r="C691" s="15"/>
+      <c r="C691" s="13"/>
       <c r="D691" s="4"/>
       <c r="E691" s="4"/>
       <c r="F691" s="4"/>
@@ -26292,7 +26290,7 @@
     <row r="692" ht="14.25" customHeight="1">
       <c r="A692" s="4"/>
       <c r="B692" s="4"/>
-      <c r="C692" s="15"/>
+      <c r="C692" s="13"/>
       <c r="D692" s="4"/>
       <c r="E692" s="4"/>
       <c r="F692" s="4"/>
@@ -26320,7 +26318,7 @@
     <row r="693" ht="14.25" customHeight="1">
       <c r="A693" s="4"/>
       <c r="B693" s="4"/>
-      <c r="C693" s="15"/>
+      <c r="C693" s="13"/>
       <c r="D693" s="4"/>
       <c r="E693" s="4"/>
       <c r="F693" s="4"/>
@@ -26348,7 +26346,7 @@
     <row r="694" ht="14.25" customHeight="1">
       <c r="A694" s="4"/>
       <c r="B694" s="4"/>
-      <c r="C694" s="15"/>
+      <c r="C694" s="13"/>
       <c r="D694" s="4"/>
       <c r="E694" s="4"/>
       <c r="F694" s="4"/>
@@ -26376,7 +26374,7 @@
     <row r="695" ht="14.25" customHeight="1">
       <c r="A695" s="4"/>
       <c r="B695" s="4"/>
-      <c r="C695" s="15"/>
+      <c r="C695" s="13"/>
       <c r="D695" s="4"/>
       <c r="E695" s="4"/>
       <c r="F695" s="4"/>
@@ -26404,7 +26402,7 @@
     <row r="696" ht="14.25" customHeight="1">
       <c r="A696" s="4"/>
       <c r="B696" s="4"/>
-      <c r="C696" s="15"/>
+      <c r="C696" s="13"/>
       <c r="D696" s="4"/>
       <c r="E696" s="4"/>
       <c r="F696" s="4"/>
@@ -26432,7 +26430,7 @@
     <row r="697" ht="14.25" customHeight="1">
       <c r="A697" s="4"/>
       <c r="B697" s="4"/>
-      <c r="C697" s="15"/>
+      <c r="C697" s="13"/>
       <c r="D697" s="4"/>
       <c r="E697" s="4"/>
       <c r="F697" s="4"/>
@@ -26460,7 +26458,7 @@
     <row r="698" ht="14.25" customHeight="1">
       <c r="A698" s="4"/>
       <c r="B698" s="4"/>
-      <c r="C698" s="15"/>
+      <c r="C698" s="13"/>
       <c r="D698" s="4"/>
       <c r="E698" s="4"/>
       <c r="F698" s="4"/>
@@ -26488,7 +26486,7 @@
     <row r="699" ht="14.25" customHeight="1">
       <c r="A699" s="4"/>
       <c r="B699" s="4"/>
-      <c r="C699" s="15"/>
+      <c r="C699" s="13"/>
       <c r="D699" s="4"/>
       <c r="E699" s="4"/>
       <c r="F699" s="4"/>
@@ -26516,7 +26514,7 @@
     <row r="700" ht="14.25" customHeight="1">
       <c r="A700" s="4"/>
       <c r="B700" s="4"/>
-      <c r="C700" s="15"/>
+      <c r="C700" s="13"/>
       <c r="D700" s="4"/>
       <c r="E700" s="4"/>
       <c r="F700" s="4"/>
@@ -26544,7 +26542,7 @@
     <row r="701" ht="14.25" customHeight="1">
       <c r="A701" s="4"/>
       <c r="B701" s="4"/>
-      <c r="C701" s="15"/>
+      <c r="C701" s="13"/>
       <c r="D701" s="4"/>
       <c r="E701" s="4"/>
       <c r="F701" s="4"/>
@@ -26572,7 +26570,7 @@
     <row r="702" ht="14.25" customHeight="1">
       <c r="A702" s="4"/>
       <c r="B702" s="4"/>
-      <c r="C702" s="15"/>
+      <c r="C702" s="13"/>
       <c r="D702" s="4"/>
       <c r="E702" s="4"/>
       <c r="F702" s="4"/>
@@ -26600,7 +26598,7 @@
     <row r="703" ht="14.25" customHeight="1">
       <c r="A703" s="4"/>
       <c r="B703" s="4"/>
-      <c r="C703" s="15"/>
+      <c r="C703" s="13"/>
       <c r="D703" s="4"/>
       <c r="E703" s="4"/>
       <c r="F703" s="4"/>
@@ -26628,7 +26626,7 @@
     <row r="704" ht="14.25" customHeight="1">
       <c r="A704" s="4"/>
       <c r="B704" s="4"/>
-      <c r="C704" s="15"/>
+      <c r="C704" s="13"/>
       <c r="D704" s="4"/>
       <c r="E704" s="4"/>
       <c r="F704" s="4"/>
@@ -26656,7 +26654,7 @@
     <row r="705" ht="14.25" customHeight="1">
       <c r="A705" s="4"/>
       <c r="B705" s="4"/>
-      <c r="C705" s="15"/>
+      <c r="C705" s="13"/>
       <c r="D705" s="4"/>
       <c r="E705" s="4"/>
       <c r="F705" s="4"/>
@@ -26684,7 +26682,7 @@
     <row r="706" ht="14.25" customHeight="1">
       <c r="A706" s="4"/>
       <c r="B706" s="4"/>
-      <c r="C706" s="15"/>
+      <c r="C706" s="13"/>
       <c r="D706" s="4"/>
       <c r="E706" s="4"/>
       <c r="F706" s="4"/>
@@ -26712,7 +26710,7 @@
     <row r="707" ht="14.25" customHeight="1">
       <c r="A707" s="4"/>
       <c r="B707" s="4"/>
-      <c r="C707" s="15"/>
+      <c r="C707" s="13"/>
       <c r="D707" s="4"/>
       <c r="E707" s="4"/>
       <c r="F707" s="4"/>
@@ -26740,7 +26738,7 @@
     <row r="708" ht="14.25" customHeight="1">
       <c r="A708" s="4"/>
       <c r="B708" s="4"/>
-      <c r="C708" s="15"/>
+      <c r="C708" s="13"/>
       <c r="D708" s="4"/>
       <c r="E708" s="4"/>
       <c r="F708" s="4"/>
@@ -26768,7 +26766,7 @@
     <row r="709" ht="14.25" customHeight="1">
       <c r="A709" s="4"/>
       <c r="B709" s="4"/>
-      <c r="C709" s="15"/>
+      <c r="C709" s="13"/>
       <c r="D709" s="4"/>
       <c r="E709" s="4"/>
       <c r="F709" s="4"/>
@@ -26796,7 +26794,7 @@
     <row r="710" ht="14.25" customHeight="1">
       <c r="A710" s="4"/>
       <c r="B710" s="4"/>
-      <c r="C710" s="15"/>
+      <c r="C710" s="13"/>
       <c r="D710" s="4"/>
       <c r="E710" s="4"/>
       <c r="F710" s="4"/>
@@ -26824,7 +26822,7 @@
     <row r="711" ht="14.25" customHeight="1">
       <c r="A711" s="4"/>
       <c r="B711" s="4"/>
-      <c r="C711" s="15"/>
+      <c r="C711" s="13"/>
       <c r="D711" s="4"/>
       <c r="E711" s="4"/>
       <c r="F711" s="4"/>
@@ -26852,7 +26850,7 @@
     <row r="712" ht="14.25" customHeight="1">
       <c r="A712" s="4"/>
       <c r="B712" s="4"/>
-      <c r="C712" s="15"/>
+      <c r="C712" s="13"/>
       <c r="D712" s="4"/>
       <c r="E712" s="4"/>
       <c r="F712" s="4"/>
@@ -26880,7 +26878,7 @@
     <row r="713" ht="14.25" customHeight="1">
       <c r="A713" s="4"/>
       <c r="B713" s="4"/>
-      <c r="C713" s="15"/>
+      <c r="C713" s="13"/>
       <c r="D713" s="4"/>
       <c r="E713" s="4"/>
       <c r="F713" s="4"/>
@@ -26908,7 +26906,7 @@
     <row r="714" ht="14.25" customHeight="1">
       <c r="A714" s="4"/>
       <c r="B714" s="4"/>
-      <c r="C714" s="15"/>
+      <c r="C714" s="13"/>
       <c r="D714" s="4"/>
       <c r="E714" s="4"/>
       <c r="F714" s="4"/>
@@ -26936,7 +26934,7 @@
     <row r="715" ht="14.25" customHeight="1">
       <c r="A715" s="4"/>
       <c r="B715" s="4"/>
-      <c r="C715" s="15"/>
+      <c r="C715" s="13"/>
       <c r="D715" s="4"/>
       <c r="E715" s="4"/>
       <c r="F715" s="4"/>
@@ -26964,7 +26962,7 @@
     <row r="716" ht="14.25" customHeight="1">
       <c r="A716" s="4"/>
       <c r="B716" s="4"/>
-      <c r="C716" s="15"/>
+      <c r="C716" s="13"/>
       <c r="D716" s="4"/>
       <c r="E716" s="4"/>
       <c r="F716" s="4"/>
@@ -26992,7 +26990,7 @@
     <row r="717" ht="14.25" customHeight="1">
       <c r="A717" s="4"/>
       <c r="B717" s="4"/>
-      <c r="C717" s="15"/>
+      <c r="C717" s="13"/>
       <c r="D717" s="4"/>
       <c r="E717" s="4"/>
       <c r="F717" s="4"/>
@@ -27020,7 +27018,7 @@
     <row r="718" ht="14.25" customHeight="1">
       <c r="A718" s="4"/>
       <c r="B718" s="4"/>
-      <c r="C718" s="15"/>
+      <c r="C718" s="13"/>
       <c r="D718" s="4"/>
       <c r="E718" s="4"/>
       <c r="F718" s="4"/>
@@ -27048,7 +27046,7 @@
     <row r="719" ht="14.25" customHeight="1">
       <c r="A719" s="4"/>
       <c r="B719" s="4"/>
-      <c r="C719" s="15"/>
+      <c r="C719" s="13"/>
       <c r="D719" s="4"/>
       <c r="E719" s="4"/>
       <c r="F719" s="4"/>
@@ -27076,7 +27074,7 @@
     <row r="720" ht="14.25" customHeight="1">
       <c r="A720" s="4"/>
       <c r="B720" s="4"/>
-      <c r="C720" s="15"/>
+      <c r="C720" s="13"/>
       <c r="D720" s="4"/>
       <c r="E720" s="4"/>
       <c r="F720" s="4"/>
@@ -27104,7 +27102,7 @@
     <row r="721" ht="14.25" customHeight="1">
       <c r="A721" s="4"/>
       <c r="B721" s="4"/>
-      <c r="C721" s="15"/>
+      <c r="C721" s="13"/>
       <c r="D721" s="4"/>
       <c r="E721" s="4"/>
       <c r="F721" s="4"/>
@@ -27132,7 +27130,7 @@
     <row r="722" ht="14.25" customHeight="1">
       <c r="A722" s="4"/>
       <c r="B722" s="4"/>
-      <c r="C722" s="15"/>
+      <c r="C722" s="13"/>
       <c r="D722" s="4"/>
       <c r="E722" s="4"/>
       <c r="F722" s="4"/>
@@ -27160,7 +27158,7 @@
     <row r="723" ht="14.25" customHeight="1">
       <c r="A723" s="4"/>
       <c r="B723" s="4"/>
-      <c r="C723" s="15"/>
+      <c r="C723" s="13"/>
       <c r="D723" s="4"/>
       <c r="E723" s="4"/>
       <c r="F723" s="4"/>
@@ -27188,7 +27186,7 @@
     <row r="724" ht="14.25" customHeight="1">
       <c r="A724" s="4"/>
       <c r="B724" s="4"/>
-      <c r="C724" s="15"/>
+      <c r="C724" s="13"/>
       <c r="D724" s="4"/>
       <c r="E724" s="4"/>
       <c r="F724" s="4"/>
@@ -27216,7 +27214,7 @@
     <row r="725" ht="14.25" customHeight="1">
       <c r="A725" s="4"/>
       <c r="B725" s="4"/>
-      <c r="C725" s="15"/>
+      <c r="C725" s="13"/>
       <c r="D725" s="4"/>
       <c r="E725" s="4"/>
       <c r="F725" s="4"/>
@@ -27244,7 +27242,7 @@
     <row r="726" ht="14.25" customHeight="1">
       <c r="A726" s="4"/>
       <c r="B726" s="4"/>
-      <c r="C726" s="15"/>
+      <c r="C726" s="13"/>
       <c r="D726" s="4"/>
       <c r="E726" s="4"/>
       <c r="F726" s="4"/>
@@ -27272,7 +27270,7 @@
     <row r="727" ht="14.25" customHeight="1">
       <c r="A727" s="4"/>
       <c r="B727" s="4"/>
-      <c r="C727" s="15"/>
+      <c r="C727" s="13"/>
       <c r="D727" s="4"/>
       <c r="E727" s="4"/>
       <c r="F727" s="4"/>
@@ -27300,7 +27298,7 @@
     <row r="728" ht="14.25" customHeight="1">
       <c r="A728" s="4"/>
       <c r="B728" s="4"/>
-      <c r="C728" s="15"/>
+      <c r="C728" s="13"/>
       <c r="D728" s="4"/>
       <c r="E728" s="4"/>
       <c r="F728" s="4"/>
@@ -27328,7 +27326,7 @@
     <row r="729" ht="14.25" customHeight="1">
       <c r="A729" s="4"/>
       <c r="B729" s="4"/>
-      <c r="C729" s="15"/>
+      <c r="C729" s="13"/>
       <c r="D729" s="4"/>
       <c r="E729" s="4"/>
       <c r="F729" s="4"/>
@@ -27356,7 +27354,7 @@
     <row r="730" ht="14.25" customHeight="1">
       <c r="A730" s="4"/>
       <c r="B730" s="4"/>
-      <c r="C730" s="15"/>
+      <c r="C730" s="13"/>
       <c r="D730" s="4"/>
       <c r="E730" s="4"/>
       <c r="F730" s="4"/>
@@ -27384,7 +27382,7 @@
     <row r="731" ht="14.25" customHeight="1">
       <c r="A731" s="4"/>
       <c r="B731" s="4"/>
-      <c r="C731" s="15"/>
+      <c r="C731" s="13"/>
       <c r="D731" s="4"/>
       <c r="E731" s="4"/>
       <c r="F731" s="4"/>
@@ -27412,7 +27410,7 @@
     <row r="732" ht="14.25" customHeight="1">
       <c r="A732" s="4"/>
       <c r="B732" s="4"/>
-      <c r="C732" s="15"/>
+      <c r="C732" s="13"/>
       <c r="D732" s="4"/>
       <c r="E732" s="4"/>
       <c r="F732" s="4"/>
@@ -27440,7 +27438,7 @@
     <row r="733" ht="14.25" customHeight="1">
       <c r="A733" s="4"/>
       <c r="B733" s="4"/>
-      <c r="C733" s="15"/>
+      <c r="C733" s="13"/>
       <c r="D733" s="4"/>
       <c r="E733" s="4"/>
       <c r="F733" s="4"/>
@@ -27468,7 +27466,7 @@
     <row r="734" ht="14.25" customHeight="1">
       <c r="A734" s="4"/>
       <c r="B734" s="4"/>
-      <c r="C734" s="15"/>
+      <c r="C734" s="13"/>
       <c r="D734" s="4"/>
       <c r="E734" s="4"/>
       <c r="F734" s="4"/>
@@ -27496,7 +27494,7 @@
     <row r="735" ht="14.25" customHeight="1">
       <c r="A735" s="4"/>
       <c r="B735" s="4"/>
-      <c r="C735" s="15"/>
+      <c r="C735" s="13"/>
       <c r="D735" s="4"/>
       <c r="E735" s="4"/>
       <c r="F735" s="4"/>
@@ -27524,7 +27522,7 @@
     <row r="736" ht="14.25" customHeight="1">
       <c r="A736" s="4"/>
       <c r="B736" s="4"/>
-      <c r="C736" s="15"/>
+      <c r="C736" s="13"/>
       <c r="D736" s="4"/>
       <c r="E736" s="4"/>
       <c r="F736" s="4"/>
@@ -27552,7 +27550,7 @@
     <row r="737" ht="14.25" customHeight="1">
       <c r="A737" s="4"/>
       <c r="B737" s="4"/>
-      <c r="C737" s="15"/>
+      <c r="C737" s="13"/>
       <c r="D737" s="4"/>
       <c r="E737" s="4"/>
       <c r="F737" s="4"/>
@@ -27580,7 +27578,7 @@
     <row r="738" ht="14.25" customHeight="1">
       <c r="A738" s="4"/>
       <c r="B738" s="4"/>
-      <c r="C738" s="15"/>
+      <c r="C738" s="13"/>
       <c r="D738" s="4"/>
       <c r="E738" s="4"/>
       <c r="F738" s="4"/>
@@ -27608,7 +27606,7 @@
     <row r="739" ht="14.25" customHeight="1">
       <c r="A739" s="4"/>
       <c r="B739" s="4"/>
-      <c r="C739" s="15"/>
+      <c r="C739" s="13"/>
       <c r="D739" s="4"/>
       <c r="E739" s="4"/>
       <c r="F739" s="4"/>
@@ -27636,7 +27634,7 @@
     <row r="740" ht="14.25" customHeight="1">
       <c r="A740" s="4"/>
       <c r="B740" s="4"/>
-      <c r="C740" s="15"/>
+      <c r="C740" s="13"/>
       <c r="D740" s="4"/>
       <c r="E740" s="4"/>
       <c r="F740" s="4"/>
@@ -27664,7 +27662,7 @@
     <row r="741" ht="14.25" customHeight="1">
       <c r="A741" s="4"/>
       <c r="B741" s="4"/>
-      <c r="C741" s="15"/>
+      <c r="C741" s="13"/>
       <c r="D741" s="4"/>
       <c r="E741" s="4"/>
       <c r="F741" s="4"/>
@@ -27692,7 +27690,7 @@
     <row r="742" ht="14.25" customHeight="1">
       <c r="A742" s="4"/>
       <c r="B742" s="4"/>
-      <c r="C742" s="15"/>
+      <c r="C742" s="13"/>
       <c r="D742" s="4"/>
       <c r="E742" s="4"/>
       <c r="F742" s="4"/>
@@ -27720,7 +27718,7 @@
     <row r="743" ht="14.25" customHeight="1">
       <c r="A743" s="4"/>
       <c r="B743" s="4"/>
-      <c r="C743" s="15"/>
+      <c r="C743" s="13"/>
       <c r="D743" s="4"/>
       <c r="E743" s="4"/>
       <c r="F743" s="4"/>
@@ -27748,7 +27746,7 @@
     <row r="744" ht="14.25" customHeight="1">
       <c r="A744" s="4"/>
       <c r="B744" s="4"/>
-      <c r="C744" s="15"/>
+      <c r="C744" s="13"/>
       <c r="D744" s="4"/>
       <c r="E744" s="4"/>
       <c r="F744" s="4"/>
@@ -27776,7 +27774,7 @@
     <row r="745" ht="14.25" customHeight="1">
       <c r="A745" s="4"/>
       <c r="B745" s="4"/>
-      <c r="C745" s="15"/>
+      <c r="C745" s="13"/>
       <c r="D745" s="4"/>
       <c r="E745" s="4"/>
       <c r="F745" s="4"/>
@@ -27804,7 +27802,7 @@
     <row r="746" ht="14.25" customHeight="1">
       <c r="A746" s="4"/>
       <c r="B746" s="4"/>
-      <c r="C746" s="15"/>
+      <c r="C746" s="13"/>
       <c r="D746" s="4"/>
       <c r="E746" s="4"/>
       <c r="F746" s="4"/>
@@ -27832,7 +27830,7 @@
     <row r="747" ht="14.25" customHeight="1">
       <c r="A747" s="4"/>
       <c r="B747" s="4"/>
-      <c r="C747" s="15"/>
+      <c r="C747" s="13"/>
       <c r="D747" s="4"/>
       <c r="E747" s="4"/>
       <c r="F747" s="4"/>
@@ -27860,7 +27858,7 @@
     <row r="748" ht="14.25" customHeight="1">
       <c r="A748" s="4"/>
       <c r="B748" s="4"/>
-      <c r="C748" s="15"/>
+      <c r="C748" s="13"/>
       <c r="D748" s="4"/>
       <c r="E748" s="4"/>
       <c r="F748" s="4"/>
@@ -27888,7 +27886,7 @@
     <row r="749" ht="14.25" customHeight="1">
       <c r="A749" s="4"/>
       <c r="B749" s="4"/>
-      <c r="C749" s="15"/>
+      <c r="C749" s="13"/>
       <c r="D749" s="4"/>
       <c r="E749" s="4"/>
       <c r="F749" s="4"/>
@@ -27916,7 +27914,7 @@
     <row r="750" ht="14.25" customHeight="1">
       <c r="A750" s="4"/>
       <c r="B750" s="4"/>
-      <c r="C750" s="15"/>
+      <c r="C750" s="13"/>
       <c r="D750" s="4"/>
       <c r="E750" s="4"/>
       <c r="F750" s="4"/>
@@ -27944,7 +27942,7 @@
     <row r="751" ht="14.25" customHeight="1">
       <c r="A751" s="4"/>
       <c r="B751" s="4"/>
-      <c r="C751" s="15"/>
+      <c r="C751" s="13"/>
       <c r="D751" s="4"/>
       <c r="E751" s="4"/>
       <c r="F751" s="4"/>
@@ -27972,7 +27970,7 @@
     <row r="752" ht="14.25" customHeight="1">
       <c r="A752" s="4"/>
       <c r="B752" s="4"/>
-      <c r="C752" s="15"/>
+      <c r="C752" s="13"/>
       <c r="D752" s="4"/>
       <c r="E752" s="4"/>
       <c r="F752" s="4"/>
@@ -28000,7 +27998,7 @@
     <row r="753" ht="14.25" customHeight="1">
       <c r="A753" s="4"/>
       <c r="B753" s="4"/>
-      <c r="C753" s="15"/>
+      <c r="C753" s="13"/>
       <c r="D753" s="4"/>
       <c r="E753" s="4"/>
       <c r="F753" s="4"/>
@@ -28028,7 +28026,7 @@
     <row r="754" ht="14.25" customHeight="1">
       <c r="A754" s="4"/>
       <c r="B754" s="4"/>
-      <c r="C754" s="15"/>
+      <c r="C754" s="13"/>
       <c r="D754" s="4"/>
       <c r="E754" s="4"/>
       <c r="F754" s="4"/>
@@ -28056,7 +28054,7 @@
     <row r="755" ht="14.25" customHeight="1">
       <c r="A755" s="4"/>
       <c r="B755" s="4"/>
-      <c r="C755" s="15"/>
+      <c r="C755" s="13"/>
       <c r="D755" s="4"/>
       <c r="E755" s="4"/>
       <c r="F755" s="4"/>
@@ -28084,7 +28082,7 @@
     <row r="756" ht="14.25" customHeight="1">
       <c r="A756" s="4"/>
       <c r="B756" s="4"/>
-      <c r="C756" s="15"/>
+      <c r="C756" s="13"/>
       <c r="D756" s="4"/>
       <c r="E756" s="4"/>
       <c r="F756" s="4"/>
@@ -28112,7 +28110,7 @@
     <row r="757" ht="14.25" customHeight="1">
       <c r="A757" s="4"/>
       <c r="B757" s="4"/>
-      <c r="C757" s="15"/>
+      <c r="C757" s="13"/>
       <c r="D757" s="4"/>
       <c r="E757" s="4"/>
       <c r="F757" s="4"/>
@@ -28140,7 +28138,7 @@
     <row r="758" ht="14.25" customHeight="1">
       <c r="A758" s="4"/>
       <c r="B758" s="4"/>
-      <c r="C758" s="15"/>
+      <c r="C758" s="13"/>
       <c r="D758" s="4"/>
       <c r="E758" s="4"/>
       <c r="F758" s="4"/>
@@ -28168,7 +28166,7 @@
     <row r="759" ht="14.25" customHeight="1">
       <c r="A759" s="4"/>
       <c r="B759" s="4"/>
-      <c r="C759" s="15"/>
+      <c r="C759" s="13"/>
       <c r="D759" s="4"/>
       <c r="E759" s="4"/>
       <c r="F759" s="4"/>
@@ -28196,7 +28194,7 @@
     <row r="760" ht="14.25" customHeight="1">
       <c r="A760" s="4"/>
       <c r="B760" s="4"/>
-      <c r="C760" s="15"/>
+      <c r="C760" s="13"/>
       <c r="D760" s="4"/>
       <c r="E760" s="4"/>
       <c r="F760" s="4"/>
@@ -28224,7 +28222,7 @@
     <row r="761" ht="14.25" customHeight="1">
       <c r="A761" s="4"/>
       <c r="B761" s="4"/>
-      <c r="C761" s="15"/>
+      <c r="C761" s="13"/>
       <c r="D761" s="4"/>
       <c r="E761" s="4"/>
       <c r="F761" s="4"/>
@@ -28252,7 +28250,7 @@
     <row r="762" ht="14.25" customHeight="1">
       <c r="A762" s="4"/>
       <c r="B762" s="4"/>
-      <c r="C762" s="15"/>
+      <c r="C762" s="13"/>
       <c r="D762" s="4"/>
       <c r="E762" s="4"/>
       <c r="F762" s="4"/>
@@ -28280,7 +28278,7 @@
     <row r="763" ht="14.25" customHeight="1">
       <c r="A763" s="4"/>
       <c r="B763" s="4"/>
-      <c r="C763" s="15"/>
+      <c r="C763" s="13"/>
       <c r="D763" s="4"/>
       <c r="E763" s="4"/>
       <c r="F763" s="4"/>
@@ -28308,7 +28306,7 @@
     <row r="764" ht="14.25" customHeight="1">
       <c r="A764" s="4"/>
       <c r="B764" s="4"/>
-      <c r="C764" s="15"/>
+      <c r="C764" s="13"/>
       <c r="D764" s="4"/>
       <c r="E764" s="4"/>
       <c r="F764" s="4"/>
@@ -28336,7 +28334,7 @@
     <row r="765" ht="14.25" customHeight="1">
       <c r="A765" s="4"/>
       <c r="B765" s="4"/>
-      <c r="C765" s="15"/>
+      <c r="C765" s="13"/>
       <c r="D765" s="4"/>
       <c r="E765" s="4"/>
       <c r="F765" s="4"/>
@@ -28364,7 +28362,7 @@
     <row r="766" ht="14.25" customHeight="1">
       <c r="A766" s="4"/>
       <c r="B766" s="4"/>
-      <c r="C766" s="15"/>
+      <c r="C766" s="13"/>
       <c r="D766" s="4"/>
       <c r="E766" s="4"/>
       <c r="F766" s="4"/>
@@ -28392,7 +28390,7 @@
     <row r="767" ht="14.25" customHeight="1">
       <c r="A767" s="4"/>
       <c r="B767" s="4"/>
-      <c r="C767" s="15"/>
+      <c r="C767" s="13"/>
       <c r="D767" s="4"/>
       <c r="E767" s="4"/>
       <c r="F767" s="4"/>
@@ -28420,7 +28418,7 @@
     <row r="768" ht="14.25" customHeight="1">
       <c r="A768" s="4"/>
       <c r="B768" s="4"/>
-      <c r="C768" s="15"/>
+      <c r="C768" s="13"/>
       <c r="D768" s="4"/>
       <c r="E768" s="4"/>
       <c r="F768" s="4"/>
@@ -28448,7 +28446,7 @@
     <row r="769" ht="14.25" customHeight="1">
       <c r="A769" s="4"/>
       <c r="B769" s="4"/>
-      <c r="C769" s="15"/>
+      <c r="C769" s="13"/>
       <c r="D769" s="4"/>
       <c r="E769" s="4"/>
       <c r="F769" s="4"/>
@@ -28476,7 +28474,7 @@
     <row r="770" ht="14.25" customHeight="1">
       <c r="A770" s="4"/>
       <c r="B770" s="4"/>
-      <c r="C770" s="15"/>
+      <c r="C770" s="13"/>
       <c r="D770" s="4"/>
       <c r="E770" s="4"/>
       <c r="F770" s="4"/>
@@ -28504,7 +28502,7 @@
     <row r="771" ht="14.25" customHeight="1">
       <c r="A771" s="4"/>
       <c r="B771" s="4"/>
-      <c r="C771" s="15"/>
+      <c r="C771" s="13"/>
       <c r="D771" s="4"/>
       <c r="E771" s="4"/>
       <c r="F771" s="4"/>
@@ -28532,7 +28530,7 @@
     <row r="772" ht="14.25" customHeight="1">
       <c r="A772" s="4"/>
       <c r="B772" s="4"/>
-      <c r="C772" s="15"/>
+      <c r="C772" s="13"/>
       <c r="D772" s="4"/>
       <c r="E772" s="4"/>
       <c r="F772" s="4"/>
@@ -28560,7 +28558,7 @@
     <row r="773" ht="14.25" customHeight="1">
       <c r="A773" s="4"/>
       <c r="B773" s="4"/>
-      <c r="C773" s="15"/>
+      <c r="C773" s="13"/>
       <c r="D773" s="4"/>
       <c r="E773" s="4"/>
       <c r="F773" s="4"/>
@@ -28588,7 +28586,7 @@
     <row r="774" ht="14.25" customHeight="1">
       <c r="A774" s="4"/>
       <c r="B774" s="4"/>
-      <c r="C774" s="15"/>
+      <c r="C774" s="13"/>
       <c r="D774" s="4"/>
       <c r="E774" s="4"/>
       <c r="F774" s="4"/>
@@ -28616,7 +28614,7 @@
     <row r="775" ht="14.25" customHeight="1">
       <c r="A775" s="4"/>
       <c r="B775" s="4"/>
-      <c r="C775" s="15"/>
+      <c r="C775" s="13"/>
       <c r="D775" s="4"/>
       <c r="E775" s="4"/>
       <c r="F775" s="4"/>
@@ -28644,7 +28642,7 @@
     <row r="776" ht="14.25" customHeight="1">
       <c r="A776" s="4"/>
       <c r="B776" s="4"/>
-      <c r="C776" s="15"/>
+      <c r="C776" s="13"/>
       <c r="D776" s="4"/>
       <c r="E776" s="4"/>
       <c r="F776" s="4"/>
@@ -28672,7 +28670,7 @@
     <row r="777" ht="14.25" customHeight="1">
       <c r="A777" s="4"/>
       <c r="B777" s="4"/>
-      <c r="C777" s="15"/>
+      <c r="C777" s="13"/>
       <c r="D777" s="4"/>
       <c r="E777" s="4"/>
       <c r="F777" s="4"/>
@@ -28700,7 +28698,7 @@
     <row r="778" ht="14.25" customHeight="1">
       <c r="A778" s="4"/>
       <c r="B778" s="4"/>
-      <c r="C778" s="15"/>
+      <c r="C778" s="13"/>
       <c r="D778" s="4"/>
       <c r="E778" s="4"/>
       <c r="F778" s="4"/>
@@ -28728,7 +28726,7 @@
     <row r="779" ht="14.25" customHeight="1">
       <c r="A779" s="4"/>
       <c r="B779" s="4"/>
-      <c r="C779" s="15"/>
+      <c r="C779" s="13"/>
       <c r="D779" s="4"/>
       <c r="E779" s="4"/>
       <c r="F779" s="4"/>
@@ -28756,7 +28754,7 @@
     <row r="780" ht="14.25" customHeight="1">
       <c r="A780" s="4"/>
       <c r="B780" s="4"/>
-      <c r="C780" s="15"/>
+      <c r="C780" s="13"/>
       <c r="D780" s="4"/>
       <c r="E780" s="4"/>
       <c r="F780" s="4"/>
@@ -28784,7 +28782,7 @@
     <row r="781" ht="14.25" customHeight="1">
       <c r="A781" s="4"/>
       <c r="B781" s="4"/>
-      <c r="C781" s="15"/>
+      <c r="C781" s="13"/>
       <c r="D781" s="4"/>
       <c r="E781" s="4"/>
       <c r="F781" s="4"/>
@@ -28812,7 +28810,7 @@
     <row r="782" ht="14.25" customHeight="1">
       <c r="A782" s="4"/>
       <c r="B782" s="4"/>
-      <c r="C782" s="15"/>
+      <c r="C782" s="13"/>
       <c r="D782" s="4"/>
       <c r="E782" s="4"/>
       <c r="F782" s="4"/>
@@ -28840,7 +28838,7 @@
     <row r="783" ht="14.25" customHeight="1">
       <c r="A783" s="4"/>
       <c r="B783" s="4"/>
-      <c r="C783" s="15"/>
+      <c r="C783" s="13"/>
       <c r="D783" s="4"/>
       <c r="E783" s="4"/>
       <c r="F783" s="4"/>
@@ -28868,7 +28866,7 @@
     <row r="784" ht="14.25" customHeight="1">
       <c r="A784" s="4"/>
       <c r="B784" s="4"/>
-      <c r="C784" s="15"/>
+      <c r="C784" s="13"/>
       <c r="D784" s="4"/>
       <c r="E784" s="4"/>
       <c r="F784" s="4"/>
@@ -28896,7 +28894,7 @@
     <row r="785" ht="14.25" customHeight="1">
       <c r="A785" s="4"/>
       <c r="B785" s="4"/>
-      <c r="C785" s="15"/>
+      <c r="C785" s="13"/>
       <c r="D785" s="4"/>
       <c r="E785" s="4"/>
       <c r="F785" s="4"/>
@@ -28924,7 +28922,7 @@
     <row r="786" ht="14.25" customHeight="1">
       <c r="A786" s="4"/>
       <c r="B786" s="4"/>
-      <c r="C786" s="15"/>
+      <c r="C786" s="13"/>
       <c r="D786" s="4"/>
       <c r="E786" s="4"/>
       <c r="F786" s="4"/>
@@ -28952,7 +28950,7 @@
     <row r="787" ht="14.25" customHeight="1">
       <c r="A787" s="4"/>
       <c r="B787" s="4"/>
-      <c r="C787" s="15"/>
+      <c r="C787" s="13"/>
       <c r="D787" s="4"/>
       <c r="E787" s="4"/>
       <c r="F787" s="4"/>
@@ -28980,7 +28978,7 @@
     <row r="788" ht="14.25" customHeight="1">
       <c r="A788" s="4"/>
       <c r="B788" s="4"/>
-      <c r="C788" s="15"/>
+      <c r="C788" s="13"/>
       <c r="D788" s="4"/>
       <c r="E788" s="4"/>
       <c r="F788" s="4"/>
@@ -29008,7 +29006,7 @@
     <row r="789" ht="14.25" customHeight="1">
       <c r="A789" s="4"/>
       <c r="B789" s="4"/>
-      <c r="C789" s="15"/>
+      <c r="C789" s="13"/>
       <c r="D789" s="4"/>
       <c r="E789" s="4"/>
       <c r="F789" s="4"/>
@@ -29036,7 +29034,7 @@
     <row r="790" ht="14.25" customHeight="1">
       <c r="A790" s="4"/>
       <c r="B790" s="4"/>
-      <c r="C790" s="15"/>
+      <c r="C790" s="13"/>
       <c r="D790" s="4"/>
       <c r="E790" s="4"/>
       <c r="F790" s="4"/>
@@ -29064,7 +29062,7 @@
     <row r="791" ht="14.25" customHeight="1">
       <c r="A791" s="4"/>
       <c r="B791" s="4"/>
-      <c r="C791" s="15"/>
+      <c r="C791" s="13"/>
       <c r="D791" s="4"/>
       <c r="E791" s="4"/>
       <c r="F791" s="4"/>
@@ -29092,7 +29090,7 @@
     <row r="792" ht="14.25" customHeight="1">
       <c r="A792" s="4"/>
       <c r="B792" s="4"/>
-      <c r="C792" s="15"/>
+      <c r="C792" s="13"/>
       <c r="D792" s="4"/>
       <c r="E792" s="4"/>
       <c r="F792" s="4"/>
@@ -29120,7 +29118,7 @@
     <row r="793" ht="14.25" customHeight="1">
       <c r="A793" s="4"/>
       <c r="B793" s="4"/>
-      <c r="C793" s="15"/>
+      <c r="C793" s="13"/>
       <c r="D793" s="4"/>
       <c r="E793" s="4"/>
       <c r="F793" s="4"/>
@@ -29148,7 +29146,7 @@
     <row r="794" ht="14.25" customHeight="1">
       <c r="A794" s="4"/>
       <c r="B794" s="4"/>
-      <c r="C794" s="15"/>
+      <c r="C794" s="13"/>
       <c r="D794" s="4"/>
       <c r="E794" s="4"/>
       <c r="F794" s="4"/>
@@ -29176,7 +29174,7 @@
     <row r="795" ht="14.25" customHeight="1">
       <c r="A795" s="4"/>
       <c r="B795" s="4"/>
-      <c r="C795" s="15"/>
+      <c r="C795" s="13"/>
       <c r="D795" s="4"/>
       <c r="E795" s="4"/>
       <c r="F795" s="4"/>
@@ -29204,7 +29202,7 @@
     <row r="796" ht="14.25" customHeight="1">
       <c r="A796" s="4"/>
       <c r="B796" s="4"/>
-      <c r="C796" s="15"/>
+      <c r="C796" s="13"/>
       <c r="D796" s="4"/>
       <c r="E796" s="4"/>
       <c r="F796" s="4"/>
@@ -29232,7 +29230,7 @@
     <row r="797" ht="14.25" customHeight="1">
       <c r="A797" s="4"/>
       <c r="B797" s="4"/>
-      <c r="C797" s="15"/>
+      <c r="C797" s="13"/>
       <c r="D797" s="4"/>
       <c r="E797" s="4"/>
       <c r="F797" s="4"/>
@@ -29260,7 +29258,7 @@
     <row r="798" ht="14.25" customHeight="1">
       <c r="A798" s="4"/>
       <c r="B798" s="4"/>
-      <c r="C798" s="15"/>
+      <c r="C798" s="13"/>
       <c r="D798" s="4"/>
       <c r="E798" s="4"/>
       <c r="F798" s="4"/>
@@ -29288,7 +29286,7 @@
     <row r="799" ht="14.25" customHeight="1">
       <c r="A799" s="4"/>
       <c r="B799" s="4"/>
-      <c r="C799" s="15"/>
+      <c r="C799" s="13"/>
       <c r="D799" s="4"/>
       <c r="E799" s="4"/>
       <c r="F799" s="4"/>
@@ -29316,7 +29314,7 @@
     <row r="800" ht="14.25" customHeight="1">
       <c r="A800" s="4"/>
       <c r="B800" s="4"/>
-      <c r="C800" s="15"/>
+      <c r="C800" s="13"/>
       <c r="D800" s="4"/>
       <c r="E800" s="4"/>
       <c r="F800" s="4"/>
@@ -29344,7 +29342,7 @@
     <row r="801" ht="14.25" customHeight="1">
       <c r="A801" s="4"/>
       <c r="B801" s="4"/>
-      <c r="C801" s="15"/>
+      <c r="C801" s="13"/>
       <c r="D801" s="4"/>
       <c r="E801" s="4"/>
       <c r="F801" s="4"/>
@@ -29372,7 +29370,7 @@
     <row r="802" ht="14.25" customHeight="1">
       <c r="A802" s="4"/>
       <c r="B802" s="4"/>
-      <c r="C802" s="15"/>
+      <c r="C802" s="13"/>
       <c r="D802" s="4"/>
       <c r="E802" s="4"/>
       <c r="F802" s="4"/>
@@ -29400,7 +29398,7 @@
     <row r="803" ht="14.25" customHeight="1">
       <c r="A803" s="4"/>
       <c r="B803" s="4"/>
-      <c r="C803" s="15"/>
+      <c r="C803" s="13"/>
       <c r="D803" s="4"/>
       <c r="E803" s="4"/>
       <c r="F803" s="4"/>
@@ -29428,7 +29426,7 @@
     <row r="804" ht="14.25" customHeight="1">
       <c r="A804" s="4"/>
       <c r="B804" s="4"/>
-      <c r="C804" s="15"/>
+      <c r="C804" s="13"/>
       <c r="D804" s="4"/>
       <c r="E804" s="4"/>
       <c r="F804" s="4"/>
@@ -29456,7 +29454,7 @@
     <row r="805" ht="14.25" customHeight="1">
       <c r="A805" s="4"/>
       <c r="B805" s="4"/>
-      <c r="C805" s="15"/>
+      <c r="C805" s="13"/>
       <c r="D805" s="4"/>
       <c r="E805" s="4"/>
       <c r="F805" s="4"/>
@@ -29484,7 +29482,7 @@
     <row r="806" ht="14.25" customHeight="1">
       <c r="A806" s="4"/>
       <c r="B806" s="4"/>
-      <c r="C806" s="15"/>
+      <c r="C806" s="13"/>
       <c r="D806" s="4"/>
       <c r="E806" s="4"/>
       <c r="F806" s="4"/>
@@ -29512,7 +29510,7 @@
     <row r="807" ht="14.25" customHeight="1">
       <c r="A807" s="4"/>
       <c r="B807" s="4"/>
-      <c r="C807" s="15"/>
+      <c r="C807" s="13"/>
       <c r="D807" s="4"/>
       <c r="E807" s="4"/>
       <c r="F807" s="4"/>
@@ -29540,7 +29538,7 @@
     <row r="808" ht="14.25" customHeight="1">
       <c r="A808" s="4"/>
       <c r="B808" s="4"/>
-      <c r="C808" s="15"/>
+      <c r="C808" s="13"/>
       <c r="D808" s="4"/>
       <c r="E808" s="4"/>
       <c r="F808" s="4"/>
@@ -29568,7 +29566,7 @@
     <row r="809" ht="14.25" customHeight="1">
       <c r="A809" s="4"/>
       <c r="B809" s="4"/>
-      <c r="C809" s="15"/>
+      <c r="C809" s="13"/>
       <c r="D809" s="4"/>
       <c r="E809" s="4"/>
       <c r="F809" s="4"/>
@@ -29596,7 +29594,7 @@
     <row r="810" ht="14.25" customHeight="1">
       <c r="A810" s="4"/>
       <c r="B810" s="4"/>
-      <c r="C810" s="15"/>
+      <c r="C810" s="13"/>
       <c r="D810" s="4"/>
       <c r="E810" s="4"/>
       <c r="F810" s="4"/>
@@ -29624,7 +29622,7 @@
     <row r="811" ht="14.25" customHeight="1">
       <c r="A811" s="4"/>
       <c r="B811" s="4"/>
-      <c r="C811" s="15"/>
+      <c r="C811" s="13"/>
       <c r="D811" s="4"/>
       <c r="E811" s="4"/>
       <c r="F811" s="4"/>
@@ -29652,7 +29650,7 @@
     <row r="812" ht="14.25" customHeight="1">
       <c r="A812" s="4"/>
       <c r="B812" s="4"/>
-      <c r="C812" s="15"/>
+      <c r="C812" s="13"/>
       <c r="D812" s="4"/>
       <c r="E812" s="4"/>
       <c r="F812" s="4"/>
@@ -29680,7 +29678,7 @@
     <row r="813" ht="14.25" customHeight="1">
       <c r="A813" s="4"/>
       <c r="B813" s="4"/>
-      <c r="C813" s="15"/>
+      <c r="C813" s="13"/>
       <c r="D813" s="4"/>
       <c r="E813" s="4"/>
       <c r="F813" s="4"/>
@@ -29708,7 +29706,7 @@
     <row r="814" ht="14.25" customHeight="1">
       <c r="A814" s="4"/>
       <c r="B814" s="4"/>
-      <c r="C814" s="15"/>
+      <c r="C814" s="13"/>
       <c r="D814" s="4"/>
       <c r="E814" s="4"/>
       <c r="F814" s="4"/>
@@ -29736,7 +29734,7 @@
     <row r="815" ht="14.25" customHeight="1">
       <c r="A815" s="4"/>
       <c r="B815" s="4"/>
-      <c r="C815" s="15"/>
+      <c r="C815" s="13"/>
       <c r="D815" s="4"/>
       <c r="E815" s="4"/>
       <c r="F815" s="4"/>
@@ -29764,7 +29762,7 @@
     <row r="816" ht="14.25" customHeight="1">
       <c r="A816" s="4"/>
       <c r="B816" s="4"/>
-      <c r="C816" s="15"/>
+      <c r="C816" s="13"/>
       <c r="D816" s="4"/>
       <c r="E816" s="4"/>
       <c r="F816" s="4"/>
@@ -29792,7 +29790,7 @@
     <row r="817" ht="14.25" customHeight="1">
       <c r="A817" s="4"/>
       <c r="B817" s="4"/>
-      <c r="C817" s="15"/>
+      <c r="C817" s="13"/>
       <c r="D817" s="4"/>
       <c r="E817" s="4"/>
       <c r="F817" s="4"/>
@@ -29820,7 +29818,7 @@
     <row r="818" ht="14.25" customHeight="1">
       <c r="A818" s="4"/>
       <c r="B818" s="4"/>
-      <c r="C818" s="15"/>
+      <c r="C818" s="13"/>
       <c r="D818" s="4"/>
       <c r="E818" s="4"/>
       <c r="F818" s="4"/>
@@ -29848,7 +29846,7 @@
     <row r="819" ht="14.25" customHeight="1">
       <c r="A819" s="4"/>
       <c r="B819" s="4"/>
-      <c r="C819" s="15"/>
+      <c r="C819" s="13"/>
       <c r="D819" s="4"/>
       <c r="E819" s="4"/>
       <c r="F819" s="4"/>
@@ -29876,7 +29874,7 @@
     <row r="820" ht="14.25" customHeight="1">
       <c r="A820" s="4"/>
       <c r="B820" s="4"/>
-      <c r="C820" s="15"/>
+      <c r="C820" s="13"/>
       <c r="D820" s="4"/>
       <c r="E820" s="4"/>
       <c r="F820" s="4"/>
@@ -29904,7 +29902,7 @@
     <row r="821" ht="14.25" customHeight="1">
       <c r="A821" s="4"/>
       <c r="B821" s="4"/>
-      <c r="C821" s="15"/>
+      <c r="C821" s="13"/>
       <c r="D821" s="4"/>
       <c r="E821" s="4"/>
       <c r="F821" s="4"/>
@@ -29932,7 +29930,7 @@
     <row r="822" ht="14.25" customHeight="1">
       <c r="A822" s="4"/>
       <c r="B822" s="4"/>
-      <c r="C822" s="15"/>
+      <c r="C822" s="13"/>
       <c r="D822" s="4"/>
       <c r="E822" s="4"/>
       <c r="F822" s="4"/>
@@ -29960,7 +29958,7 @@
     <row r="823" ht="14.25" customHeight="1">
       <c r="A823" s="4"/>
       <c r="B823" s="4"/>
-      <c r="C823" s="15"/>
+      <c r="C823" s="13"/>
       <c r="D823" s="4"/>
       <c r="E823" s="4"/>
       <c r="F823" s="4"/>
@@ -29988,7 +29986,7 @@
     <row r="824" ht="14.25" customHeight="1">
       <c r="A824" s="4"/>
       <c r="B824" s="4"/>
-      <c r="C824" s="15"/>
+      <c r="C824" s="13"/>
       <c r="D824" s="4"/>
       <c r="E824" s="4"/>
       <c r="F824" s="4"/>
@@ -30016,7 +30014,7 @@
     <row r="825" ht="14.25" customHeight="1">
       <c r="A825" s="4"/>
       <c r="B825" s="4"/>
-      <c r="C825" s="15"/>
+      <c r="C825" s="13"/>
       <c r="D825" s="4"/>
       <c r="E825" s="4"/>
       <c r="F825" s="4"/>
@@ -30044,7 +30042,7 @@
     <row r="826" ht="14.25" customHeight="1">
       <c r="A826" s="4"/>
       <c r="B826" s="4"/>
-      <c r="C826" s="15"/>
+      <c r="C826" s="13"/>
       <c r="D826" s="4"/>
       <c r="E826" s="4"/>
       <c r="F826" s="4"/>
@@ -30072,7 +30070,7 @@
     <row r="827" ht="14.25" customHeight="1">
       <c r="A827" s="4"/>
       <c r="B827" s="4"/>
-      <c r="C827" s="15"/>
+      <c r="C827" s="13"/>
       <c r="D827" s="4"/>
       <c r="E827" s="4"/>
       <c r="F827" s="4"/>
@@ -30100,7 +30098,7 @@
     <row r="828" ht="14.25" customHeight="1">
       <c r="A828" s="4"/>
       <c r="B828" s="4"/>
-      <c r="C828" s="15"/>
+      <c r="C828" s="13"/>
       <c r="D828" s="4"/>
       <c r="E828" s="4"/>
       <c r="F828" s="4"/>
@@ -30128,7 +30126,7 @@
     <row r="829" ht="14.25" customHeight="1">
       <c r="A829" s="4"/>
       <c r="B829" s="4"/>
-      <c r="C829" s="15"/>
+      <c r="C829" s="13"/>
       <c r="D829" s="4"/>
       <c r="E829" s="4"/>
       <c r="F829" s="4"/>
@@ -30156,7 +30154,7 @@
     <row r="830" ht="14.25" customHeight="1">
       <c r="A830" s="4"/>
       <c r="B830" s="4"/>
-      <c r="C830" s="15"/>
+      <c r="C830" s="13"/>
       <c r="D830" s="4"/>
       <c r="E830" s="4"/>
       <c r="F830" s="4"/>
@@ -30184,7 +30182,7 @@
     <row r="831" ht="14.25" customHeight="1">
       <c r="A831" s="4"/>
       <c r="B831" s="4"/>
-      <c r="C831" s="15"/>
+      <c r="C831" s="13"/>
       <c r="D831" s="4"/>
       <c r="E831" s="4"/>
       <c r="F831" s="4"/>
@@ -30212,7 +30210,7 @@
     <row r="832" ht="14.25" customHeight="1">
       <c r="A832" s="4"/>
       <c r="B832" s="4"/>
-      <c r="C832" s="15"/>
+      <c r="C832" s="13"/>
       <c r="D832" s="4"/>
       <c r="E832" s="4"/>
       <c r="F832" s="4"/>
@@ -30240,7 +30238,7 @@
     <row r="833" ht="14.25" customHeight="1">
       <c r="A833" s="4"/>
       <c r="B833" s="4"/>
-      <c r="C833" s="15"/>
+      <c r="C833" s="13"/>
       <c r="D833" s="4"/>
       <c r="E833" s="4"/>
       <c r="F833" s="4"/>
@@ -30268,7 +30266,7 @@
     <row r="834" ht="14.25" customHeight="1">
       <c r="A834" s="4"/>
       <c r="B834" s="4"/>
-      <c r="C834" s="15"/>
+      <c r="C834" s="13"/>
       <c r="D834" s="4"/>
       <c r="E834" s="4"/>
       <c r="F834" s="4"/>
@@ -30296,7 +30294,7 @@
     <row r="835" ht="14.25" customHeight="1">
       <c r="A835" s="4"/>
       <c r="B835" s="4"/>
-      <c r="C835" s="15"/>
+      <c r="C835" s="13"/>
       <c r="D835" s="4"/>
       <c r="E835" s="4"/>
       <c r="F835" s="4"/>
@@ -30324,7 +30322,7 @@
     <row r="836" ht="14.25" customHeight="1">
       <c r="A836" s="4"/>
       <c r="B836" s="4"/>
-      <c r="C836" s="15"/>
+      <c r="C836" s="13"/>
       <c r="D836" s="4"/>
       <c r="E836" s="4"/>
       <c r="F836" s="4"/>
@@ -30352,7 +30350,7 @@
     <row r="837" ht="14.25" customHeight="1">
       <c r="A837" s="4"/>
       <c r="B837" s="4"/>
-      <c r="C837" s="15"/>
+      <c r="C837" s="13"/>
       <c r="D837" s="4"/>
       <c r="E837" s="4"/>
       <c r="F837" s="4"/>
@@ -30380,7 +30378,7 @@
     <row r="838" ht="14.25" customHeight="1">
       <c r="A838" s="4"/>
       <c r="B838" s="4"/>
-      <c r="C838" s="15"/>
+      <c r="C838" s="13"/>
       <c r="D838" s="4"/>
       <c r="E838" s="4"/>
       <c r="F838" s="4"/>
@@ -30408,7 +30406,7 @@
     <row r="839" ht="14.25" customHeight="1">
       <c r="A839" s="4"/>
       <c r="B839" s="4"/>
-      <c r="C839" s="15"/>
+      <c r="C839" s="13"/>
       <c r="D839" s="4"/>
       <c r="E839" s="4"/>
       <c r="F839" s="4"/>
@@ -30436,7 +30434,7 @@
     <row r="840" ht="14.25" customHeight="1">
       <c r="A840" s="4"/>
       <c r="B840" s="4"/>
-      <c r="C840" s="15"/>
+      <c r="C840" s="13"/>
       <c r="D840" s="4"/>
       <c r="E840" s="4"/>
       <c r="F840" s="4"/>
@@ -30464,7 +30462,7 @@
     <row r="841" ht="14.25" customHeight="1">
       <c r="A841" s="4"/>
       <c r="B841" s="4"/>
-      <c r="C841" s="15"/>
+      <c r="C841" s="13"/>
       <c r="D841" s="4"/>
       <c r="E841" s="4"/>
       <c r="F841" s="4"/>
@@ -30492,7 +30490,7 @@
     <row r="842" ht="14.25" customHeight="1">
       <c r="A842" s="4"/>
       <c r="B842" s="4"/>
-      <c r="C842" s="15"/>
+      <c r="C842" s="13"/>
       <c r="D842" s="4"/>
       <c r="E842" s="4"/>
       <c r="F842" s="4"/>
@@ -30520,7 +30518,7 @@
     <row r="843" ht="14.25" customHeight="1">
       <c r="A843" s="4"/>
       <c r="B843" s="4"/>
-      <c r="C843" s="15"/>
+      <c r="C843" s="13"/>
       <c r="D843" s="4"/>
       <c r="E843" s="4"/>
       <c r="F843" s="4"/>
@@ -30548,7 +30546,7 @@
     <row r="844" ht="14.25" customHeight="1">
       <c r="A844" s="4"/>
       <c r="B844" s="4"/>
-      <c r="C844" s="15"/>
+      <c r="C844" s="13"/>
       <c r="D844" s="4"/>
       <c r="E844" s="4"/>
       <c r="F844" s="4"/>
@@ -30576,7 +30574,7 @@
     <row r="845" ht="14.25" customHeight="1">
       <c r="A845" s="4"/>
       <c r="B845" s="4"/>
-      <c r="C845" s="15"/>
+      <c r="C845" s="13"/>
       <c r="D845" s="4"/>
       <c r="E845" s="4"/>
       <c r="F845" s="4"/>
@@ -30604,7 +30602,7 @@
     <row r="846" ht="14.25" customHeight="1">
       <c r="A846" s="4"/>
       <c r="B846" s="4"/>
-      <c r="C846" s="15"/>
+      <c r="C846" s="13"/>
       <c r="D846" s="4"/>
       <c r="E846" s="4"/>
       <c r="F846" s="4"/>
@@ -30632,7 +30630,7 @@
     <row r="847" ht="14.25" customHeight="1">
       <c r="A847" s="4"/>
       <c r="B847" s="4"/>
-      <c r="C847" s="15"/>
+      <c r="C847" s="13"/>
       <c r="D847" s="4"/>
       <c r="E847" s="4"/>
       <c r="F847" s="4"/>
@@ -30660,7 +30658,7 @@
     <row r="848" ht="14.25" customHeight="1">
       <c r="A848" s="4"/>
       <c r="B848" s="4"/>
-      <c r="C848" s="15"/>
+      <c r="C848" s="13"/>
       <c r="D848" s="4"/>
       <c r="E848" s="4"/>
       <c r="F848" s="4"/>
@@ -30688,7 +30686,7 @@
     <row r="849" ht="14.25" customHeight="1">
       <c r="A849" s="4"/>
       <c r="B849" s="4"/>
-      <c r="C849" s="15"/>
+      <c r="C849" s="13"/>
       <c r="D849" s="4"/>
       <c r="E849" s="4"/>
       <c r="F849" s="4"/>
@@ -30716,7 +30714,7 @@
     <row r="850" ht="14.25" customHeight="1">
       <c r="A850" s="4"/>
       <c r="B850" s="4"/>
-      <c r="C850" s="15"/>
+      <c r="C850" s="13"/>
       <c r="D850" s="4"/>
       <c r="E850" s="4"/>
       <c r="F850" s="4"/>
@@ -30744,7 +30742,7 @@
     <row r="851" ht="14.25" customHeight="1">
       <c r="A851" s="4"/>
       <c r="B851" s="4"/>
-      <c r="C851" s="15"/>
+      <c r="C851" s="13"/>
       <c r="D851" s="4"/>
       <c r="E851" s="4"/>
       <c r="F851" s="4"/>
@@ -30772,7 +30770,7 @@
     <row r="852" ht="14.25" customHeight="1">
       <c r="A852" s="4"/>
       <c r="B852" s="4"/>
-      <c r="C852" s="15"/>
+      <c r="C852" s="13"/>
       <c r="D852" s="4"/>
       <c r="E852" s="4"/>
       <c r="F852" s="4"/>
@@ -30800,7 +30798,7 @@
     <row r="853" ht="14.25" customHeight="1">
       <c r="A853" s="4"/>
       <c r="B853" s="4"/>
-      <c r="C853" s="15"/>
+      <c r="C853" s="13"/>
       <c r="D853" s="4"/>
       <c r="E853" s="4"/>
       <c r="F853" s="4"/>
@@ -30828,7 +30826,7 @@
     <row r="854" ht="14.25" customHeight="1">
       <c r="A854" s="4"/>
       <c r="B854" s="4"/>
-      <c r="C854" s="15"/>
+      <c r="C854" s="13"/>
       <c r="D854" s="4"/>
       <c r="E854" s="4"/>
       <c r="F854" s="4"/>
@@ -30856,7 +30854,7 @@
     <row r="855" ht="14.25" customHeight="1">
       <c r="A855" s="4"/>
       <c r="B855" s="4"/>
-      <c r="C855" s="15"/>
+      <c r="C855" s="13"/>
       <c r="D855" s="4"/>
       <c r="E855" s="4"/>
       <c r="F855" s="4"/>
@@ -30884,7 +30882,7 @@
     <row r="856" ht="14.25" customHeight="1">
       <c r="A856" s="4"/>
       <c r="B856" s="4"/>
-      <c r="C856" s="15"/>
+      <c r="C856" s="13"/>
       <c r="D856" s="4"/>
       <c r="E856" s="4"/>
       <c r="F856" s="4"/>
@@ -30912,7 +30910,7 @@
     <row r="857" ht="14.25" customHeight="1">
       <c r="A857" s="4"/>
       <c r="B857" s="4"/>
-      <c r="C857" s="15"/>
+      <c r="C857" s="13"/>
       <c r="D857" s="4"/>
       <c r="E857" s="4"/>
       <c r="F857" s="4"/>
@@ -30940,7 +30938,7 @@
     <row r="858" ht="14.25" customHeight="1">
       <c r="A858" s="4"/>
       <c r="B858" s="4"/>
-      <c r="C858" s="15"/>
+      <c r="C858" s="13"/>
       <c r="D858" s="4"/>
       <c r="E858" s="4"/>
       <c r="F858" s="4"/>
@@ -30968,7 +30966,7 @@
     <row r="859" ht="14.25" customHeight="1">
       <c r="A859" s="4"/>
       <c r="B859" s="4"/>
-      <c r="C859" s="15"/>
+      <c r="C859" s="13"/>
       <c r="D859" s="4"/>
       <c r="E859" s="4"/>
       <c r="F859" s="4"/>
@@ -30996,7 +30994,7 @@
     <row r="860" ht="14.25" customHeight="1">
       <c r="A860" s="4"/>
       <c r="B860" s="4"/>
-      <c r="C860" s="15"/>
+      <c r="C860" s="13"/>
       <c r="D860" s="4"/>
       <c r="E860" s="4"/>
       <c r="F860" s="4"/>
@@ -31024,7 +31022,7 @@
     <row r="861" ht="14.25" customHeight="1">
       <c r="A861" s="4"/>
       <c r="B861" s="4"/>
-      <c r="C861" s="15"/>
+      <c r="C861" s="13"/>
       <c r="D861" s="4"/>
       <c r="E861" s="4"/>
       <c r="F861" s="4"/>
@@ -31052,7 +31050,7 @@
     <row r="862" ht="14.25" customHeight="1">
       <c r="A862" s="4"/>
       <c r="B862" s="4"/>
-      <c r="C862" s="15"/>
+      <c r="C862" s="13"/>
       <c r="D862" s="4"/>
       <c r="E862" s="4"/>
       <c r="F862" s="4"/>
@@ -31080,7 +31078,7 @@
     <row r="863" ht="14.25" customHeight="1">
       <c r="A863" s="4"/>
       <c r="B863" s="4"/>
-      <c r="C863" s="15"/>
+      <c r="C863" s="13"/>
       <c r="D863" s="4"/>
       <c r="E863" s="4"/>
       <c r="F863" s="4"/>
@@ -31108,7 +31106,7 @@
     <row r="864" ht="14.25" customHeight="1">
       <c r="A864" s="4"/>
       <c r="B864" s="4"/>
-      <c r="C864" s="15"/>
+      <c r="C864" s="13"/>
       <c r="D864" s="4"/>
       <c r="E864" s="4"/>
       <c r="F864" s="4"/>
@@ -31136,7 +31134,7 @@
     <row r="865" ht="14.25" customHeight="1">
       <c r="A865" s="4"/>
       <c r="B865" s="4"/>
-      <c r="C865" s="15"/>
+      <c r="C865" s="13"/>
       <c r="D865" s="4"/>
       <c r="E865" s="4"/>
       <c r="F865" s="4"/>
@@ -31164,7 +31162,7 @@
     <row r="866" ht="14.25" customHeight="1">
       <c r="A866" s="4"/>
       <c r="B866" s="4"/>
-      <c r="C866" s="15"/>
+      <c r="C866" s="13"/>
       <c r="D866" s="4"/>
       <c r="E866" s="4"/>
       <c r="F866" s="4"/>
@@ -31192,7 +31190,7 @@
     <row r="867" ht="14.25" customHeight="1">
       <c r="A867" s="4"/>
       <c r="B867" s="4"/>
-      <c r="C867" s="15"/>
+      <c r="C867" s="13"/>
       <c r="D867" s="4"/>
       <c r="E867" s="4"/>
       <c r="F867" s="4"/>
@@ -31220,7 +31218,7 @@
     <row r="868" ht="14.25" customHeight="1">
       <c r="A868" s="4"/>
       <c r="B868" s="4"/>
-      <c r="C868" s="15"/>
+      <c r="C868" s="13"/>
       <c r="D868" s="4"/>
       <c r="E868" s="4"/>
       <c r="F868" s="4"/>
@@ -31248,7 +31246,7 @@
     <row r="869" ht="14.25" customHeight="1">
       <c r="A869" s="4"/>
       <c r="B869" s="4"/>
-      <c r="C869" s="15"/>
+      <c r="C869" s="13"/>
       <c r="D869" s="4"/>
       <c r="E869" s="4"/>
       <c r="F869" s="4"/>
@@ -31276,7 +31274,7 @@
     <row r="870" ht="14.25" customHeight="1">
       <c r="A870" s="4"/>
       <c r="B870" s="4"/>
-      <c r="C870" s="15"/>
+      <c r="C870" s="13"/>
       <c r="D870" s="4"/>
       <c r="E870" s="4"/>
       <c r="F870" s="4"/>
@@ -31304,7 +31302,7 @@
     <row r="871" ht="14.25" customHeight="1">
       <c r="A871" s="4"/>
       <c r="B871" s="4"/>
-      <c r="C871" s="15"/>
+      <c r="C871" s="13"/>
       <c r="D871" s="4"/>
       <c r="E871" s="4"/>
       <c r="F871" s="4"/>
@@ -31332,7 +31330,7 @@
     <row r="872" ht="14.25" customHeight="1">
       <c r="A872" s="4"/>
       <c r="B872" s="4"/>
-      <c r="C872" s="15"/>
+      <c r="C872" s="13"/>
       <c r="D872" s="4"/>
       <c r="E872" s="4"/>
       <c r="F872" s="4"/>
@@ -31360,7 +31358,7 @@
     <row r="873" ht="14.25" customHeight="1">
       <c r="A873" s="4"/>
       <c r="B873" s="4"/>
-      <c r="C873" s="15"/>
+      <c r="C873" s="13"/>
       <c r="D873" s="4"/>
       <c r="E873" s="4"/>
       <c r="F873" s="4"/>
@@ -31388,7 +31386,7 @@
     <row r="874" ht="14.25" customHeight="1">
       <c r="A874" s="4"/>
       <c r="B874" s="4"/>
-      <c r="C874" s="15"/>
+      <c r="C874" s="13"/>
       <c r="D874" s="4"/>
       <c r="E874" s="4"/>
       <c r="F874" s="4"/>
@@ -31416,7 +31414,7 @@
     <row r="875" ht="14.25" customHeight="1">
       <c r="A875" s="4"/>
       <c r="B875" s="4"/>
-      <c r="C875" s="15"/>
+      <c r="C875" s="13"/>
       <c r="D875" s="4"/>
       <c r="E875" s="4"/>
       <c r="F875" s="4"/>
@@ -31444,7 +31442,7 @@
     <row r="876" ht="14.25" customHeight="1">
       <c r="A876" s="4"/>
       <c r="B876" s="4"/>
-      <c r="C876" s="15"/>
+      <c r="C876" s="13"/>
       <c r="D876" s="4"/>
       <c r="E876" s="4"/>
       <c r="F876" s="4"/>
@@ -31472,7 +31470,7 @@
     <row r="877" ht="14.25" customHeight="1">
       <c r="A877" s="4"/>
       <c r="B877" s="4"/>
-      <c r="C877" s="15"/>
+      <c r="C877" s="13"/>
       <c r="D877" s="4"/>
       <c r="E877" s="4"/>
       <c r="F877" s="4"/>
@@ -31500,7 +31498,7 @@
     <row r="878" ht="14.25" customHeight="1">
       <c r="A878" s="4"/>
       <c r="B878" s="4"/>
-      <c r="C878" s="15"/>
+      <c r="C878" s="13"/>
       <c r="D878" s="4"/>
       <c r="E878" s="4"/>
       <c r="F878" s="4"/>
@@ -31528,7 +31526,7 @@
     <row r="879" ht="14.25" customHeight="1">
       <c r="A879" s="4"/>
       <c r="B879" s="4"/>
-      <c r="C879" s="15"/>
+      <c r="C879" s="13"/>
       <c r="D879" s="4"/>
       <c r="E879" s="4"/>
       <c r="F879" s="4"/>
@@ -31556,7 +31554,7 @@
     <row r="880" ht="14.25" customHeight="1">
       <c r="A880" s="4"/>
       <c r="B880" s="4"/>
-      <c r="C880" s="15"/>
+      <c r="C880" s="13"/>
       <c r="D880" s="4"/>
       <c r="E880" s="4"/>
       <c r="F880" s="4"/>
@@ -31584,7 +31582,7 @@
     <row r="881" ht="14.25" customHeight="1">
       <c r="A881" s="4"/>
       <c r="B881" s="4"/>
-      <c r="C881" s="15"/>
+      <c r="C881" s="13"/>
       <c r="D881" s="4"/>
       <c r="E881" s="4"/>
       <c r="F881" s="4"/>
@@ -31612,7 +31610,7 @@
     <row r="882" ht="14.25" customHeight="1">
       <c r="A882" s="4"/>
       <c r="B882" s="4"/>
-      <c r="C882" s="15"/>
+      <c r="C882" s="13"/>
       <c r="D882" s="4"/>
       <c r="E882" s="4"/>
       <c r="F882" s="4"/>
@@ -31640,7 +31638,7 @@
     <row r="883" ht="14.25" customHeight="1">
       <c r="A883" s="4"/>
       <c r="B883" s="4"/>
-      <c r="C883" s="15"/>
+      <c r="C883" s="13"/>
       <c r="D883" s="4"/>
       <c r="E883" s="4"/>
       <c r="F883" s="4"/>
@@ -31668,7 +31666,7 @@
     <row r="884" ht="14.25" customHeight="1">
       <c r="A884" s="4"/>
       <c r="B884" s="4"/>
-      <c r="C884" s="15"/>
+      <c r="C884" s="13"/>
       <c r="D884" s="4"/>
       <c r="E884" s="4"/>
       <c r="F884" s="4"/>
@@ -31696,7 +31694,7 @@
     <row r="885" ht="14.25" customHeight="1">
       <c r="A885" s="4"/>
       <c r="B885" s="4"/>
-      <c r="C885" s="15"/>
+      <c r="C885" s="13"/>
       <c r="D885" s="4"/>
       <c r="E885" s="4"/>
       <c r="F885" s="4"/>
@@ -31724,7 +31722,7 @@
     <row r="886" ht="14.25" customHeight="1">
       <c r="A886" s="4"/>
       <c r="B886" s="4"/>
-      <c r="C886" s="15"/>
+      <c r="C886" s="13"/>
       <c r="D886" s="4"/>
       <c r="E886" s="4"/>
       <c r="F886" s="4"/>
@@ -31752,7 +31750,7 @@
     <row r="887" ht="14.25" customHeight="1">
       <c r="A887" s="4"/>
       <c r="B887" s="4"/>
-      <c r="C887" s="15"/>
+      <c r="C887" s="13"/>
       <c r="D887" s="4"/>
       <c r="E887" s="4"/>
       <c r="F887" s="4"/>
@@ -31780,7 +31778,7 @@
     <row r="888" ht="14.25" customHeight="1">
       <c r="A888" s="4"/>
       <c r="B888" s="4"/>
-      <c r="C888" s="15"/>
+      <c r="C888" s="13"/>
       <c r="D888" s="4"/>
       <c r="E888" s="4"/>
       <c r="F888" s="4"/>
@@ -31808,7 +31806,7 @@
     <row r="889" ht="14.25" customHeight="1">
       <c r="A889" s="4"/>
       <c r="B889" s="4"/>
-      <c r="C889" s="15"/>
+      <c r="C889" s="13"/>
       <c r="D889" s="4"/>
       <c r="E889" s="4"/>
       <c r="F889" s="4"/>
@@ -31836,7 +31834,7 @@
     <row r="890" ht="14.25" customHeight="1">
       <c r="A890" s="4"/>
       <c r="B890" s="4"/>
-      <c r="C890" s="15"/>
+      <c r="C890" s="13"/>
       <c r="D890" s="4"/>
       <c r="E890" s="4"/>
       <c r="F890" s="4"/>
@@ -31864,7 +31862,7 @@
     <row r="891" ht="14.25" customHeight="1">
       <c r="A891" s="4"/>
       <c r="B891" s="4"/>
-      <c r="C891" s="15"/>
+      <c r="C891" s="13"/>
       <c r="D891" s="4"/>
       <c r="E891" s="4"/>
       <c r="F891" s="4"/>
@@ -31892,7 +31890,7 @@
     <row r="892" ht="14.25" customHeight="1">
       <c r="A892" s="4"/>
       <c r="B892" s="4"/>
-      <c r="C892" s="15"/>
+      <c r="C892" s="13"/>
       <c r="D892" s="4"/>
       <c r="E892" s="4"/>
       <c r="F892" s="4"/>
@@ -31920,7 +31918,7 @@
     <row r="893" ht="14.25" customHeight="1">
       <c r="A893" s="4"/>
       <c r="B893" s="4"/>
-      <c r="C893" s="15"/>
+      <c r="C893" s="13"/>
       <c r="D893" s="4"/>
       <c r="E893" s="4"/>
       <c r="F893" s="4"/>
@@ -31948,7 +31946,7 @@
     <row r="894" ht="14.25" customHeight="1">
       <c r="A894" s="4"/>
       <c r="B894" s="4"/>
-      <c r="C894" s="15"/>
+      <c r="C894" s="13"/>
       <c r="D894" s="4"/>
       <c r="E894" s="4"/>
       <c r="F894" s="4"/>
@@ -31976,7 +31974,7 @@
     <row r="895" ht="14.25" customHeight="1">
       <c r="A895" s="4"/>
       <c r="B895" s="4"/>
-      <c r="C895" s="15"/>
+      <c r="C895" s="13"/>
       <c r="D895" s="4"/>
       <c r="E895" s="4"/>
       <c r="F895" s="4"/>
@@ -32004,7 +32002,7 @@
     <row r="896" ht="14.25" customHeight="1">
       <c r="A896" s="4"/>
       <c r="B896" s="4"/>
-      <c r="C896" s="15"/>
+      <c r="C896" s="13"/>
       <c r="D896" s="4"/>
       <c r="E896" s="4"/>
       <c r="F896" s="4"/>
@@ -32032,7 +32030,7 @@
     <row r="897" ht="14.25" customHeight="1">
       <c r="A897" s="4"/>
       <c r="B897" s="4"/>
-      <c r="C897" s="15"/>
+      <c r="C897" s="13"/>
       <c r="D897" s="4"/>
       <c r="E897" s="4"/>
       <c r="F897" s="4"/>
@@ -32060,7 +32058,7 @@
     <row r="898" ht="14.25" customHeight="1">
       <c r="A898" s="4"/>
       <c r="B898" s="4"/>
-      <c r="C898" s="15"/>
+      <c r="C898" s="13"/>
       <c r="D898" s="4"/>
       <c r="E898" s="4"/>
       <c r="F898" s="4"/>
@@ -32088,7 +32086,7 @@
     <row r="899" ht="14.25" customHeight="1">
       <c r="A899" s="4"/>
       <c r="B899" s="4"/>
-      <c r="C899" s="15"/>
+      <c r="C899" s="13"/>
       <c r="D899" s="4"/>
       <c r="E899" s="4"/>
       <c r="F899" s="4"/>
@@ -32116,7 +32114,7 @@
     <row r="900" ht="14.25" customHeight="1">
       <c r="A900" s="4"/>
       <c r="B900" s="4"/>
-      <c r="C900" s="15"/>
+      <c r="C900" s="13"/>
       <c r="D900" s="4"/>
       <c r="E900" s="4"/>
       <c r="F900" s="4"/>
@@ -32144,7 +32142,7 @@
     <row r="901" ht="14.25" customHeight="1">
       <c r="A901" s="4"/>
       <c r="B901" s="4"/>
-      <c r="C901" s="15"/>
+      <c r="C901" s="13"/>
       <c r="D901" s="4"/>
       <c r="E901" s="4"/>
       <c r="F901" s="4"/>
@@ -32172,7 +32170,7 @@
     <row r="902" ht="14.25" customHeight="1">
       <c r="A902" s="4"/>
       <c r="B902" s="4"/>
-      <c r="C902" s="15"/>
+      <c r="C902" s="13"/>
       <c r="D902" s="4"/>
       <c r="E902" s="4"/>
       <c r="F902" s="4"/>
@@ -32200,7 +32198,7 @@
     <row r="903" ht="14.25" customHeight="1">
       <c r="A903" s="4"/>
       <c r="B903" s="4"/>
-      <c r="C903" s="15"/>
+      <c r="C903" s="13"/>
       <c r="D903" s="4"/>
       <c r="E903" s="4"/>
       <c r="F903" s="4"/>
@@ -32228,7 +32226,7 @@
     <row r="904" ht="14.25" customHeight="1">
       <c r="A904" s="4"/>
       <c r="B904" s="4"/>
-      <c r="C904" s="15"/>
+      <c r="C904" s="13"/>
       <c r="D904" s="4"/>
       <c r="E904" s="4"/>
       <c r="F904" s="4"/>
@@ -32256,7 +32254,7 @@
     <row r="905" ht="14.25" customHeight="1">
       <c r="A905" s="4"/>
       <c r="B905" s="4"/>
-      <c r="C905" s="15"/>
+      <c r="C905" s="13"/>
       <c r="D905" s="4"/>
       <c r="E905" s="4"/>
       <c r="F905" s="4"/>
@@ -32284,7 +32282,7 @@
     <row r="906" ht="14.25" customHeight="1">
       <c r="A906" s="4"/>
       <c r="B906" s="4"/>
-      <c r="C906" s="15"/>
+      <c r="C906" s="13"/>
       <c r="D906" s="4"/>
       <c r="E906" s="4"/>
       <c r="F906" s="4"/>
@@ -32312,7 +32310,7 @@
     <row r="907" ht="14.25" customHeight="1">
       <c r="A907" s="4"/>
       <c r="B907" s="4"/>
-      <c r="C907" s="15"/>
+      <c r="C907" s="13"/>
       <c r="D907" s="4"/>
       <c r="E907" s="4"/>
       <c r="F907" s="4"/>
@@ -32340,7 +32338,7 @@
     <row r="908" ht="14.25" customHeight="1">
       <c r="A908" s="4"/>
       <c r="B908" s="4"/>
-      <c r="C908" s="15"/>
+      <c r="C908" s="13"/>
       <c r="D908" s="4"/>
       <c r="E908" s="4"/>
       <c r="F908" s="4"/>
@@ -32368,7 +32366,7 @@
     <row r="909" ht="14.25" customHeight="1">
       <c r="A909" s="4"/>
       <c r="B909" s="4"/>
-      <c r="C909" s="15"/>
+      <c r="C909" s="13"/>
       <c r="D909" s="4"/>
       <c r="E909" s="4"/>
       <c r="F909" s="4"/>
@@ -32396,7 +32394,7 @@
     <row r="910" ht="14.25" customHeight="1">
       <c r="A910" s="4"/>
       <c r="B910" s="4"/>
-      <c r="C910" s="15"/>
+      <c r="C910" s="13"/>
       <c r="D910" s="4"/>
       <c r="E910" s="4"/>
       <c r="F910" s="4"/>
@@ -32424,7 +32422,7 @@
     <row r="911" ht="14.25" customHeight="1">
       <c r="A911" s="4"/>
       <c r="B911" s="4"/>
-      <c r="C911" s="15"/>
+      <c r="C911" s="13"/>
       <c r="D911" s="4"/>
       <c r="E911" s="4"/>
       <c r="F911" s="4"/>
@@ -32452,7 +32450,7 @@
     <row r="912" ht="14.25" customHeight="1">
       <c r="A912" s="4"/>
       <c r="B912" s="4"/>
-      <c r="C912" s="15"/>
+      <c r="C912" s="13"/>
       <c r="D912" s="4"/>
       <c r="E912" s="4"/>
       <c r="F912" s="4"/>
@@ -32480,7 +32478,7 @@
     <row r="913" ht="14.25" customHeight="1">
       <c r="A913" s="4"/>
       <c r="B913" s="4"/>
-      <c r="C913" s="15"/>
+      <c r="C913" s="13"/>
       <c r="D913" s="4"/>
       <c r="E913" s="4"/>
       <c r="F913" s="4"/>
@@ -32508,7 +32506,7 @@
     <row r="914" ht="14.25" customHeight="1">
       <c r="A914" s="4"/>
       <c r="B914" s="4"/>
-      <c r="C914" s="15"/>
+      <c r="C914" s="13"/>
       <c r="D914" s="4"/>
       <c r="E914" s="4"/>
       <c r="F914" s="4"/>
@@ -32536,7 +32534,7 @@
     <row r="915" ht="14.25" customHeight="1">
       <c r="A915" s="4"/>
       <c r="B915" s="4"/>
-      <c r="C915" s="15"/>
+      <c r="C915" s="13"/>
       <c r="D915" s="4"/>
       <c r="E915" s="4"/>
       <c r="F915" s="4"/>
@@ -32564,7 +32562,7 @@
     <row r="916" ht="14.25" customHeight="1">
       <c r="A916" s="4"/>
       <c r="B916" s="4"/>
-      <c r="C916" s="15"/>
+      <c r="C916" s="13"/>
       <c r="D916" s="4"/>
       <c r="E916" s="4"/>
       <c r="F916" s="4"/>
@@ -32592,7 +32590,7 @@
     <row r="917" ht="14.25" customHeight="1">
       <c r="A917" s="4"/>
       <c r="B917" s="4"/>
-      <c r="C917" s="15"/>
+      <c r="C917" s="13"/>
       <c r="D917" s="4"/>
       <c r="E917" s="4"/>
       <c r="F917" s="4"/>
@@ -32620,7 +32618,7 @@
     <row r="918" ht="14.25" customHeight="1">
       <c r="A918" s="4"/>
       <c r="B918" s="4"/>
-      <c r="C918" s="15"/>
+      <c r="C918" s="13"/>
       <c r="D918" s="4"/>
       <c r="E918" s="4"/>
       <c r="F918" s="4"/>
@@ -32648,7 +32646,7 @@
     <row r="919" ht="14.25" customHeight="1">
       <c r="A919" s="4"/>
       <c r="B919" s="4"/>
-      <c r="C919" s="15"/>
+      <c r="C919" s="13"/>
       <c r="D919" s="4"/>
       <c r="E919" s="4"/>
       <c r="F919" s="4"/>
@@ -32676,7 +32674,7 @@
     <row r="920" ht="14.25" customHeight="1">
       <c r="A920" s="4"/>
       <c r="B920" s="4"/>
-      <c r="C920" s="15"/>
+      <c r="C920" s="13"/>
       <c r="D920" s="4"/>
       <c r="E920" s="4"/>
       <c r="F920" s="4"/>
@@ -32704,7 +32702,7 @@
     <row r="921" ht="14.25" customHeight="1">
       <c r="A921" s="4"/>
       <c r="B921" s="4"/>
-      <c r="C921" s="15"/>
+      <c r="C921" s="13"/>
       <c r="D921" s="4"/>
       <c r="E921" s="4"/>
       <c r="F921" s="4"/>
@@ -32732,7 +32730,7 @@
     <row r="922" ht="14.25" customHeight="1">
       <c r="A922" s="4"/>
       <c r="B922" s="4"/>
-      <c r="C922" s="15"/>
+      <c r="C922" s="13"/>
       <c r="D922" s="4"/>
       <c r="E922" s="4"/>
       <c r="F922" s="4"/>
@@ -32760,7 +32758,7 @@
     <row r="923" ht="14.25" customHeight="1">
       <c r="A923" s="4"/>
       <c r="B923" s="4"/>
-      <c r="C923" s="15"/>
+      <c r="C923" s="13"/>
       <c r="D923" s="4"/>
       <c r="E923" s="4"/>
       <c r="F923" s="4"/>
@@ -32788,7 +32786,7 @@
     <row r="924" ht="14.25" customHeight="1">
       <c r="A924" s="4"/>
       <c r="B924" s="4"/>
-      <c r="C924" s="15"/>
+      <c r="C924" s="13"/>
       <c r="D924" s="4"/>
       <c r="E924" s="4"/>
       <c r="F924" s="4"/>
@@ -32816,7 +32814,7 @@
     <row r="925" ht="14.25" customHeight="1">
       <c r="A925" s="4"/>
       <c r="B925" s="4"/>
-      <c r="C925" s="15"/>
+      <c r="C925" s="13"/>
       <c r="D925" s="4"/>
       <c r="E925" s="4"/>
       <c r="F925" s="4"/>
@@ -32844,7 +32842,7 @@
     <row r="926" ht="14.25" customHeight="1">
       <c r="A926" s="4"/>
       <c r="B926" s="4"/>
-      <c r="C926" s="15"/>
+      <c r="C926" s="13"/>
       <c r="D926" s="4"/>
       <c r="E926" s="4"/>
       <c r="F926" s="4"/>
@@ -32872,7 +32870,7 @@
     <row r="927" ht="14.25" customHeight="1">
       <c r="A927" s="4"/>
       <c r="B927" s="4"/>
-      <c r="C927" s="15"/>
+      <c r="C927" s="13"/>
       <c r="D927" s="4"/>
       <c r="E927" s="4"/>
       <c r="F927" s="4"/>
@@ -32900,7 +32898,7 @@
     <row r="928" ht="14.25" customHeight="1">
       <c r="A928" s="4"/>
       <c r="B928" s="4"/>
-      <c r="C928" s="15"/>
+      <c r="C928" s="13"/>
       <c r="D928" s="4"/>
       <c r="E928" s="4"/>
       <c r="F928" s="4"/>
@@ -32928,7 +32926,7 @@
     <row r="929" ht="14.25" customHeight="1">
       <c r="A929" s="4"/>
       <c r="B929" s="4"/>
-      <c r="C929" s="15"/>
+      <c r="C929" s="13"/>
       <c r="D929" s="4"/>
       <c r="E929" s="4"/>
       <c r="F929" s="4"/>
@@ -32956,7 +32954,7 @@
     <row r="930" ht="14.25" customHeight="1">
       <c r="A930" s="4"/>
       <c r="B930" s="4"/>
-      <c r="C930" s="15"/>
+      <c r="C930" s="13"/>
       <c r="D930" s="4"/>
       <c r="E930" s="4"/>
       <c r="F930" s="4"/>
@@ -32984,7 +32982,7 @@
     <row r="931" ht="14.25" customHeight="1">
       <c r="A931" s="4"/>
       <c r="B931" s="4"/>
-      <c r="C931" s="15"/>
+      <c r="C931" s="13"/>
       <c r="D931" s="4"/>
       <c r="E931" s="4"/>
       <c r="F931" s="4"/>
@@ -33012,7 +33010,7 @@
     <row r="932" ht="14.25" customHeight="1">
       <c r="A932" s="4"/>
       <c r="B932" s="4"/>
-      <c r="C932" s="15"/>
+      <c r="C932" s="13"/>
       <c r="D932" s="4"/>
       <c r="E932" s="4"/>
       <c r="F932" s="4"/>
@@ -33040,7 +33038,7 @@
     <row r="933" ht="14.25" customHeight="1">
       <c r="A933" s="4"/>
       <c r="B933" s="4"/>
-      <c r="C933" s="15"/>
+      <c r="C933" s="13"/>
       <c r="D933" s="4"/>
       <c r="E933" s="4"/>
       <c r="F933" s="4"/>
@@ -33068,7 +33066,7 @@
     <row r="934" ht="14.25" customHeight="1">
       <c r="A934" s="4"/>
       <c r="B934" s="4"/>
-      <c r="C934" s="15"/>
+      <c r="C934" s="13"/>
       <c r="D934" s="4"/>
       <c r="E934" s="4"/>
       <c r="F934" s="4"/>
@@ -33096,7 +33094,7 @@
     <row r="935" ht="14.25" customHeight="1">
       <c r="A935" s="4"/>
       <c r="B935" s="4"/>
-      <c r="C935" s="15"/>
+      <c r="C935" s="13"/>
       <c r="D935" s="4"/>
       <c r="E935" s="4"/>
       <c r="F935" s="4"/>
@@ -33124,7 +33122,7 @@
     <row r="936" ht="14.25" customHeight="1">
       <c r="A936" s="4"/>
       <c r="B936" s="4"/>
-      <c r="C936" s="15"/>
+      <c r="C936" s="13"/>
       <c r="D936" s="4"/>
       <c r="E936" s="4"/>
       <c r="F936" s="4"/>
@@ -33152,7 +33150,7 @@
     <row r="937" ht="14.25" customHeight="1">
       <c r="A937" s="4"/>
       <c r="B937" s="4"/>
-      <c r="C937" s="15"/>
+      <c r="C937" s="13"/>
       <c r="D937" s="4"/>
       <c r="E937" s="4"/>
       <c r="F937" s="4"/>
@@ -33180,7 +33178,7 @@
     <row r="938" ht="14.25" customHeight="1">
       <c r="A938" s="4"/>
       <c r="B938" s="4"/>
-      <c r="C938" s="15"/>
+      <c r="C938" s="13"/>
       <c r="D938" s="4"/>
       <c r="E938" s="4"/>
       <c r="F938" s="4"/>
@@ -33208,7 +33206,7 @@
     <row r="939" ht="14.25" customHeight="1">
       <c r="A939" s="4"/>
       <c r="B939" s="4"/>
-      <c r="C939" s="15"/>
+      <c r="C939" s="13"/>
       <c r="D939" s="4"/>
       <c r="E939" s="4"/>
       <c r="F939" s="4"/>
@@ -33236,7 +33234,7 @@
     <row r="940" ht="14.25" customHeight="1">
       <c r="A940" s="4"/>
       <c r="B940" s="4"/>
-      <c r="C940" s="15"/>
+      <c r="C940" s="13"/>
       <c r="D940" s="4"/>
       <c r="E940" s="4"/>
       <c r="F940" s="4"/>
@@ -33261,118 +33259,6 @@
       <c r="Y940" s="4"/>
       <c r="Z940" s="4"/>
     </row>
-    <row r="941" ht="14.25" customHeight="1">
-      <c r="A941" s="4"/>
-      <c r="B941" s="4"/>
-      <c r="C941" s="15"/>
-      <c r="D941" s="4"/>
-      <c r="E941" s="4"/>
-      <c r="F941" s="4"/>
-      <c r="G941" s="4"/>
-      <c r="H941" s="4"/>
-      <c r="I941" s="4"/>
-      <c r="J941" s="4"/>
-      <c r="K941" s="4"/>
-      <c r="L941" s="4"/>
-      <c r="M941" s="4"/>
-      <c r="N941" s="4"/>
-      <c r="O941" s="4"/>
-      <c r="P941" s="4"/>
-      <c r="Q941" s="4"/>
-      <c r="R941" s="4"/>
-      <c r="S941" s="4"/>
-      <c r="T941" s="4"/>
-      <c r="U941" s="4"/>
-      <c r="V941" s="4"/>
-      <c r="W941" s="4"/>
-      <c r="X941" s="4"/>
-      <c r="Y941" s="4"/>
-      <c r="Z941" s="4"/>
-    </row>
-    <row r="942" ht="14.25" customHeight="1">
-      <c r="A942" s="4"/>
-      <c r="B942" s="4"/>
-      <c r="C942" s="15"/>
-      <c r="D942" s="4"/>
-      <c r="E942" s="4"/>
-      <c r="F942" s="4"/>
-      <c r="G942" s="4"/>
-      <c r="H942" s="4"/>
-      <c r="I942" s="4"/>
-      <c r="J942" s="4"/>
-      <c r="K942" s="4"/>
-      <c r="L942" s="4"/>
-      <c r="M942" s="4"/>
-      <c r="N942" s="4"/>
-      <c r="O942" s="4"/>
-      <c r="P942" s="4"/>
-      <c r="Q942" s="4"/>
-      <c r="R942" s="4"/>
-      <c r="S942" s="4"/>
-      <c r="T942" s="4"/>
-      <c r="U942" s="4"/>
-      <c r="V942" s="4"/>
-      <c r="W942" s="4"/>
-      <c r="X942" s="4"/>
-      <c r="Y942" s="4"/>
-      <c r="Z942" s="4"/>
-    </row>
-    <row r="943" ht="14.25" customHeight="1">
-      <c r="A943" s="4"/>
-      <c r="B943" s="4"/>
-      <c r="C943" s="15"/>
-      <c r="D943" s="4"/>
-      <c r="E943" s="4"/>
-      <c r="F943" s="4"/>
-      <c r="G943" s="4"/>
-      <c r="H943" s="4"/>
-      <c r="I943" s="4"/>
-      <c r="J943" s="4"/>
-      <c r="K943" s="4"/>
-      <c r="L943" s="4"/>
-      <c r="M943" s="4"/>
-      <c r="N943" s="4"/>
-      <c r="O943" s="4"/>
-      <c r="P943" s="4"/>
-      <c r="Q943" s="4"/>
-      <c r="R943" s="4"/>
-      <c r="S943" s="4"/>
-      <c r="T943" s="4"/>
-      <c r="U943" s="4"/>
-      <c r="V943" s="4"/>
-      <c r="W943" s="4"/>
-      <c r="X943" s="4"/>
-      <c r="Y943" s="4"/>
-      <c r="Z943" s="4"/>
-    </row>
-    <row r="944" ht="14.25" customHeight="1">
-      <c r="A944" s="4"/>
-      <c r="B944" s="4"/>
-      <c r="C944" s="15"/>
-      <c r="D944" s="4"/>
-      <c r="E944" s="4"/>
-      <c r="F944" s="4"/>
-      <c r="G944" s="4"/>
-      <c r="H944" s="4"/>
-      <c r="I944" s="4"/>
-      <c r="J944" s="4"/>
-      <c r="K944" s="4"/>
-      <c r="L944" s="4"/>
-      <c r="M944" s="4"/>
-      <c r="N944" s="4"/>
-      <c r="O944" s="4"/>
-      <c r="P944" s="4"/>
-      <c r="Q944" s="4"/>
-      <c r="R944" s="4"/>
-      <c r="S944" s="4"/>
-      <c r="T944" s="4"/>
-      <c r="U944" s="4"/>
-      <c r="V944" s="4"/>
-      <c r="W944" s="4"/>
-      <c r="X944" s="4"/>
-      <c r="Y944" s="4"/>
-      <c r="Z944" s="4"/>
-    </row>
   </sheetData>
   <autoFilter ref="$A$1:$H$461"/>
   <printOptions/>

</xml_diff>

<commit_message>
Actualización automática - 2025-10-01 10:32
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -15,7 +15,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="UgepXM4+o4zN/2W73SOBnJ05ynlfjcTKIvBl6ElTvIg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="3R536KseNjw9HdDQOGu8UJ0m0QSSj1JqSQYIOijwJSI="/>
     </ext>
   </extLst>
 </workbook>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="5">
-        <f t="shared" ref="A2:A357" si="1">VLOOKUP(B2,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A2:A357" si="1">VLOOKUP(B2,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -15325,7 +15325,7 @@
     </row>
     <row r="360" ht="14.25" customHeight="1">
       <c r="A360" s="5">
-        <f t="shared" ref="A360:A384" si="2">VLOOKUP(B360,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A360:A384" si="2">VLOOKUP(B360,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>250</v>
       </c>
       <c r="B360" s="4" t="s">
@@ -16570,7 +16570,7 @@
     </row>
     <row r="389" ht="14.25" customHeight="1">
       <c r="A389" s="5">
-        <f t="shared" ref="A389:A392" si="3">VLOOKUP(B389,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A389:A392" si="3">VLOOKUP(B389,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>251</v>
       </c>
       <c r="B389" s="4" t="s">
@@ -16794,7 +16794,7 @@
     </row>
     <row r="394" ht="14.25" customHeight="1">
       <c r="A394" s="5">
-        <f t="shared" ref="A394:A402" si="4">VLOOKUP(B394,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A394:A402" si="4">VLOOKUP(B394,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>1002</v>
       </c>
       <c r="B394" s="4" t="s">
@@ -17243,7 +17243,7 @@
     </row>
     <row r="404" ht="14.25" customHeight="1">
       <c r="A404" s="5">
-        <f t="shared" ref="A404:A452" si="5">VLOOKUP(B404,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A404:A452" si="5">VLOOKUP(B404,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="B404" s="4" t="s">
@@ -19492,7 +19492,7 @@
     </row>
     <row r="454" ht="14.25" customHeight="1">
       <c r="A454" s="5">
-        <f t="shared" ref="A454:A457" si="6">VLOOKUP(B454,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A454:A457" si="6">VLOOKUP(B454,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>263</v>
       </c>
       <c r="B454" s="4" t="s">
@@ -19804,7 +19804,7 @@
     </row>
     <row r="461" ht="14.25" customHeight="1">
       <c r="A461" s="5">
-        <f>VLOOKUP(B461,'Empleados c nro legajo'!$B$1:$F$120,2,FALSE)</f>
+        <f>VLOOKUP(B461,'Empleados c nro legajo'!$B$1:$F$114,2,FALSE)</f>
         <v>227</v>
       </c>
       <c r="B461" s="10" t="s">

</xml_diff>

<commit_message>
Actualización automática - 2025-10-29 15:12
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -7,6 +7,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="MP">'[1]MATERIA PRIMA'!$B$3:$B$135</definedName>
@@ -15,14 +16,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="fCRLKyd+zgCLbRc/ukyfFqZJ6bGfBm4g2g2sXQ8bjls="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="Sg75gXipNuLACsvV+70+SQIFqUD4whWokkr1utqG+dc="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Legajo</t>
   </si>
@@ -46,6 +47,15 @@
   </si>
   <si>
     <t>IMPORTE_GABI</t>
+  </si>
+  <si>
+    <t>maxi zega</t>
+  </si>
+  <si>
+    <t>zarasa</t>
+  </si>
+  <si>
+    <t>Prueba desc</t>
   </si>
 </sst>
 </file>
@@ -237,6 +247,27 @@
       <sheetData sheetId="31"/>
       <sheetData sheetId="32"/>
       <sheetData sheetId="33"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <externalBook r:id="rId1">
+    <sheetNames>
+      <sheetName val="Descuentos 10 2025"/>
+      <sheetName val="descuentos anteriores"/>
+      <sheetName val="Empleados"/>
+      <sheetName val="De adelanto a prestamos"/>
+      <sheetName val="Instructivo"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -506,14 +537,30 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="7"/>
+      <c r="A2" s="5">
+        <v>196.0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45958.0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4">
+        <v>123.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>123.0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7">
+        <v>765532.0</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>

</xml_diff>

<commit_message>
Actualización automática - 2025-10-29 16:05
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -16,14 +16,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="Sg75gXipNuLACsvV+70+SQIFqUD4whWokkr1utqG+dc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="UBnKSqdGoNy2H3eJlVtSIsBXsYkzqt3VlvH3wiE7uw8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Legajo</t>
   </si>
@@ -47,15 +47,6 @@
   </si>
   <si>
     <t>IMPORTE_GABI</t>
-  </si>
-  <si>
-    <t>maxi zega</t>
-  </si>
-  <si>
-    <t>zarasa</t>
-  </si>
-  <si>
-    <t>Prueba desc</t>
   </si>
 </sst>
 </file>
@@ -537,30 +528,14 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="5">
-        <v>196.0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6">
-        <v>45958.0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4">
-        <v>123.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>123.0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="7">
-        <v>765532.0</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>

</xml_diff>

<commit_message>
Actualización automática - 2025-10-30 10:46
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -16,7 +16,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="y8A70j/RDFFNQAYvKgBy03K+TOpZfj9x1P+c3Lf9RgU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="8+JCB3YTKtyO3QwNs5MbQiKcyo2TlO1bp5RuccyslBQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="4">
-        <f t="shared" ref="A2:A316" si="1">VLOOKUP(B2,'Empleados c nro legajo'!$B$2:$F$120,2,FALSE)</f>
+        <f t="shared" ref="A2:A316" si="1">VLOOKUP(B2,'Empleados c nro legajo'!$B$2:$F$106,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">

</xml_diff>